<commit_message>
maj durif ajout des ressources modification du script pour générer les entetes
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14160" activeTab="1"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId1"/>
@@ -2286,8 +2286,8 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36:D40"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3432,7 +3432,9 @@
       <c r="H35" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I35" s="21"/>
+      <c r="I35" s="21">
+        <v>15</v>
+      </c>
       <c r="J35" s="68" t="s">
         <v>18</v>
       </c>
@@ -3640,7 +3642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
maj entete cours et TP
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="2280" yWindow="460" windowWidth="20880" windowHeight="14660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Cycles MPSI IPT'!$A$3:$B$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Semanier MPSI IPT 2019-2020'!$A$18:$H$20</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="296">
   <si>
     <t>Cours</t>
   </si>
@@ -930,6 +930,15 @@
   </si>
   <si>
     <t>Image entête</t>
+  </si>
+  <si>
+    <t>architecture/ARCHI-000</t>
+  </si>
+  <si>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -3331,8 +3340,8 @@
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L15" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3345,7 +3354,8 @@
     <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="5.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="37.33203125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="32.6640625" style="1" customWidth="1"/>
     <col min="15" max="18" width="10.83203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="41.33203125" style="1" customWidth="1"/>
@@ -3447,7 +3457,9 @@
         <v>27</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>293</v>
+      </c>
       <c r="M2" s="73" t="s">
         <v>291</v>
       </c>
@@ -5372,16 +5384,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="70"/>
-    <col min="2" max="2" width="75.83203125" style="71" customWidth="1"/>
+    <col min="2" max="2" width="108.5" style="71" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100.5" style="71" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="70"/>
   </cols>
@@ -5397,7 +5409,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
         <v>189</v>
       </c>
@@ -5408,7 +5420,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>210</v>
       </c>
@@ -5661,7 +5673,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="79" t="s">
         <v>245</v>
       </c>
@@ -5705,7 +5717,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
         <v>218</v>
       </c>
@@ -5727,7 +5739,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
         <v>220</v>
       </c>
@@ -5738,7 +5750,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="36" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A38" s="70" t="s">
         <v>247</v>
       </c>
@@ -5749,7 +5761,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="70" t="s">
         <v>248</v>
       </c>
@@ -5758,6 +5770,16 @@
       </c>
       <c r="C39" s="71" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="70" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" x14ac:dyDescent="0.15">
@@ -5771,7 +5793,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="36" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A43" s="70" t="s">
         <v>222</v>
       </c>
@@ -5804,7 +5826,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="70" t="s">
         <v>225</v>
       </c>
@@ -5837,7 +5859,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="70" t="s">
         <v>228</v>
       </c>
@@ -5859,6 +5881,16 @@
         <v>270</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="70" t="s">
         <v>230</v>
@@ -5903,7 +5935,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="70" t="s">
         <v>234</v>
       </c>
@@ -5958,6 +5990,11 @@
         <v>176</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="70" t="s">
         <v>241</v>
@@ -5991,12 +6028,20 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="36" x14ac:dyDescent="0.15">
+      <c r="A66" s="70" t="s">
+        <v>295</v>
+      </c>
       <c r="B66" s="71" t="s">
         <v>185</v>
       </c>
       <c r="C66" s="71" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A67" s="70" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gestion de séparateurs de dossiers
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="460" windowWidth="20880" windowHeight="14660" activeTab="2"/>
+    <workbookView xWindow="-27500" yWindow="120" windowWidth="20880" windowHeight="14660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="296">
   <si>
     <t>Cours</t>
   </si>
@@ -5386,8 +5386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -5497,6 +5497,16 @@
         <v>92</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="70" t="s">
         <v>192</v>
@@ -5627,6 +5637,16 @@
       </c>
       <c r="C24" s="71" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="70" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
maj cours 1 et 2 reduction image et test pythontex
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Informatique_MPSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliendurif/Documents/prepa/MPSI/ipt_mpsi_lamartin/Informatique_MPSI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A15E9D8-1A7A-4DE0-A9A3-AD31BDF22881}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29740" yWindow="560" windowWidth="25360" windowHeight="14860"/>
   </bookViews>
   <sheets>
     <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId1"/>
@@ -27,13 +26,13 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -951,8 +950,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2248,18 +2247,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2309,42 +2344,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3023,13 +3022,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="651" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="653" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="Normal 4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="Normal 4 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 4 2" xfId="5"/>
+    <cellStyle name="Normal 4 3" xfId="6"/>
+    <cellStyle name="Normal 5" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3341,38 +3340,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I24" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="26" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="10.81640625" style="1"/>
-    <col min="4" max="4" width="20.36328125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.36328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.36328125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="32.6328125" style="1" customWidth="1"/>
-    <col min="15" max="18" width="10.81640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="41.36328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.81640625" style="1"/>
-    <col min="22" max="22" width="10.81640625" style="1" customWidth="1"/>
-    <col min="23" max="24" width="58.453125" style="74" customWidth="1"/>
-    <col min="25" max="16384" width="10.81640625" style="1"/>
+    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="32.6640625" style="1" customWidth="1"/>
+    <col min="15" max="18" width="10.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="10.83203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="58.5" style="74" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="26" customHeight="1">
+    <row r="1" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -3431,17 +3430,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="26" customHeight="1">
+    <row r="2" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="9">
         <v>43711</v>
       </c>
-      <c r="C2" s="109">
+      <c r="C2" s="90">
         <v>1</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="93" t="s">
         <v>272</v>
       </c>
       <c r="E2" s="26">
@@ -3485,7 +3484,7 @@
       <c r="W2" s="75"/>
       <c r="X2" s="75"/>
     </row>
-    <row r="3" spans="1:24" ht="26" customHeight="1">
+    <row r="3" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3493,8 +3492,8 @@
         <f>B2+7</f>
         <v>43718</v>
       </c>
-      <c r="C3" s="110"/>
-      <c r="D3" s="113"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="94"/>
       <c r="E3" s="26">
         <v>2</v>
       </c>
@@ -3535,7 +3534,7 @@
       <c r="W3" s="75"/>
       <c r="X3" s="75"/>
     </row>
-    <row r="4" spans="1:24" ht="26" customHeight="1">
+    <row r="4" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3543,8 +3542,8 @@
         <f>B3+7</f>
         <v>43725</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="113"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="26">
         <v>2</v>
       </c>
@@ -3584,7 +3583,7 @@
       <c r="W4" s="75"/>
       <c r="X4" s="75"/>
     </row>
-    <row r="5" spans="1:24" ht="26" customHeight="1">
+    <row r="5" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3592,8 +3591,8 @@
         <f t="shared" ref="B5:B8" si="0">B4+7</f>
         <v>43732</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="113"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="26">
         <v>3</v>
       </c>
@@ -3633,7 +3632,7 @@
       <c r="W5" s="75"/>
       <c r="X5" s="75"/>
     </row>
-    <row r="6" spans="1:24" ht="26" customHeight="1">
+    <row r="6" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3641,8 +3640,8 @@
         <f>B5+7</f>
         <v>43739</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="113"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="94"/>
       <c r="E6" s="26">
         <v>4</v>
       </c>
@@ -3680,7 +3679,7 @@
       <c r="W6" s="75"/>
       <c r="X6" s="75"/>
     </row>
-    <row r="7" spans="1:24" ht="26" customHeight="1">
+    <row r="7" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3688,8 +3687,8 @@
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="113"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="26">
         <v>4</v>
       </c>
@@ -3727,7 +3726,7 @@
       <c r="W7" s="75"/>
       <c r="X7" s="75"/>
     </row>
-    <row r="8" spans="1:24" ht="26" customHeight="1">
+    <row r="8" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3735,8 +3734,8 @@
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
-      <c r="C8" s="111"/>
-      <c r="D8" s="114"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="26">
         <v>5</v>
       </c>
@@ -3776,25 +3775,25 @@
       <c r="W8" s="75"/>
       <c r="X8" s="75"/>
     </row>
-    <row r="9" spans="1:24" ht="26" customHeight="1">
-      <c r="A9" s="84" t="s">
+    <row r="9" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+      <c r="P9" s="89"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="41"/>
       <c r="S9" s="32"/>
@@ -3802,7 +3801,7 @@
       <c r="W9" s="75"/>
       <c r="X9" s="75"/>
     </row>
-    <row r="10" spans="1:24" ht="26" customHeight="1">
+    <row r="10" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3810,10 +3809,10 @@
         <f>B8+21</f>
         <v>43774</v>
       </c>
-      <c r="C10" s="109">
+      <c r="C10" s="90">
         <v>1</v>
       </c>
-      <c r="D10" s="112" t="s">
+      <c r="D10" s="93" t="s">
         <v>272</v>
       </c>
       <c r="E10" s="26">
@@ -3855,7 +3854,7 @@
       <c r="W10" s="75"/>
       <c r="X10" s="75"/>
     </row>
-    <row r="11" spans="1:24" ht="26" customHeight="1">
+    <row r="11" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3863,8 +3862,8 @@
         <f t="shared" ref="B11:B16" si="1">B10+7</f>
         <v>43781</v>
       </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="113"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="94"/>
       <c r="E11" s="26">
         <v>6</v>
       </c>
@@ -3902,7 +3901,7 @@
       <c r="W11" s="75"/>
       <c r="X11" s="75"/>
     </row>
-    <row r="12" spans="1:24" ht="26" customHeight="1">
+    <row r="12" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3910,8 +3909,8 @@
         <f t="shared" si="1"/>
         <v>43788</v>
       </c>
-      <c r="C12" s="110"/>
-      <c r="D12" s="113"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="94"/>
       <c r="E12" s="26">
         <v>6</v>
       </c>
@@ -3948,7 +3947,7 @@
       <c r="W12" s="75"/>
       <c r="X12" s="75"/>
     </row>
-    <row r="13" spans="1:24" ht="26" customHeight="1">
+    <row r="13" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3956,8 +3955,8 @@
         <f t="shared" si="1"/>
         <v>43795</v>
       </c>
-      <c r="C13" s="110"/>
-      <c r="D13" s="113"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="94"/>
       <c r="E13" s="26">
         <v>7</v>
       </c>
@@ -3997,7 +3996,7 @@
       <c r="W13" s="75"/>
       <c r="X13" s="75"/>
     </row>
-    <row r="14" spans="1:24" ht="26" customHeight="1">
+    <row r="14" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4005,8 +4004,8 @@
         <f t="shared" si="1"/>
         <v>43802</v>
       </c>
-      <c r="C14" s="110"/>
-      <c r="D14" s="113"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="94"/>
       <c r="E14" s="26">
         <v>7</v>
       </c>
@@ -4045,7 +4044,7 @@
       <c r="W14" s="75"/>
       <c r="X14" s="75"/>
     </row>
-    <row r="15" spans="1:24" ht="26" customHeight="1">
+    <row r="15" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4053,8 +4052,8 @@
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="113"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="94"/>
       <c r="E15" s="26">
         <v>8</v>
       </c>
@@ -4096,7 +4095,7 @@
       <c r="W15" s="75"/>
       <c r="X15" s="75"/>
     </row>
-    <row r="16" spans="1:24" ht="26" customHeight="1">
+    <row r="16" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4104,8 +4103,8 @@
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="114"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="95"/>
       <c r="E16" s="26">
         <v>8</v>
       </c>
@@ -4145,25 +4144,25 @@
       <c r="W16" s="75"/>
       <c r="X16" s="75"/>
     </row>
-    <row r="17" spans="1:24" ht="26" customHeight="1">
-      <c r="A17" s="84" t="s">
+    <row r="17" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="85"/>
-      <c r="K17" s="85"/>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="85"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+      <c r="P17" s="89"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="41"/>
       <c r="S17" s="32"/>
@@ -4171,7 +4170,7 @@
       <c r="W17" s="75"/>
       <c r="X17" s="75"/>
     </row>
-    <row r="18" spans="1:24" ht="26" customHeight="1">
+    <row r="18" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -4179,10 +4178,10 @@
         <f>B16+21</f>
         <v>43837</v>
       </c>
-      <c r="C18" s="103">
+      <c r="C18" s="82">
         <v>2</v>
       </c>
-      <c r="D18" s="106" t="s">
+      <c r="D18" s="85" t="s">
         <v>186</v>
       </c>
       <c r="E18" s="28">
@@ -4224,7 +4223,7 @@
       <c r="W18" s="75"/>
       <c r="X18" s="75"/>
     </row>
-    <row r="19" spans="1:24" ht="26" customHeight="1">
+    <row r="19" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -4232,8 +4231,8 @@
         <f>B18+7</f>
         <v>43844</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="107"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="86"/>
       <c r="E19" s="28">
         <v>1</v>
       </c>
@@ -4273,7 +4272,7 @@
       <c r="W19" s="75"/>
       <c r="X19" s="75"/>
     </row>
-    <row r="20" spans="1:24" ht="26" customHeight="1">
+    <row r="20" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -4281,8 +4280,8 @@
         <f t="shared" ref="B20:B40" si="2">B19+7</f>
         <v>43851</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="107"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="86"/>
       <c r="E20" s="28">
         <v>2</v>
       </c>
@@ -4322,7 +4321,7 @@
       <c r="W20" s="75"/>
       <c r="X20" s="75"/>
     </row>
-    <row r="21" spans="1:24" ht="26" customHeight="1">
+    <row r="21" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -4330,8 +4329,8 @@
         <f>B20+7</f>
         <v>43858</v>
       </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="108"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="28">
         <v>2</v>
       </c>
@@ -4371,7 +4370,7 @@
       <c r="W21" s="75"/>
       <c r="X21" s="75"/>
     </row>
-    <row r="22" spans="1:24" ht="26" customHeight="1">
+    <row r="22" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -4379,10 +4378,10 @@
         <f>B21+7</f>
         <v>43865</v>
       </c>
-      <c r="C22" s="89">
+      <c r="C22" s="101">
         <v>3</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="98" t="s">
         <v>61</v>
       </c>
       <c r="E22" s="35">
@@ -4424,7 +4423,7 @@
       <c r="W22" s="75"/>
       <c r="X22" s="75"/>
     </row>
-    <row r="23" spans="1:24" ht="26" customHeight="1">
+    <row r="23" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -4432,8 +4431,8 @@
         <f>B22+7</f>
         <v>43872</v>
       </c>
-      <c r="C23" s="90"/>
-      <c r="D23" s="87"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="99"/>
       <c r="E23" s="35">
         <v>2</v>
       </c>
@@ -4472,7 +4471,7 @@
       </c>
       <c r="S23" s="33"/>
     </row>
-    <row r="24" spans="1:24" ht="26" customHeight="1">
+    <row r="24" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -4480,8 +4479,8 @@
         <f>B23+7</f>
         <v>43879</v>
       </c>
-      <c r="C24" s="91"/>
-      <c r="D24" s="88"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="100"/>
       <c r="E24" s="34">
         <v>2</v>
       </c>
@@ -4516,25 +4515,25 @@
       </c>
       <c r="S24" s="33"/>
     </row>
-    <row r="25" spans="1:24" ht="26" customHeight="1">
-      <c r="A25" s="84" t="s">
+    <row r="25" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="85"/>
-      <c r="M25" s="85"/>
-      <c r="N25" s="85"/>
-      <c r="O25" s="85"/>
-      <c r="P25" s="85"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="89"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="50"/>
       <c r="S25" s="32"/>
@@ -4542,7 +4541,7 @@
       <c r="W25" s="75"/>
       <c r="X25" s="75"/>
     </row>
-    <row r="26" spans="1:24" ht="26" customHeight="1">
+    <row r="26" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -4550,10 +4549,10 @@
         <f>B24+21</f>
         <v>43900</v>
       </c>
-      <c r="C26" s="89">
+      <c r="C26" s="101">
         <v>3</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="98" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="29">
@@ -4595,7 +4594,7 @@
       <c r="W26" s="75"/>
       <c r="X26" s="75"/>
     </row>
-    <row r="27" spans="1:24" ht="26" customHeight="1">
+    <row r="27" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -4603,8 +4602,8 @@
         <f t="shared" si="2"/>
         <v>43907</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="87"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="99"/>
       <c r="E27" s="35">
         <v>3</v>
       </c>
@@ -4641,7 +4640,7 @@
       <c r="W27" s="75"/>
       <c r="X27" s="75"/>
     </row>
-    <row r="28" spans="1:24" ht="26" customHeight="1">
+    <row r="28" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>21</v>
       </c>
@@ -4649,8 +4648,8 @@
         <f t="shared" si="2"/>
         <v>43914</v>
       </c>
-      <c r="C28" s="90"/>
-      <c r="D28" s="87"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="99"/>
       <c r="E28" s="29">
         <v>4</v>
       </c>
@@ -4690,7 +4689,7 @@
       <c r="W28" s="75"/>
       <c r="X28" s="75"/>
     </row>
-    <row r="29" spans="1:24" ht="26" customHeight="1">
+    <row r="29" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>22</v>
       </c>
@@ -4698,8 +4697,8 @@
         <f t="shared" si="2"/>
         <v>43921</v>
       </c>
-      <c r="C29" s="91"/>
-      <c r="D29" s="88"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="100"/>
       <c r="E29" s="35">
         <v>4</v>
       </c>
@@ -4737,7 +4736,7 @@
       <c r="W29" s="75"/>
       <c r="X29" s="75"/>
     </row>
-    <row r="30" spans="1:24" ht="26" customHeight="1">
+    <row r="30" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>23</v>
       </c>
@@ -4745,10 +4744,10 @@
         <f t="shared" si="2"/>
         <v>43928</v>
       </c>
-      <c r="C30" s="92">
+      <c r="C30" s="104">
         <v>4</v>
       </c>
-      <c r="D30" s="94" t="s">
+      <c r="D30" s="106" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="30">
@@ -4792,7 +4791,7 @@
       <c r="W30" s="75"/>
       <c r="X30" s="75"/>
     </row>
-    <row r="31" spans="1:24" ht="26" customHeight="1">
+    <row r="31" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>24</v>
       </c>
@@ -4800,8 +4799,8 @@
         <f t="shared" si="2"/>
         <v>43935</v>
       </c>
-      <c r="C31" s="93"/>
-      <c r="D31" s="95"/>
+      <c r="C31" s="105"/>
+      <c r="D31" s="107"/>
       <c r="E31" s="30">
         <v>2</v>
       </c>
@@ -4841,25 +4840,25 @@
       <c r="W31" s="75"/>
       <c r="X31" s="75"/>
     </row>
-    <row r="32" spans="1:24" ht="26" customHeight="1">
-      <c r="A32" s="82" t="s">
+    <row r="32" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="83"/>
-      <c r="N32" s="83"/>
-      <c r="O32" s="83"/>
-      <c r="P32" s="83"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="97"/>
+      <c r="N32" s="97"/>
+      <c r="O32" s="97"/>
+      <c r="P32" s="97"/>
       <c r="Q32" s="47"/>
       <c r="R32" s="51"/>
       <c r="S32" s="32"/>
@@ -4867,7 +4866,7 @@
       <c r="W32" s="75"/>
       <c r="X32" s="75"/>
     </row>
-    <row r="33" spans="1:24" ht="26" customHeight="1">
+    <row r="33" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>25</v>
       </c>
@@ -4875,10 +4874,10 @@
         <f>B31+21</f>
         <v>43956</v>
       </c>
-      <c r="C33" s="92">
+      <c r="C33" s="104">
         <v>4</v>
       </c>
-      <c r="D33" s="94" t="s">
+      <c r="D33" s="106" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="30">
@@ -4915,7 +4914,7 @@
       </c>
       <c r="S33" s="33"/>
     </row>
-    <row r="34" spans="1:24" ht="26" customHeight="1">
+    <row r="34" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -4923,8 +4922,8 @@
         <f t="shared" si="2"/>
         <v>43963</v>
       </c>
-      <c r="C34" s="97"/>
-      <c r="D34" s="96"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="108"/>
       <c r="E34" s="30">
         <v>3</v>
       </c>
@@ -4961,7 +4960,7 @@
       </c>
       <c r="S34" s="32"/>
     </row>
-    <row r="35" spans="1:24" ht="26" customHeight="1">
+    <row r="35" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -4969,8 +4968,8 @@
         <f t="shared" si="2"/>
         <v>43970</v>
       </c>
-      <c r="C35" s="93"/>
-      <c r="D35" s="95"/>
+      <c r="C35" s="105"/>
+      <c r="D35" s="107"/>
       <c r="E35" s="30">
         <v>4</v>
       </c>
@@ -5006,7 +5005,7 @@
       </c>
       <c r="S35" s="46"/>
     </row>
-    <row r="36" spans="1:24" ht="26" customHeight="1">
+    <row r="36" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -5014,10 +5013,10 @@
         <f t="shared" si="2"/>
         <v>43977</v>
       </c>
-      <c r="C36" s="100">
+      <c r="C36" s="112">
         <v>5</v>
       </c>
-      <c r="D36" s="98" t="s">
+      <c r="D36" s="110" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="31">
@@ -5049,7 +5048,7 @@
       <c r="W36" s="75"/>
       <c r="X36" s="75"/>
     </row>
-    <row r="37" spans="1:24" ht="26" customHeight="1">
+    <row r="37" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -5057,8 +5056,8 @@
         <f t="shared" si="2"/>
         <v>43984</v>
       </c>
-      <c r="C37" s="101"/>
-      <c r="D37" s="99"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="111"/>
       <c r="E37" s="31">
         <v>1</v>
       </c>
@@ -5090,7 +5089,7 @@
       <c r="W37" s="75"/>
       <c r="X37" s="75"/>
     </row>
-    <row r="38" spans="1:24" ht="26" customHeight="1">
+    <row r="38" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>30</v>
       </c>
@@ -5098,8 +5097,8 @@
         <f t="shared" si="2"/>
         <v>43991</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="99"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="111"/>
       <c r="E38" s="31">
         <v>1</v>
       </c>
@@ -5129,7 +5128,7 @@
       <c r="W38" s="75"/>
       <c r="X38" s="75"/>
     </row>
-    <row r="39" spans="1:24" ht="26" customHeight="1">
+    <row r="39" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>31</v>
       </c>
@@ -5137,8 +5136,8 @@
         <f t="shared" si="2"/>
         <v>43998</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="99"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="111"/>
       <c r="E39" s="31">
         <v>1</v>
       </c>
@@ -5168,7 +5167,7 @@
       <c r="W39" s="75"/>
       <c r="X39" s="75"/>
     </row>
-    <row r="40" spans="1:24" ht="26" customHeight="1">
+    <row r="40" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>32</v>
       </c>
@@ -5176,8 +5175,8 @@
         <f t="shared" si="2"/>
         <v>44005</v>
       </c>
-      <c r="C40" s="102"/>
-      <c r="D40" s="99"/>
+      <c r="C40" s="114"/>
+      <c r="D40" s="111"/>
       <c r="E40" s="31">
         <v>1</v>
       </c>
@@ -5205,101 +5204,93 @@
       <c r="W40" s="75"/>
       <c r="X40" s="75"/>
     </row>
-    <row r="41" spans="1:24" ht="26" customHeight="1">
-      <c r="A41" s="82" t="s">
+    <row r="41" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="83"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
-      <c r="H41" s="83"/>
-      <c r="I41" s="83"/>
-      <c r="J41" s="83"/>
-      <c r="K41" s="83"/>
-      <c r="L41" s="83"/>
-      <c r="M41" s="83"/>
-      <c r="N41" s="83"/>
-      <c r="O41" s="83"/>
-      <c r="P41" s="83"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="97"/>
+      <c r="D41" s="97"/>
+      <c r="E41" s="97"/>
+      <c r="F41" s="97"/>
+      <c r="G41" s="97"/>
+      <c r="H41" s="97"/>
+      <c r="I41" s="97"/>
+      <c r="J41" s="97"/>
+      <c r="K41" s="97"/>
+      <c r="L41" s="97"/>
+      <c r="M41" s="97"/>
+      <c r="N41" s="97"/>
+      <c r="O41" s="97"/>
+      <c r="P41" s="97"/>
       <c r="Q41" s="47"/>
       <c r="R41" s="51"/>
       <c r="V41" s="70"/>
       <c r="W41" s="75"/>
       <c r="X41" s="75"/>
     </row>
-    <row r="42" spans="1:24" ht="26" customHeight="1">
+    <row r="42" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V42" s="70"/>
       <c r="W42" s="75"/>
       <c r="X42" s="75"/>
     </row>
-    <row r="43" spans="1:24" ht="26" customHeight="1">
+    <row r="43" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V43" s="70"/>
       <c r="W43" s="75"/>
       <c r="X43" s="75"/>
     </row>
-    <row r="44" spans="1:24" ht="26" customHeight="1">
+    <row r="44" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V44" s="70"/>
       <c r="W44" s="75"/>
       <c r="X44" s="75"/>
     </row>
-    <row r="45" spans="1:24" ht="26" customHeight="1">
+    <row r="45" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V45" s="70"/>
       <c r="W45" s="75"/>
       <c r="X45" s="75"/>
     </row>
-    <row r="46" spans="1:24" ht="26" customHeight="1">
+    <row r="46" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V46" s="70"/>
       <c r="W46" s="75"/>
       <c r="X46" s="75"/>
     </row>
-    <row r="47" spans="1:24" ht="26" customHeight="1">
+    <row r="47" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V47" s="70"/>
       <c r="W47" s="75"/>
       <c r="X47" s="75"/>
     </row>
-    <row r="48" spans="1:24" ht="26" customHeight="1">
+    <row r="48" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V48" s="70"/>
       <c r="W48" s="75"/>
       <c r="X48" s="75"/>
     </row>
-    <row r="49" spans="22:24" ht="26" customHeight="1">
+    <row r="49" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V49" s="70"/>
       <c r="W49" s="75"/>
       <c r="X49" s="75"/>
     </row>
-    <row r="50" spans="22:24" ht="26" customHeight="1">
+    <row r="50" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V50" s="70"/>
       <c r="W50" s="75"/>
       <c r="X50" s="75"/>
     </row>
-    <row r="51" spans="22:24" ht="26" customHeight="1">
+    <row r="51" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V51" s="70"/>
       <c r="W51" s="75"/>
       <c r="X51" s="75"/>
     </row>
-    <row r="52" spans="22:24" ht="26" customHeight="1">
+    <row r="52" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V52" s="70"/>
       <c r="W52" s="75"/>
       <c r="X52" s="75"/>
     </row>
-    <row r="53" spans="22:24" ht="26" customHeight="1">
+    <row r="53" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V53" s="70"/>
       <c r="W53" s="75"/>
       <c r="X53" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="A9:P9"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D10:D16"/>
-    <mergeCell ref="C10:C16"/>
     <mergeCell ref="A41:P41"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A25:P25"/>
@@ -5313,6 +5304,14 @@
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="D36:D40"/>
     <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A9:P9"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D10:D16"/>
+    <mergeCell ref="C10:C16"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5321,22 +5320,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="70.453125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.81640625" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="70.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" customHeight="1"/>
-    <row r="2" spans="1:2" ht="31">
+    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -5344,7 +5343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1">
+    <row r="3" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -5352,7 +5351,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1">
+    <row r="4" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
         <v>55</v>
       </c>
@@ -5360,7 +5359,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1">
+    <row r="5" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="23" t="s">
         <v>56</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="38" customHeight="1">
+    <row r="6" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="24" t="s">
         <v>6</v>
       </c>
@@ -5376,7 +5375,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38" customHeight="1">
+    <row r="7" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
@@ -5392,22 +5391,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="70"/>
-    <col min="2" max="2" width="108.453125" style="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.453125" style="71" customWidth="1"/>
-    <col min="4" max="16384" width="10.81640625" style="70"/>
+    <col min="1" max="1" width="10.83203125" style="70"/>
+    <col min="2" max="2" width="108.5" style="71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.5" style="71" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="70" t="s">
         <v>249</v>
       </c>
@@ -5418,7 +5417,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
         <v>189</v>
       </c>
@@ -5429,7 +5428,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>210</v>
       </c>
@@ -5440,7 +5439,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>211</v>
       </c>
@@ -5451,7 +5450,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>212</v>
       </c>
@@ -5462,7 +5461,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="70" t="s">
         <v>190</v>
       </c>
@@ -5473,7 +5472,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="70" t="s">
         <v>191</v>
       </c>
@@ -5484,7 +5483,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="70" t="s">
         <v>213</v>
       </c>
@@ -5495,7 +5494,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="70" t="s">
         <v>214</v>
       </c>
@@ -5506,17 +5505,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="70" t="s">
         <v>192</v>
       </c>
@@ -5527,7 +5526,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="70" t="s">
         <v>193</v>
       </c>
@@ -5538,7 +5537,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
         <v>194</v>
       </c>
@@ -5549,7 +5548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
         <v>204</v>
       </c>
@@ -5560,7 +5559,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
         <v>206</v>
       </c>
@@ -5571,7 +5570,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
         <v>195</v>
       </c>
@@ -5582,7 +5581,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
         <v>196</v>
       </c>
@@ -5593,7 +5592,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
         <v>197</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
         <v>198</v>
       </c>
@@ -5615,7 +5614,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24">
+    <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
         <v>199</v>
       </c>
@@ -5626,7 +5625,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
         <v>201</v>
       </c>
@@ -5637,7 +5636,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
         <v>202</v>
       </c>
@@ -5648,17 +5647,17 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="79" t="s">
         <v>205</v>
       </c>
@@ -5669,7 +5668,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="79" t="s">
         <v>207</v>
       </c>
@@ -5680,7 +5679,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="79" t="s">
         <v>208</v>
       </c>
@@ -5691,7 +5690,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="79" t="s">
         <v>209</v>
       </c>
@@ -5702,7 +5701,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="79" t="s">
         <v>245</v>
       </c>
@@ -5713,7 +5712,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="79" t="s">
         <v>246</v>
       </c>
@@ -5724,7 +5723,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
         <v>215</v>
       </c>
@@ -5735,7 +5734,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
         <v>217</v>
       </c>
@@ -5746,7 +5745,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
         <v>218</v>
       </c>
@@ -5757,7 +5756,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="70" t="s">
         <v>219</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
         <v>220</v>
       </c>
@@ -5779,7 +5778,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24">
+    <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A38" s="70" t="s">
         <v>247</v>
       </c>
@@ -5790,7 +5789,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="70" t="s">
         <v>248</v>
       </c>
@@ -5801,17 +5800,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24">
+    <row r="42" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A42" s="70" t="s">
         <v>221</v>
       </c>
@@ -5822,7 +5821,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="36">
+    <row r="43" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A43" s="70" t="s">
         <v>222</v>
       </c>
@@ -5833,7 +5832,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24">
+    <row r="44" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A44" s="70" t="s">
         <v>223</v>
       </c>
@@ -5844,7 +5843,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="70" t="s">
         <v>224</v>
       </c>
@@ -5855,7 +5854,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="70" t="s">
         <v>225</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="70" t="s">
         <v>226</v>
       </c>
@@ -5877,7 +5876,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24">
+    <row r="48" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A48" s="70" t="s">
         <v>227</v>
       </c>
@@ -5888,7 +5887,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="70" t="s">
         <v>228</v>
       </c>
@@ -5899,7 +5898,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="24">
+    <row r="50" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A50" s="70" t="s">
         <v>229</v>
       </c>
@@ -5910,17 +5909,17 @@
         <v>270</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="70" t="s">
         <v>230</v>
       </c>
@@ -5931,7 +5930,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="70" t="s">
         <v>231</v>
       </c>
@@ -5942,7 +5941,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="70" t="s">
         <v>232</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="70" t="s">
         <v>233</v>
       </c>
@@ -5964,7 +5963,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="70" t="s">
         <v>234</v>
       </c>
@@ -5975,7 +5974,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="70" t="s">
         <v>235</v>
       </c>
@@ -5986,7 +5985,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="70" t="s">
         <v>238</v>
       </c>
@@ -5997,7 +5996,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="24">
+    <row r="60" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A60" s="70" t="s">
         <v>239</v>
       </c>
@@ -6008,7 +6007,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="70" t="s">
         <v>240</v>
       </c>
@@ -6019,12 +6018,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="70" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="70" t="s">
         <v>241</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="70" t="s">
         <v>242</v>
       </c>
@@ -6046,7 +6045,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="70" t="s">
         <v>243</v>
       </c>
@@ -6057,7 +6056,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="36">
+    <row r="66" spans="1:3" ht="36" x14ac:dyDescent="0.15">
       <c r="A66" s="70" t="s">
         <v>295</v>
       </c>
@@ -6068,7 +6067,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="70" t="s">
         <v>294</v>
       </c>
@@ -6081,20 +6080,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="47.36328125" customWidth="1"/>
+    <col min="2" max="4" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="115" t="s">
         <v>79</v>
       </c>
@@ -6102,7 +6101,7 @@
       <c r="C1" s="116"/>
       <c r="D1" s="117"/>
     </row>
-    <row r="2" spans="1:4" ht="21">
+    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
         <v>80</v>
       </c>
@@ -6112,7 +6111,7 @@
       <c r="C2" s="55"/>
       <c r="D2" s="56"/>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A3" s="54"/>
       <c r="B3" s="55"/>
       <c r="C3" s="55" t="s">
@@ -6120,7 +6119,7 @@
       </c>
       <c r="D3" s="56"/>
     </row>
-    <row r="4" spans="1:4" ht="31.5">
+    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="55" t="s">
@@ -6128,7 +6127,7 @@
       </c>
       <c r="D4" s="56"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55" t="s">
@@ -6136,13 +6135,13 @@
       </c>
       <c r="D5" s="56"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="54"/>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:4" ht="21">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="54" t="s">
         <v>85</v>
       </c>
@@ -6152,7 +6151,7 @@
       <c r="C7" s="55"/>
       <c r="D7" s="56"/>
     </row>
-    <row r="8" spans="1:4" ht="21">
+    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A8" s="54" t="s">
         <v>87</v>
       </c>
@@ -6164,7 +6163,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42">
+    <row r="9" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="54"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -6174,7 +6173,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="53" thickBot="1">
+    <row r="10" spans="1:4" ht="56" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="58" t="s">
@@ -6184,13 +6183,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13" thickBot="1">
+    <row r="11" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
       <c r="D11" s="61"/>
     </row>
-    <row r="12" spans="1:4" ht="14.5">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="115" t="s">
         <v>94</v>
       </c>
@@ -6198,7 +6197,7 @@
       <c r="C12" s="116"/>
       <c r="D12" s="117"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="54" t="s">
         <v>95</v>
       </c>
@@ -6208,7 +6207,7 @@
       <c r="C13" s="55"/>
       <c r="D13" s="56"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="54" t="s">
         <v>97</v>
       </c>
@@ -6218,7 +6217,7 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="54" t="s">
         <v>99</v>
       </c>
@@ -6228,7 +6227,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="56"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="54" t="s">
         <v>101</v>
       </c>
@@ -6238,7 +6237,7 @@
       <c r="C16" s="55"/>
       <c r="D16" s="56"/>
     </row>
-    <row r="17" spans="1:4" ht="21">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="54" t="s">
         <v>103</v>
       </c>
@@ -6248,7 +6247,7 @@
       <c r="C17" s="55"/>
       <c r="D17" s="56"/>
     </row>
-    <row r="18" spans="1:4" ht="21">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="54" t="s">
         <v>105</v>
       </c>
@@ -6258,7 +6257,7 @@
       <c r="C18" s="55"/>
       <c r="D18" s="56"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="54" t="s">
         <v>107</v>
       </c>
@@ -6268,7 +6267,7 @@
       <c r="C19" s="55"/>
       <c r="D19" s="56"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="54" t="s">
         <v>109</v>
       </c>
@@ -6278,7 +6277,7 @@
       <c r="C20" s="55"/>
       <c r="D20" s="56"/>
     </row>
-    <row r="21" spans="1:4" ht="21">
+    <row r="21" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A21" s="54"/>
       <c r="B21" s="55"/>
       <c r="C21" s="55" t="s">
@@ -6286,7 +6285,7 @@
       </c>
       <c r="D21" s="56"/>
     </row>
-    <row r="22" spans="1:4" ht="21">
+    <row r="22" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A22" s="54"/>
       <c r="B22" s="55"/>
       <c r="C22" s="55" t="s">
@@ -6294,7 +6293,7 @@
       </c>
       <c r="D22" s="56"/>
     </row>
-    <row r="23" spans="1:4" ht="21">
+    <row r="23" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A23" s="54"/>
       <c r="B23" s="55"/>
       <c r="C23" s="55" t="s">
@@ -6302,7 +6301,7 @@
       </c>
       <c r="D23" s="56"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="54"/>
       <c r="B24" s="55"/>
       <c r="C24" s="55" t="s">
@@ -6310,7 +6309,7 @@
       </c>
       <c r="D24" s="56"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="54"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55" t="s">
@@ -6318,13 +6317,13 @@
       </c>
       <c r="D25" s="56"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="54"/>
       <c r="B26" s="55"/>
       <c r="C26" s="55"/>
       <c r="D26" s="56"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="54" t="s">
         <v>116</v>
       </c>
@@ -6334,7 +6333,7 @@
       <c r="C27" s="55"/>
       <c r="D27" s="56"/>
     </row>
-    <row r="28" spans="1:4" ht="21">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="54" t="s">
         <v>118</v>
       </c>
@@ -6344,7 +6343,7 @@
       <c r="C28" s="55"/>
       <c r="D28" s="56"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="54" t="s">
         <v>120</v>
       </c>
@@ -6354,7 +6353,7 @@
       <c r="C29" s="55"/>
       <c r="D29" s="56"/>
     </row>
-    <row r="30" spans="1:4" ht="21">
+    <row r="30" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A30" s="54" t="s">
         <v>122</v>
       </c>
@@ -6364,7 +6363,7 @@
       <c r="C30" s="55"/>
       <c r="D30" s="56"/>
     </row>
-    <row r="31" spans="1:4" ht="21">
+    <row r="31" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A31" s="54" t="s">
         <v>124</v>
       </c>
@@ -6374,7 +6373,7 @@
       <c r="C31" s="55"/>
       <c r="D31" s="56"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="54" t="s">
         <v>126</v>
       </c>
@@ -6384,7 +6383,7 @@
       <c r="C32" s="55"/>
       <c r="D32" s="56"/>
     </row>
-    <row r="33" spans="1:4" ht="21">
+    <row r="33" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A33" s="54"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55" t="s">
@@ -6394,7 +6393,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21">
+    <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A34" s="54"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55" t="s">
@@ -6404,7 +6403,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31.5">
+    <row r="35" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A35" s="54"/>
       <c r="B35" s="55"/>
       <c r="C35" s="55" t="s">
@@ -6414,7 +6413,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31.5">
+    <row r="36" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A36" s="54"/>
       <c r="B36" s="55"/>
       <c r="C36" s="55" t="s">
@@ -6424,7 +6423,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31.5">
+    <row r="37" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A37" s="54"/>
       <c r="B37" s="55"/>
       <c r="C37" s="55" t="s">
@@ -6434,7 +6433,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="52.5">
+    <row r="38" spans="1:4" ht="55" x14ac:dyDescent="0.15">
       <c r="A38" s="54"/>
       <c r="B38" s="55"/>
       <c r="C38" s="55" t="s">
@@ -6444,7 +6443,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" thickBot="1">
+    <row r="39" spans="1:4" ht="34" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="57"/>
       <c r="B39" s="58"/>
       <c r="C39" s="58" t="s">
@@ -6454,13 +6453,13 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="13" thickBot="1">
+    <row r="40" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="60"/>
       <c r="B40" s="61"/>
       <c r="C40" s="61"/>
       <c r="D40" s="61"/>
     </row>
-    <row r="41" spans="1:4" ht="14.5">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="118" t="s">
         <v>142</v>
       </c>
@@ -6468,7 +6467,7 @@
       <c r="C41" s="119"/>
       <c r="D41" s="120"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5">
+    <row r="42" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A42" s="54" t="s">
         <v>143</v>
       </c>
@@ -6478,7 +6477,7 @@
       <c r="C42" s="62"/>
       <c r="D42" s="63"/>
     </row>
-    <row r="43" spans="1:4" ht="52.5">
+    <row r="43" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A43" s="54" t="s">
         <v>145</v>
       </c>
@@ -6488,7 +6487,7 @@
       <c r="C43" s="62"/>
       <c r="D43" s="63"/>
     </row>
-    <row r="44" spans="1:4" ht="31.5">
+    <row r="44" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A44" s="54" t="s">
         <v>147</v>
       </c>
@@ -6498,7 +6497,7 @@
       <c r="C44" s="62"/>
       <c r="D44" s="63"/>
     </row>
-    <row r="45" spans="1:4" ht="21">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="54" t="s">
         <v>149</v>
       </c>
@@ -6508,7 +6507,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="63"/>
     </row>
-    <row r="46" spans="1:4" ht="21">
+    <row r="46" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A46" s="54" t="s">
         <v>151</v>
       </c>
@@ -6518,7 +6517,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="63"/>
     </row>
-    <row r="47" spans="1:4" ht="42">
+    <row r="47" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A47" s="54"/>
       <c r="B47" s="62"/>
       <c r="C47" s="62" t="s">
@@ -6528,7 +6527,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="31.5">
+    <row r="48" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A48" s="54"/>
       <c r="B48" s="62"/>
       <c r="C48" s="62" t="s">
@@ -6538,7 +6537,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="52.5">
+    <row r="49" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A49" s="54"/>
       <c r="B49" s="62"/>
       <c r="C49" s="62" t="s">
@@ -6548,7 +6547,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="74" thickBot="1">
+    <row r="50" spans="1:4" ht="67" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="57"/>
       <c r="B50" s="64"/>
       <c r="C50" s="64" t="s">
@@ -6558,13 +6557,13 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1">
+    <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="60"/>
       <c r="B51" s="66"/>
       <c r="C51" s="66"/>
       <c r="D51" s="66"/>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1">
+    <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="121" t="s">
         <v>161</v>
       </c>
@@ -6572,7 +6571,7 @@
       <c r="C52" s="122"/>
       <c r="D52" s="123"/>
     </row>
-    <row r="53" spans="1:4" ht="21">
+    <row r="53" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A53" s="67" t="s">
         <v>162</v>
       </c>
@@ -6582,7 +6581,7 @@
       <c r="C53" s="68"/>
       <c r="D53" s="68"/>
     </row>
-    <row r="54" spans="1:4" ht="21">
+    <row r="54" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A54" s="69" t="s">
         <v>164</v>
       </c>
@@ -6592,7 +6591,7 @@
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
     </row>
-    <row r="55" spans="1:4" ht="21">
+    <row r="55" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A55" s="69" t="s">
         <v>166</v>
       </c>
@@ -6602,7 +6601,7 @@
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
     </row>
-    <row r="56" spans="1:4" ht="21">
+    <row r="56" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A56" s="69" t="s">
         <v>168</v>
       </c>
@@ -6612,7 +6611,7 @@
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
     </row>
-    <row r="57" spans="1:4" ht="21">
+    <row r="57" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A57" s="69" t="s">
         <v>170</v>
       </c>
@@ -6622,7 +6621,7 @@
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
     </row>
-    <row r="58" spans="1:4" ht="21">
+    <row r="58" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A58" s="69"/>
       <c r="B58" s="55"/>
       <c r="C58" s="55" t="s">
@@ -6632,7 +6631,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="52.5">
+    <row r="59" spans="1:4" ht="55" x14ac:dyDescent="0.15">
       <c r="A59" s="69"/>
       <c r="B59" s="55"/>
       <c r="C59" s="55" t="s">
@@ -6642,7 +6641,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="21.5" thickBot="1">
+    <row r="60" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="69"/>
       <c r="B60" s="55"/>
       <c r="C60" s="55" t="s">
@@ -6652,13 +6651,13 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1">
+    <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="60"/>
       <c r="B61" s="66"/>
       <c r="C61" s="66"/>
       <c r="D61" s="66"/>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1">
+    <row r="62" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="121" t="s">
         <v>178</v>
       </c>
@@ -6666,7 +6665,7 @@
       <c r="C62" s="122"/>
       <c r="D62" s="123"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="67" t="s">
         <v>179</v>
       </c>
@@ -6676,7 +6675,7 @@
       <c r="C63" s="68"/>
       <c r="D63" s="68"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="69" t="s">
         <v>181</v>
       </c>
@@ -6686,7 +6685,7 @@
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
     </row>
-    <row r="65" spans="1:4" ht="42">
+    <row r="65" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A65" s="69" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
maj debut cours 3 et TP2
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34380" yWindow="340" windowWidth="28580" windowHeight="16180"/>
+    <workbookView xWindow="-34380" yWindow="340" windowWidth="28580" windowHeight="16180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="326">
   <si>
     <t>Cours</t>
   </si>
@@ -652,302 +652,385 @@
     <t>AN.S2</t>
   </si>
   <si>
+    <t>AN.S3</t>
+  </si>
+  <si>
+    <t>AN.S4</t>
+  </si>
+  <si>
+    <t>AA.C7</t>
+  </si>
+  <si>
+    <t>AA.C9</t>
+  </si>
+  <si>
+    <t>AA.C8</t>
+  </si>
+  <si>
+    <t>AA.C10</t>
+  </si>
+  <si>
+    <t>AA.C11</t>
+  </si>
+  <si>
+    <t>AA.C12</t>
+  </si>
+  <si>
+    <t>AA.S1</t>
+  </si>
+  <si>
+    <t>AA.S2</t>
+  </si>
+  <si>
+    <t>AA.S3</t>
+  </si>
+  <si>
+    <t>AA.S4</t>
+  </si>
+  <si>
+    <t>AA.S5</t>
+  </si>
+  <si>
+    <t>AA.S6</t>
+  </si>
+  <si>
+    <t>AA.S7</t>
+  </si>
+  <si>
+    <t>AA.S8</t>
+  </si>
+  <si>
+    <t>AA.S9</t>
+  </si>
+  <si>
+    <t>AA.S10</t>
+  </si>
+  <si>
+    <t>SN.C1</t>
+  </si>
+  <si>
+    <t>SN.C2</t>
+  </si>
+  <si>
+    <t>SN.C3</t>
+  </si>
+  <si>
+    <t>SN.C4</t>
+  </si>
+  <si>
+    <t>SN.C5</t>
+  </si>
+  <si>
+    <t>SN.S1</t>
+  </si>
+  <si>
+    <t>SN.S2</t>
+  </si>
+  <si>
+    <t>SN.S3</t>
+  </si>
+  <si>
+    <t>SN.S4</t>
+  </si>
+  <si>
+    <t>BDD.C1</t>
+  </si>
+  <si>
+    <t>BDD.C2</t>
+  </si>
+  <si>
+    <t>BDD.C3</t>
+  </si>
+  <si>
+    <t>BDD.C4</t>
+  </si>
+  <si>
+    <t>BDD.C5</t>
+  </si>
+  <si>
+    <t>BDD.S1</t>
+  </si>
+  <si>
+    <t>Opérateurs usuels sur les ensembles dans un contexte de bases de données : union, intersection, différence.</t>
+  </si>
+  <si>
+    <t>Opérateurs spécifiques de l'algèbre relationnelle : projection, sélection (ou restriction), renommage, jointure, produit et division cartésiennes ; fonctions d'agrégation : min, max, somme, moyenne, comptage.</t>
+  </si>
+  <si>
+    <t>BDD.S2</t>
+  </si>
+  <si>
+    <t>BDD.S3</t>
+  </si>
+  <si>
+    <t>BDD.S4</t>
+  </si>
+  <si>
+    <t>AL.C1</t>
+  </si>
+  <si>
+    <t>AL.C2</t>
+  </si>
+  <si>
+    <t>AL.C3</t>
+  </si>
+  <si>
+    <t>AA.C13</t>
+  </si>
+  <si>
+    <t>AA.C14</t>
+  </si>
+  <si>
+    <t>AA.S11</t>
+  </si>
+  <si>
+    <t>AA.S12</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Nom long</t>
+  </si>
+  <si>
+    <t>Nom court</t>
+  </si>
+  <si>
+    <t>Manipuler un OS ou un IDE</t>
+  </si>
+  <si>
+    <t>Se familiariser aux principaux composants d'une machine numérique</t>
+  </si>
+  <si>
+    <t>Se familiariser à la manipulation d'un OS</t>
+  </si>
+  <si>
+    <t>Se familiariser à la manipulation d'un IDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche par dichotomie. </t>
+  </si>
+  <si>
+    <t>Expressions et instructions simples</t>
+  </si>
+  <si>
+    <t>Instructions conditionnelles</t>
+  </si>
+  <si>
+    <t>Instructions itératives</t>
+  </si>
+  <si>
+    <t>Notion de fonction informatique</t>
+  </si>
+  <si>
+    <t>Manipulation de quelques structures de données.</t>
+  </si>
+  <si>
+    <t>Réaliser un programme complet structuré</t>
+  </si>
+  <si>
+    <t>Utiliser les bibliothèques de calcul standard</t>
+  </si>
+  <si>
+    <t>Utiliser les bibliothèques standard pour afficher les résultats sous forme graphique</t>
+  </si>
+  <si>
+    <t>Bibliothèques logicielles</t>
+  </si>
+  <si>
+    <t>Problème stationnaire à une dimension. Méthode de dichotomie, méthode de Newton.</t>
+  </si>
+  <si>
+    <t>Problème discret multidimensionnel linéaire. Méthode de Gauss avec recherche partielle du pivot.</t>
+  </si>
+  <si>
+    <t>Problèmes</t>
+  </si>
+  <si>
+    <t>Architecture matérielle et initiation à l'algorithmique</t>
+  </si>
+  <si>
+    <t>BDD.S1; BDD.S2</t>
+  </si>
+  <si>
+    <t>BDD.C4; BDD.C5; BDD.S2; BDD.S3</t>
+  </si>
+  <si>
+    <t>BDD.C1; BDD.C2; BDD.C5; BDD.S2; BDD.S3</t>
+  </si>
+  <si>
+    <t>BDD.C3; BDD.S4</t>
+  </si>
+  <si>
+    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; SN.S3</t>
+  </si>
+  <si>
+    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; SN.S2</t>
+  </si>
+  <si>
+    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; SN.S4</t>
+  </si>
+  <si>
+    <t>AA.C1; AA.S1; AA.S3; AA.S3</t>
+  </si>
+  <si>
+    <t>AA.C2: AA.C3; AA.S4; AA.S5</t>
+  </si>
+  <si>
+    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; AN.S3</t>
+  </si>
+  <si>
+    <t>AN.C1; AN.C2; AN.S1; AN.S2; AN.S4</t>
+  </si>
+  <si>
+    <t>AN.C3; AN.S1; AN.S2; AN.S4</t>
+  </si>
+  <si>
+    <t>AA.C4; AA.C5; AA.C6; AA.C7; AA.C8; AA.S8; AA.S9</t>
+  </si>
+  <si>
+    <t>AA.C9; AA.S12</t>
+  </si>
+  <si>
+    <t>AA.C9; AA.S11</t>
+  </si>
+  <si>
+    <t>AA.C4; AA.C5; AA.C6; AA.C7; AA.C8; AA.C9; AA.S6; AA.S7; AA.S10</t>
+  </si>
+  <si>
+    <t>Compétences cours</t>
+  </si>
+  <si>
+    <t>Compétences TP</t>
+  </si>
+  <si>
+    <t>AA.C1; AA.S1; AA.S2; AA.S3</t>
+  </si>
+  <si>
+    <t>Image entête</t>
+  </si>
+  <si>
+    <t>architecture/ARCHI-000</t>
+  </si>
+  <si>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>AA.C4; AA.C5; AA.C6; AA.C7; AA.C9; AA.S6; AA.S7; AA.S10</t>
+  </si>
+  <si>
+    <t>python_bases/PYB-000;python_bases/PYB-002;python_bases/PYB-003;python_bases/PYB-004</t>
+  </si>
+  <si>
+    <t>architecture/ARCHI-001</t>
+  </si>
+  <si>
+    <t>Manipuler en mode « utilisateur » les principales fonctions d'un système d'exploitation et d'un environnement de développement</t>
+  </si>
+  <si>
+    <t>Se familiariser aux principaux composants d'une machine numérique telle que l'ordinateur personnel, une tablette, etc : sources d'énergie, mémoire vive, mémoire de masse, unité centrale, périphériques d'entrée-sortie, ports de communication avec d'autres composants numériques</t>
+  </si>
+  <si>
+    <t>Se familiariser à la manipulation d'un système d'exploitation (gestion des ressources, essentiellement : organisation des fichiers, arborescence, droits d'accès, de modification, entrées/sorties)</t>
+  </si>
+  <si>
+    <t>Se familiariser à la manipulation d'un environnement de développement</t>
+  </si>
+  <si>
+    <t>Comprendre un algorithme et expliquer ce qu'il fait</t>
+  </si>
+  <si>
+    <t>Expliquer le fonctionnement d'un algorithme</t>
+  </si>
+  <si>
+    <t>Justifier qu'une itération (ou boucle) produit l'effet attendu au moyen d'un invariant</t>
+  </si>
+  <si>
+    <t>Démontrer qu'une boucle se termine effectivement</t>
+  </si>
+  <si>
+    <t>S'interroger sur l'efficacité algorithmique temporelle d'un algorithme</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recherche par dichotomie dans un tableau trié. 
-Recherche par dichotomie du zéro d’une fonction continue et monotone. </t>
-  </si>
-  <si>
-    <t>AN.S3</t>
-  </si>
-  <si>
-    <t>AN.S4</t>
-  </si>
-  <si>
-    <t>Recherche d’un mot dans une chaîne de caractères. On se limite ici à l’algorithme « naïf », en estimant sa complexité.</t>
-  </si>
-  <si>
-    <t>AA.C7</t>
-  </si>
-  <si>
-    <t>AA.C9</t>
-  </si>
-  <si>
-    <t>AA.C8</t>
-  </si>
-  <si>
-    <t>AA.C10</t>
-  </si>
-  <si>
-    <t>AA.C11</t>
-  </si>
-  <si>
-    <t>AA.C12</t>
-  </si>
-  <si>
-    <t>AA.S1</t>
-  </si>
-  <si>
-    <t>AA.S2</t>
-  </si>
-  <si>
-    <t>AA.S3</t>
-  </si>
-  <si>
-    <t>AA.S4</t>
-  </si>
-  <si>
-    <t>AA.S5</t>
-  </si>
-  <si>
-    <t>AA.S6</t>
-  </si>
-  <si>
-    <t>Manipulation de quelques structures de données : chaînes de caractères (création, accès à un caractère, concaténation), listes (création, ajout d’un élément, suppression d’un élément, accès à un élément, extraction d’une partie de liste), tableaux à une ou plusieurs dimensions.</t>
-  </si>
-  <si>
-    <t>AA.S7</t>
-  </si>
-  <si>
-    <t>AA.S8</t>
-  </si>
-  <si>
-    <t>AA.S9</t>
-  </si>
-  <si>
-    <t>AA.S10</t>
-  </si>
-  <si>
-    <t>SN.C1</t>
-  </si>
-  <si>
-    <t>SN.C2</t>
-  </si>
-  <si>
-    <t>SN.C3</t>
-  </si>
-  <si>
-    <t>SN.C4</t>
-  </si>
-  <si>
-    <t>SN.C5</t>
-  </si>
-  <si>
-    <t>SN.S1</t>
-  </si>
-  <si>
-    <t>SN.S2</t>
-  </si>
-  <si>
-    <t>SN.S3</t>
-  </si>
-  <si>
-    <t>SN.S4</t>
-  </si>
-  <si>
-    <t>BDD.C1</t>
-  </si>
-  <si>
-    <t>BDD.C2</t>
-  </si>
-  <si>
-    <t>BDD.C3</t>
-  </si>
-  <si>
-    <t>BDD.C4</t>
-  </si>
-  <si>
-    <t>BDD.C5</t>
-  </si>
-  <si>
-    <t>BDD.S1</t>
-  </si>
-  <si>
-    <t>Opérateurs usuels sur les ensembles dans un contexte de bases de données : union, intersection, différence.</t>
-  </si>
-  <si>
-    <t>Opérateurs spécifiques de l'algèbre relationnelle : projection, sélection (ou restriction), renommage, jointure, produit et division cartésiennes ; fonctions d'agrégation : min, max, somme, moyenne, comptage.</t>
-  </si>
-  <si>
-    <t>BDD.S2</t>
-  </si>
-  <si>
-    <t>BDD.S3</t>
-  </si>
-  <si>
-    <t>BDD.S4</t>
-  </si>
-  <si>
-    <t>AL.C1</t>
-  </si>
-  <si>
-    <t>AL.C2</t>
-  </si>
-  <si>
-    <t>AL.C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tris d’un tableau à une dimension de valeurs numériques. </t>
-  </si>
-  <si>
-    <t>AA.C13</t>
-  </si>
-  <si>
-    <t>AA.C14</t>
-  </si>
-  <si>
-    <t>AA.S11</t>
-  </si>
-  <si>
-    <t>AA.S12</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Nom long</t>
-  </si>
-  <si>
-    <t>Nom court</t>
-  </si>
-  <si>
-    <t>Manipuler un OS ou un IDE</t>
-  </si>
-  <si>
-    <t>Se familiariser aux principaux composants d'une machine numérique</t>
-  </si>
-  <si>
-    <t>Se familiariser à la manipulation d'un OS</t>
-  </si>
-  <si>
-    <t>Se familiariser à la manipulation d'un IDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recherche par dichotomie. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recherche d’un mot dans une chaîne de caractères. </t>
-  </si>
-  <si>
-    <t>Rechercher une information au sein d’une documentation</t>
-  </si>
-  <si>
-    <t>Expressions et instructions simples</t>
-  </si>
-  <si>
-    <t>Instructions conditionnelles</t>
-  </si>
-  <si>
-    <t>Instructions itératives</t>
-  </si>
-  <si>
-    <t>Notion de fonction informatique</t>
-  </si>
-  <si>
-    <t>Manipulation de quelques structures de données.</t>
-  </si>
-  <si>
-    <t>Réaliser un programme complet structuré</t>
-  </si>
-  <si>
-    <t>Utiliser les bibliothèques de calcul standard</t>
-  </si>
-  <si>
-    <t>Utiliser les bibliothèques standard pour afficher les résultats sous forme graphique</t>
-  </si>
-  <si>
-    <t>Bibliothèques logicielles</t>
-  </si>
-  <si>
-    <t>Problème stationnaire à une dimension. Méthode de dichotomie, méthode de Newton.</t>
-  </si>
-  <si>
-    <t>Problème dynamique à une dimension,  linéaire ou non. Méthode d’Euler.</t>
-  </si>
-  <si>
-    <t>Problème discret multidimensionnel linéaire. Méthode de Gauss avec recherche partielle du pivot.</t>
-  </si>
-  <si>
-    <t>Problèmes</t>
-  </si>
-  <si>
-    <t>Architecture matérielle et initiation à l'algorithmique</t>
-  </si>
-  <si>
-    <t>BDD.S1; BDD.S2</t>
-  </si>
-  <si>
-    <t>BDD.C4; BDD.C5; BDD.S2; BDD.S3</t>
-  </si>
-  <si>
-    <t>BDD.C1; BDD.C2; BDD.C5; BDD.S2; BDD.S3</t>
-  </si>
-  <si>
-    <t>BDD.C3; BDD.S4</t>
-  </si>
-  <si>
-    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; SN.S3</t>
-  </si>
-  <si>
-    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; SN.S2</t>
-  </si>
-  <si>
-    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; SN.S4</t>
-  </si>
-  <si>
-    <t>AA.C1; AA.S1; AA.S3; AA.S3</t>
-  </si>
-  <si>
-    <t>AA.C2: AA.C3; AA.S4; AA.S5</t>
-  </si>
-  <si>
-    <t>SN.C1; SN.C2; SN.C3; SN.C4; SN.C5; SN.S1; AN.S3</t>
-  </si>
-  <si>
-    <t>AN.C1; AN.C2; AN.S1; AN.S2; AN.S4</t>
-  </si>
-  <si>
-    <t>AN.C3; AN.S1; AN.S2; AN.S4</t>
-  </si>
-  <si>
-    <t>AA.C4; AA.C5; AA.C6; AA.C7; AA.C8; AA.S8; AA.S9</t>
-  </si>
-  <si>
-    <t>AA.C9; AA.S12</t>
-  </si>
-  <si>
-    <t>AA.C9; AA.S11</t>
-  </si>
-  <si>
-    <t>AA.C4; AA.C5; AA.C6; AA.C7; AA.C8; AA.C9; AA.S6; AA.S7; AA.S10</t>
-  </si>
-  <si>
-    <t>Compétences cours</t>
-  </si>
-  <si>
-    <t>Compétences TP</t>
-  </si>
-  <si>
-    <t>AA.C1; AA.S1; AA.S2; AA.S3</t>
-  </si>
-  <si>
-    <t>Image entête</t>
-  </si>
-  <si>
-    <t>architecture/ARCHI-000</t>
-  </si>
-  <si>
-    <t>fin</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>AA.C4; AA.C5; AA.C6; AA.C7; AA.C9; AA.S6; AA.S7; AA.S10</t>
-  </si>
-  <si>
-    <t>python_bases/PYB-000;python_bases/PYB-002;python_bases/PYB-003;python_bases/PYB-004</t>
-  </si>
-  <si>
-    <t>architecture/ARCHI-001</t>
+Recherche par dichotomie du zéro d'une fonction continue et monotone. </t>
+  </si>
+  <si>
+    <t>Méthodes des rectangles et des trapèzes pour le calcul approché d'une intégrale sur un segment.</t>
+  </si>
+  <si>
+    <t>Recherche d'un mot dans une chaîne de caractères. On se limite ici à l'algorithme « naïf », en estimant sa complexité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche d'un mot dans une chaîne de caractères. </t>
+  </si>
+  <si>
+    <t>Choisir un type de données en fonction d'un problème à résoudre</t>
+  </si>
+  <si>
+    <t>Concevoir l'en-tête (ou la spécification) d'une fonction, puis la fonction elle-même</t>
+  </si>
+  <si>
+    <t>Gérer efficacement un ensemble de fichiers correspondant à des versions successives d'un fichier source</t>
+  </si>
+  <si>
+    <t>Rechercher une information au sein d'une documentation en ligne, analyser des exemples fournis dans cette documentation</t>
+  </si>
+  <si>
+    <t>Rechercher une information au sein d'une documentation</t>
+  </si>
+  <si>
+    <t>Variables : notion de type et de valeur d'une variable, types simples.</t>
+  </si>
+  <si>
+    <t>Manipulation de quelques structures de données : chaînes de caractères (création, accès à un caractère, concaténation), listes (création, ajout d'un élément, suppression d'un élément, accès à un élément, extraction d'une partie de liste), tableaux à une ou plusieurs dimensions.</t>
+  </si>
+  <si>
+    <t>Fichiers : notion de chemin d'accès, lecture et écriture de données numériques ou de type chaîne de caractères depuis ou vers un fichier.</t>
+  </si>
+  <si>
+    <t>Étudier l'effet d'une variation des paramètres sur le temps de calcul, sur la précision des résultats, sur la forme des solutions pour des programmes d'ingénierie numérique choisis, tout en contextualisant l'observation du temps de calcul par rapport à la complexité algorithmique de ces programmes</t>
+  </si>
+  <si>
+    <t>Utiliser les bibliothèques de calcul standard pour résoudre un problème scientifique mis en équation lors des enseignements de chimie, physique, mathématiques, sciences industrielles et de l'ingénieur</t>
+  </si>
+  <si>
+    <t>Tenir compte des aspects pratiques comme l'impact des erreurs d'arrondi sur les résultats, le temps de calcul ou le stockage en mémoire.</t>
+  </si>
+  <si>
+    <t>Bibliothèques logicielles : utilisation de quelques fonctions d'une bibliothèque et de leur documentation en ligne.</t>
+  </si>
+  <si>
+    <t>Problème stationnaire à une dimension, linéaire ou non conduisant à la résolution approchée d'une équation algébrique ou transcendante. Méthode de dichotomie, méthode de Newton.</t>
+  </si>
+  <si>
+    <t>Problème dynamique à une dimension,  linéaire ou non, conduisant à la résolution approchée d'une équation différentielle ordinaire par la méthode d'Euler.</t>
+  </si>
+  <si>
+    <t>Problème dynamique à une dimension,  linéaire ou non. Méthode d'Euler.</t>
+  </si>
+  <si>
+    <t>Problème discret multidimensionnel, linéaire, conduisant à la résolution d'un système linéaire inversible (ou de Cramer) par la méthode de Gauss avec recherche partielle du pivot.</t>
+  </si>
+  <si>
+    <t>Utiliser une application offrant une interface graphique pour créer une base de données et l'alimenter</t>
+  </si>
+  <si>
+    <t>Traduire dans le langage de l'algèbre relationnelle des requêtes écrites en langage courant</t>
+  </si>
+  <si>
+    <t>Concept de client-serveur. Brève extension au cas de l'architecture trois-tiers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tris d'un tableau à une dimension de valeurs numériques. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tri par insertion, tri rapide (ou « quicksort »), tri par fusion.
+Application à la recherche de la médiane d'une liste de nombres. 
+On étudie et on compare ces algorithmes de tri du point de vue des complexités temporelles dans le meilleur et dans le pire cas. </t>
   </si>
 </sst>
 </file>
@@ -3352,7 +3435,7 @@
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -3416,10 +3499,10 @@
         <v>58</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>13</v>
@@ -3428,7 +3511,7 @@
         <v>22</v>
       </c>
       <c r="Q1" s="41" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>64</v>
@@ -3448,7 +3531,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="112" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E2" s="26">
         <v>1</v>
@@ -3470,13 +3553,13 @@
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M2" s="73" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="N2" s="73" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="42"/>
@@ -3520,13 +3603,13 @@
         <v>27</v>
       </c>
       <c r="K3" s="124" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="M3" s="73" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="N3" s="73" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="42"/>
@@ -3571,13 +3654,13 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="M4" s="73" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="N4" s="73" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="42"/>
@@ -3623,10 +3706,10 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="73" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="N5" s="73" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="42"/>
@@ -3673,7 +3756,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="73" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="42"/>
@@ -3720,7 +3803,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="73" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="36"/>
@@ -3764,10 +3847,10 @@
         <v>28</v>
       </c>
       <c r="M8" s="78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="N8" s="73" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="36" t="s">
@@ -3822,7 +3905,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="112" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E10" s="26">
         <v>5</v>
@@ -3845,10 +3928,10 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="N10" s="73" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="42"/>
@@ -3894,7 +3977,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="3"/>
@@ -3941,7 +4024,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="3"/>
@@ -3987,10 +4070,10 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="78" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="N13" s="78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="42"/>
@@ -4036,10 +4119,10 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="78" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="N14" s="78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="42"/>
@@ -4084,10 +4167,10 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="73" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="N15" s="78" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>53</v>
@@ -4135,10 +4218,10 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="73" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="N16" s="78" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="36"/>
@@ -4214,10 +4297,10 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="73" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="N18" s="73" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="O18" s="27"/>
       <c r="P18" s="43"/>
@@ -4263,10 +4346,10 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="73" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="N19" s="73" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="O19" s="27"/>
       <c r="P19" s="43"/>
@@ -4312,10 +4395,10 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="73" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="N20" s="73" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="42"/>
@@ -4361,10 +4444,10 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="73" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="N21" s="73" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="42"/>
@@ -4414,10 +4497,10 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="73" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="N22" s="73" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="42"/>
@@ -4463,10 +4546,10 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="73" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="N23" s="73" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>16</v>
@@ -4511,10 +4594,10 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="73" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="N24" s="73" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="O24" s="27"/>
       <c r="P24" s="42"/>
@@ -4585,10 +4668,10 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="73" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="N26" s="73" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O26" s="27"/>
       <c r="P26" s="42"/>
@@ -4634,10 +4717,10 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="77" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="N27" s="73" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="P27" s="36"/>
       <c r="Q27" s="4"/>
@@ -4680,10 +4763,10 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="73" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="N28" s="73" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="36"/>
@@ -4729,10 +4812,10 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="73" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="N29" s="73" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="42"/>
@@ -4780,10 +4863,10 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="73" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="N30" s="73" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="O30" s="4" t="s">
         <v>54</v>
@@ -4831,10 +4914,10 @@
       <c r="K31" s="39"/>
       <c r="L31" s="39"/>
       <c r="M31" s="73" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="N31" s="73" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="O31" s="27"/>
       <c r="P31" s="43"/>
@@ -4910,10 +4993,10 @@
       <c r="K33" s="38"/>
       <c r="L33" s="38"/>
       <c r="M33" s="73" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="N33" s="73" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="O33" s="6"/>
       <c r="P33" s="44"/>
@@ -4954,10 +5037,10 @@
       <c r="K34" s="39"/>
       <c r="L34" s="39"/>
       <c r="M34" s="76" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="N34" s="76" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="44"/>
@@ -5000,10 +5083,10 @@
       <c r="K35" s="39"/>
       <c r="L35" s="39"/>
       <c r="M35" s="77" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="N35" s="77" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="P35" s="36"/>
       <c r="Q35" s="78" t="s">
@@ -5357,7 +5440,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
@@ -5389,7 +5472,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5403,8 +5486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -5417,13 +5500,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="70" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -5431,43 +5514,43 @@
         <v>189</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>81</v>
+        <v>292</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>82</v>
+        <v>293</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>83</v>
+        <v>294</v>
       </c>
       <c r="C4" s="71" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B5" s="71" t="s">
-        <v>84</v>
+        <v>295</v>
       </c>
       <c r="C5" s="71" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -5494,7 +5577,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="70" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B9" s="71" t="s">
         <v>90</v>
@@ -5505,7 +5588,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="70" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B10" s="71" t="s">
         <v>92</v>
@@ -5516,12 +5599,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -5529,10 +5612,10 @@
         <v>192</v>
       </c>
       <c r="B13" s="71" t="s">
-        <v>96</v>
+        <v>296</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>96</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -5559,18 +5642,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>102</v>
+        <v>297</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>102</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B17" s="71" t="s">
         <v>104</v>
@@ -5584,10 +5667,10 @@
         <v>195</v>
       </c>
       <c r="B18" s="71" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -5595,10 +5678,10 @@
         <v>196</v>
       </c>
       <c r="B19" s="71" t="s">
-        <v>108</v>
+        <v>299</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>108</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -5606,10 +5689,10 @@
         <v>197</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
       <c r="C20" s="71" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -5628,69 +5711,69 @@
         <v>199</v>
       </c>
       <c r="B22" s="71" t="s">
-        <v>200</v>
+        <v>301</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="71" t="s">
-        <v>113</v>
+        <v>302</v>
       </c>
       <c r="C23" s="71" t="s">
-        <v>113</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24" s="71" t="s">
-        <v>203</v>
+        <v>303</v>
       </c>
       <c r="C24" s="71" t="s">
-        <v>257</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="79" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B27" s="80" t="s">
-        <v>117</v>
+        <v>305</v>
       </c>
       <c r="C27" s="80" t="s">
-        <v>117</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="79" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B28" s="80" t="s">
-        <v>119</v>
+        <v>306</v>
       </c>
       <c r="C28" s="80" t="s">
-        <v>119</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="79" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B29" s="80" t="s">
         <v>121</v>
@@ -5701,29 +5784,29 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="79" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B30" s="80" t="s">
-        <v>123</v>
+        <v>307</v>
       </c>
       <c r="C30" s="80" t="s">
-        <v>123</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="79" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B31" s="80" t="s">
-        <v>125</v>
+        <v>308</v>
       </c>
       <c r="C31" s="80" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="79" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B32" s="80" t="s">
         <v>127</v>
@@ -5734,76 +5817,76 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B33" s="71" t="s">
-        <v>128</v>
+        <v>310</v>
       </c>
       <c r="C33" s="71" t="s">
-        <v>128</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B34" s="71" t="s">
         <v>130</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B35" s="71" t="s">
         <v>132</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="70" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B36" s="71" t="s">
         <v>134</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B37" s="71" t="s">
         <v>136</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A38" s="70" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B38" s="71" t="s">
-        <v>216</v>
+        <v>311</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="70" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B39" s="71" t="s">
-        <v>140</v>
+        <v>312</v>
       </c>
       <c r="C39" s="71" t="s">
         <v>32</v>
@@ -5811,137 +5894,137 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A42" s="70" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B42" s="71" t="s">
         <v>144</v>
       </c>
       <c r="C42" s="71" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A43" s="70" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>146</v>
+        <v>313</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>146</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A44" s="70" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B44" s="71" t="s">
-        <v>148</v>
+        <v>314</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="70" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B45" s="71" t="s">
         <v>150</v>
       </c>
       <c r="C45" s="71" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="70" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B46" s="71" t="s">
-        <v>152</v>
+        <v>315</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>152</v>
+        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="70" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B47" s="71" t="s">
-        <v>153</v>
+        <v>316</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A48" s="70" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B48" s="71" t="s">
-        <v>155</v>
+        <v>317</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="70" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B49" s="71" t="s">
-        <v>157</v>
+        <v>318</v>
       </c>
       <c r="C49" s="71" t="s">
-        <v>269</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A50" s="70" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B50" s="71" t="s">
-        <v>159</v>
+        <v>320</v>
       </c>
       <c r="C50" s="71" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="70" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B53" s="71" t="s">
-        <v>163</v>
+        <v>321</v>
       </c>
       <c r="C53" s="71" t="s">
-        <v>163</v>
+        <v>321</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="70" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B54" s="71" t="s">
         <v>165</v>
@@ -5952,7 +6035,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="70" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B55" s="71" t="s">
         <v>167</v>
@@ -5963,18 +6046,18 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="70" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B56" s="71" t="s">
-        <v>169</v>
+        <v>322</v>
       </c>
       <c r="C56" s="71" t="s">
-        <v>169</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="70" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B57" s="71" t="s">
         <v>171</v>
@@ -5985,7 +6068,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="70" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B58" s="71" t="s">
         <v>172</v>
@@ -5996,45 +6079,45 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="70" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B59" s="71" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C59" s="71" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A60" s="70" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B60" s="71" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C60" s="71" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="70" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B61" s="71" t="s">
-        <v>176</v>
+        <v>323</v>
       </c>
       <c r="C61" s="71" t="s">
-        <v>176</v>
+        <v>323</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="70" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B63" s="71" t="s">
         <v>180</v>
@@ -6045,7 +6128,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="70" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B64" s="71" t="s">
         <v>182</v>
@@ -6056,29 +6139,29 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="70" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B65" s="71" t="s">
-        <v>244</v>
+        <v>324</v>
       </c>
       <c r="C65" s="71" t="s">
-        <v>244</v>
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="36" x14ac:dyDescent="0.15">
       <c r="A66" s="70" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B66" s="71" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
       <c r="C66" s="71" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="70" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj TP04 et export DS
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -12,14 +12,16 @@
     <workbookView xWindow="-34660" yWindow="-1120" windowWidth="29380" windowHeight="18380"/>
   </bookViews>
   <sheets>
-    <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId1"/>
-    <sheet name="Cycles MPSI IPT" sheetId="11" r:id="rId2"/>
-    <sheet name="Competences" sheetId="14" r:id="rId3"/>
-    <sheet name="Programme" sheetId="13" r:id="rId4"/>
+    <sheet name="Planning DS" sheetId="16" r:id="rId1"/>
+    <sheet name="Planning DS0" sheetId="15" r:id="rId2"/>
+    <sheet name="Semanier MPSI IPT 2019-2020" sheetId="12" r:id="rId3"/>
+    <sheet name="Cycles MPSI IPT" sheetId="11" r:id="rId4"/>
+    <sheet name="Competences" sheetId="14" r:id="rId5"/>
+    <sheet name="Programme" sheetId="13" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Cycles MPSI IPT'!$A$3:$B$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Semanier MPSI IPT 2019-2020'!$A$18:$H$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Cycles MPSI IPT'!$A$3:$B$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Semanier MPSI IPT 2019-2020'!$A$18:$H$20</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="443">
   <si>
     <t>Cours</t>
   </si>
@@ -1052,13 +1054,343 @@
   </si>
   <si>
     <t>consignes/consignes_TP4;python_bases/PYB-501;python_bases/PYB-523;python_bases/PYB-506;F:python_bases/PYB-507</t>
+  </si>
+  <si>
+    <t>2019-2020</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
+  </si>
+  <si>
+    <t>Titre</t>
+  </si>
+  <si>
+    <t>Modélisation de l'auto-focus d'un appareil photo réflex</t>
+  </si>
+  <si>
+    <t>Fauteuil dynamique de cinéma</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>Téléchirurgie</t>
+  </si>
+  <si>
+    <t>Supports</t>
+  </si>
+  <si>
+    <t>DS/autofocus_appareil_reflex</t>
+  </si>
+  <si>
+    <t>automatique/fauteuil_dynamique_cinema</t>
+  </si>
+  <si>
+    <t>CCP PSI 2015</t>
+  </si>
+  <si>
+    <t>Thèmes</t>
+  </si>
+  <si>
+    <t>SLCI, analyse temporelle, chaine fonctionnelle</t>
+  </si>
+  <si>
+    <t>AF SysML, SLCI, temporel, multiphysique</t>
+  </si>
+  <si>
+    <t>SLCI, Bode, multihysique, Chaine fonctionnelle</t>
+  </si>
+  <si>
+    <t>PFS 2D, SysML, combinatoire, Fermeture geo</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Cellule d'assemblage pour l'avion Falcon</t>
+  </si>
+  <si>
+    <t>Fauteuil roulant handicapé +Imagerie EOS</t>
+  </si>
+  <si>
+    <t>Vanoise express</t>
+  </si>
+  <si>
+    <t>Porte de tram et micromanipulateurendoscopique</t>
+  </si>
+  <si>
+    <t>automatique/assemblage_falcon</t>
+  </si>
+  <si>
+    <t>Central PSI 2008 et CCP PSI 2016</t>
+  </si>
+  <si>
+    <t>SLCI, analyse temporelle et fréquentielle, chaine fonctionnelle</t>
+  </si>
+  <si>
+    <t>AF SysML, SLCI, Bode, correcteurs</t>
+  </si>
+  <si>
+    <t>AF SysML, Théorie des mécanismes, Liaison équivalente, Cinématique engrenage, Statique</t>
+  </si>
+  <si>
+    <t>4H</t>
+  </si>
+  <si>
+    <t>2H+2H</t>
+  </si>
+  <si>
+    <t>Tete de découpe de tissu</t>
+  </si>
+  <si>
+    <t>Transmission tramway</t>
+  </si>
+  <si>
+    <t>Train atterrissage hélicoptère</t>
+  </si>
+  <si>
+    <t>DS/tete_decoupe_tissu</t>
+  </si>
+  <si>
+    <t>CCP MP 2018</t>
+  </si>
+  <si>
+    <t>SIA PT 2014</t>
+  </si>
+  <si>
+    <t>SLCI Correcteur, analyse temporelle, fermeture geo, dynamique simple</t>
+  </si>
+  <si>
+    <t>Dynamique simple, lois de vitesse, asservissement</t>
+  </si>
+  <si>
+    <t>Dynamique, AF en SysML</t>
+  </si>
+  <si>
+    <t>3;4</t>
+  </si>
+  <si>
+    <t>Modélisation du robot d'exploration ROBOVOLC</t>
+  </si>
+  <si>
+    <t>ROBOVOLC</t>
+  </si>
+  <si>
+    <t>FLIR</t>
+  </si>
+  <si>
+    <t>ROBUCAR</t>
+  </si>
+  <si>
+    <t>DS/robovolc</t>
+  </si>
+  <si>
+    <t>XENS2017</t>
+  </si>
+  <si>
+    <t>Central psi 2014</t>
+  </si>
+  <si>
+    <t>e3a 2015 MP SII</t>
+  </si>
+  <si>
+    <t>Dynamique, Cinématique simple, SLCI avec Bode et correcteur AF SysML</t>
+  </si>
+  <si>
+    <t>Dynamique, TEC, Cinématique simple, SLCI avec Bode</t>
+  </si>
+  <si>
+    <t>2;3;4;5;6</t>
+  </si>
+  <si>
+    <t>DS5</t>
+  </si>
+  <si>
+    <t>Modélisation multiphysique d'un système</t>
+  </si>
+  <si>
+    <t>DS/central_2018</t>
+  </si>
+  <si>
+    <t>DS6</t>
+  </si>
+  <si>
+    <t>Modélisation d'un système d' Anti Blocage des Roues</t>
+  </si>
+  <si>
+    <t>Exosquelette</t>
+  </si>
+  <si>
+    <t>Twizy</t>
+  </si>
+  <si>
+    <t>Eolienne</t>
+  </si>
+  <si>
+    <t>automatique/ABS</t>
+  </si>
+  <si>
+    <t>Central TSI 2017</t>
+  </si>
+  <si>
+    <t>Mines-pont 2017</t>
+  </si>
+  <si>
+    <t>upsti</t>
+  </si>
+  <si>
+    <t>chaine fonctionnelle, schémas bloc, analyse temporelle</t>
+  </si>
+  <si>
+    <t>AF SysML, Frottement, résolution d'un problème de statique</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>DM2</t>
+  </si>
+  <si>
+    <t>Presse à vis</t>
+  </si>
+  <si>
+    <t>Assemblage Falcon</t>
+  </si>
+  <si>
+    <t>DS/presse_a_vis</t>
+  </si>
+  <si>
+    <t>e3a PSI 2017</t>
+  </si>
+  <si>
+    <t>e3a psi 2015</t>
+  </si>
+  <si>
+    <t>SLCI, correcteur à avance de phase</t>
+  </si>
+  <si>
+    <t>chaine fonctionnelle, schémas bloc, analyse temporelle et fréquentielle</t>
+  </si>
+  <si>
+    <t>2;3</t>
+  </si>
+  <si>
+    <t>DM3</t>
+  </si>
+  <si>
+    <t>Robot Kuka</t>
+  </si>
+  <si>
+    <t>Simulateur de vol</t>
+  </si>
+  <si>
+    <t>Tapis de course</t>
+  </si>
+  <si>
+    <t>DS/robot_kuka</t>
+  </si>
+  <si>
+    <t>CCP MP 2010</t>
+  </si>
+  <si>
+    <t>Central PSI 2017</t>
+  </si>
+  <si>
+    <t>PT SIB 2011</t>
+  </si>
+  <si>
+    <t>Cinématique/Statique</t>
+  </si>
+  <si>
+    <t>Cinématique, fermeture geo, statique, asservissement</t>
+  </si>
+  <si>
+    <t>Analyse fonctionnelle sans SysML, Cinétique, fermeture geo, Statique, PFD, statique, frottement, hyperstatisme, Energétique, Automatique</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>DM4</t>
+  </si>
+  <si>
+    <t>Modélisation d'une barrière automatique</t>
+  </si>
+  <si>
+    <t>Drone miniature</t>
+  </si>
+  <si>
+    <t>Clever</t>
+  </si>
+  <si>
+    <t>DS/canne_robotise</t>
+  </si>
+  <si>
+    <t>dynamique/barriere_sympact</t>
+  </si>
+  <si>
+    <t>Mines-pont 2010 MP</t>
+  </si>
+  <si>
+    <t>SIA 2013</t>
+  </si>
+  <si>
+    <t>Cinétique, dynamique, asservissement correcteur, AF avec SysML</t>
+  </si>
+  <si>
+    <t>4;5</t>
+  </si>
+  <si>
+    <t>3H</t>
+  </si>
+  <si>
+    <t>DM5</t>
+  </si>
+  <si>
+    <t>Modélisation d'une canne robotisée</t>
+  </si>
+  <si>
+    <t>DM6</t>
+  </si>
+  <si>
+    <t>Chargement et déchargement de porte-conteneur</t>
+  </si>
+  <si>
+    <t>Central PSI 2013</t>
+  </si>
+  <si>
+    <t>Dynamique Energétique, AF en SysML, SLCI</t>
+  </si>
+  <si>
+    <t>2;3;4;5;6;7</t>
+  </si>
+  <si>
+    <t>Algorithmique et programmation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1149,6 +1481,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1200,7 +1554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1466,6 +1820,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="654">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2123,7 +2579,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2363,18 +2819,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2424,42 +2916,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2488,6 +2944,90 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="654">
@@ -3457,13 +3997,1404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+      <c r="A2" s="128">
+        <v>1</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="130" t="s">
+        <v>442</v>
+      </c>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="131"/>
+      <c r="B3" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="131"/>
+      <c r="B4" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="132"/>
+      <c r="B5" s="133" t="s">
+        <v>355</v>
+      </c>
+      <c r="C5" s="135">
+        <v>43754</v>
+      </c>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="64" x14ac:dyDescent="0.15">
+      <c r="A2" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="128" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="130" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" s="130" t="s">
+        <v>339</v>
+      </c>
+      <c r="F2" s="130" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="130" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A3" s="127"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+      <c r="A4" s="127"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>347</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>349</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="127"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>352</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="127"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="127"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="133" t="s">
+        <v>355</v>
+      </c>
+      <c r="D7" s="134">
+        <v>43731</v>
+      </c>
+      <c r="E7" s="134">
+        <v>43731</v>
+      </c>
+      <c r="F7" s="135">
+        <v>43010</v>
+      </c>
+      <c r="G7" s="135">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+      <c r="A8" s="127"/>
+      <c r="B8" s="128" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D8" s="129" t="s">
+        <v>356</v>
+      </c>
+      <c r="E8" s="129" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" s="129" t="s">
+        <v>358</v>
+      </c>
+      <c r="G8" s="130" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A9" s="127"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+      <c r="A10" s="127"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="127"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="127"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="127"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="133" t="s">
+        <v>355</v>
+      </c>
+      <c r="D13" s="135">
+        <v>43745</v>
+      </c>
+      <c r="E13" s="135"/>
+      <c r="F13" s="135">
+        <v>43052</v>
+      </c>
+      <c r="G13" s="135">
+        <v>42660</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A14" s="127"/>
+      <c r="B14" s="136" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D14" s="137" t="s">
+        <v>367</v>
+      </c>
+      <c r="E14" s="137" t="s">
+        <v>367</v>
+      </c>
+      <c r="F14" s="137" t="s">
+        <v>368</v>
+      </c>
+      <c r="G14" s="137" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="127"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="138" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="91" x14ac:dyDescent="0.15">
+      <c r="A16" s="127"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="127"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="127"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="127"/>
+      <c r="B19" s="131"/>
+      <c r="C19" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D19" s="135">
+        <v>43781</v>
+      </c>
+      <c r="E19" s="139">
+        <v>43444</v>
+      </c>
+      <c r="F19" s="139">
+        <v>43087</v>
+      </c>
+      <c r="G19" s="139">
+        <v>42738</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="64" x14ac:dyDescent="0.15">
+      <c r="A20" s="127"/>
+      <c r="B20" s="136" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D20" s="137" t="s">
+        <v>377</v>
+      </c>
+      <c r="E20" s="137" t="s">
+        <v>378</v>
+      </c>
+      <c r="F20" s="137" t="s">
+        <v>379</v>
+      </c>
+      <c r="G20" s="137" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="127"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="78" x14ac:dyDescent="0.15">
+      <c r="A22" s="127"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42" t="s">
+        <v>385</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="127"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="127"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="127"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D25" s="139">
+        <v>43808</v>
+      </c>
+      <c r="E25" s="139">
+        <v>43114</v>
+      </c>
+      <c r="F25" s="139">
+        <v>43115</v>
+      </c>
+      <c r="G25" s="139">
+        <v>42800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A26" s="127"/>
+      <c r="B26" s="136" t="s">
+        <v>388</v>
+      </c>
+      <c r="C26" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D26" s="137" t="s">
+        <v>389</v>
+      </c>
+      <c r="E26" s="137" t="s">
+        <v>389</v>
+      </c>
+      <c r="F26" s="137" t="s">
+        <v>368</v>
+      </c>
+      <c r="G26" s="137" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="127"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="138" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+      <c r="A28" s="127"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="127"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="127"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="127"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D31" s="135">
+        <v>43857</v>
+      </c>
+      <c r="E31" s="139"/>
+      <c r="F31" s="139">
+        <v>43087</v>
+      </c>
+      <c r="G31" s="139">
+        <v>42738</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A32" s="127"/>
+      <c r="B32" s="136" t="s">
+        <v>391</v>
+      </c>
+      <c r="C32" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D32" s="137" t="s">
+        <v>389</v>
+      </c>
+      <c r="E32" s="137"/>
+      <c r="F32" s="137" t="s">
+        <v>379</v>
+      </c>
+      <c r="G32" s="137" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="127"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="78" x14ac:dyDescent="0.15">
+      <c r="A34" s="127"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42" t="s">
+        <v>385</v>
+      </c>
+      <c r="G34" s="42" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="127"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="127"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="127"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="141" t="s">
+        <v>355</v>
+      </c>
+      <c r="D37" s="134">
+        <v>43906</v>
+      </c>
+      <c r="E37" s="134"/>
+      <c r="F37" s="134">
+        <v>43115</v>
+      </c>
+      <c r="G37" s="134">
+        <v>42800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="89" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="142" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="128" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D38" s="130" t="s">
+        <v>392</v>
+      </c>
+      <c r="E38" s="130" t="s">
+        <v>393</v>
+      </c>
+      <c r="F38" s="130" t="s">
+        <v>394</v>
+      </c>
+      <c r="G38" s="143" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="144"/>
+      <c r="B39" s="131"/>
+      <c r="C39" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G39" s="145" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+      <c r="A40" s="144"/>
+      <c r="B40" s="131"/>
+      <c r="C40" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>349</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F40" s="42" t="s">
+        <v>400</v>
+      </c>
+      <c r="G40" s="145" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="144"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>352</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="145"/>
+    </row>
+    <row r="42" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="144"/>
+      <c r="B42" s="131"/>
+      <c r="C42" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="G42" s="145" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="144"/>
+      <c r="B43" s="140"/>
+      <c r="C43" s="141" t="s">
+        <v>355</v>
+      </c>
+      <c r="D43" s="134">
+        <v>43738</v>
+      </c>
+      <c r="E43" s="134">
+        <v>43364</v>
+      </c>
+      <c r="F43" s="134">
+        <v>42999</v>
+      </c>
+      <c r="G43" s="146">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="32" x14ac:dyDescent="0.15">
+      <c r="A44" s="144"/>
+      <c r="B44" s="131" t="s">
+        <v>403</v>
+      </c>
+      <c r="C44" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D44" s="137" t="s">
+        <v>404</v>
+      </c>
+      <c r="E44" s="137" t="s">
+        <v>404</v>
+      </c>
+      <c r="F44" s="137" t="s">
+        <v>405</v>
+      </c>
+      <c r="G44" s="147" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="144"/>
+      <c r="B45" s="131"/>
+      <c r="C45" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="G45" s="145"/>
+    </row>
+    <row r="46" spans="1:7" ht="78" x14ac:dyDescent="0.15">
+      <c r="A46" s="144"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>410</v>
+      </c>
+      <c r="G46" s="145"/>
+    </row>
+    <row r="47" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="144"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="145"/>
+    </row>
+    <row r="48" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="144"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="G48" s="145" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="144"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="141" t="s">
+        <v>355</v>
+      </c>
+      <c r="D49" s="134">
+        <v>43773</v>
+      </c>
+      <c r="E49" s="134"/>
+      <c r="F49" s="134">
+        <v>43026</v>
+      </c>
+      <c r="G49" s="146">
+        <v>42697</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="32" x14ac:dyDescent="0.15">
+      <c r="A50" s="144"/>
+      <c r="B50" s="136" t="s">
+        <v>412</v>
+      </c>
+      <c r="C50" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D50" s="130" t="s">
+        <v>413</v>
+      </c>
+      <c r="E50" s="130" t="s">
+        <v>413</v>
+      </c>
+      <c r="F50" s="130" t="s">
+        <v>414</v>
+      </c>
+      <c r="G50" s="143" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="144"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="G51" s="145" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="144"/>
+      <c r="B52" s="131"/>
+      <c r="C52" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="G52" s="145" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="144"/>
+      <c r="B53" s="131"/>
+      <c r="C53" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D53" s="3">
+        <v>4</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="145"/>
+    </row>
+    <row r="54" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="144"/>
+      <c r="B54" s="131"/>
+      <c r="C54" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="G54" s="145" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="144"/>
+      <c r="B55" s="132"/>
+      <c r="C55" s="133" t="s">
+        <v>355</v>
+      </c>
+      <c r="D55" s="135">
+        <v>43794</v>
+      </c>
+      <c r="E55" s="148"/>
+      <c r="F55" s="148">
+        <v>43040</v>
+      </c>
+      <c r="G55" s="149">
+        <v>42697</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A56" s="144"/>
+      <c r="B56" s="136" t="s">
+        <v>424</v>
+      </c>
+      <c r="C56" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D56" s="137" t="s">
+        <v>425</v>
+      </c>
+      <c r="E56" s="137" t="s">
+        <v>425</v>
+      </c>
+      <c r="F56" s="137" t="s">
+        <v>426</v>
+      </c>
+      <c r="G56" s="147" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="144"/>
+      <c r="B57" s="131"/>
+      <c r="C57" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="G57" s="145" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="144"/>
+      <c r="B58" s="131"/>
+      <c r="C58" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D58" s="138"/>
+      <c r="E58" s="138"/>
+      <c r="F58" s="138" t="s">
+        <v>432</v>
+      </c>
+      <c r="G58" s="145" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="144"/>
+      <c r="B59" s="131"/>
+      <c r="C59" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F59" s="42"/>
+      <c r="G59" s="145"/>
+    </row>
+    <row r="60" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="144"/>
+      <c r="B60" s="131"/>
+      <c r="C60" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="G60" s="145" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="144"/>
+      <c r="B61" s="131"/>
+      <c r="C61" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D61" s="135">
+        <v>43836</v>
+      </c>
+      <c r="E61" s="135"/>
+      <c r="F61" s="139">
+        <v>43091</v>
+      </c>
+      <c r="G61" s="150">
+        <v>42706</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="64" x14ac:dyDescent="0.15">
+      <c r="A62" s="144"/>
+      <c r="B62" s="136" t="s">
+        <v>435</v>
+      </c>
+      <c r="C62" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D62" s="151" t="s">
+        <v>436</v>
+      </c>
+      <c r="E62" s="151" t="s">
+        <v>436</v>
+      </c>
+      <c r="F62" s="137" t="s">
+        <v>368</v>
+      </c>
+      <c r="G62" s="147" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="144"/>
+      <c r="B63" s="131"/>
+      <c r="C63" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="152" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="104" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="144"/>
+      <c r="B64" s="131"/>
+      <c r="C64" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G64" s="145" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="144"/>
+      <c r="B65" s="131"/>
+      <c r="C65" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="F65" s="42"/>
+      <c r="G65" s="145"/>
+    </row>
+    <row r="66" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="144"/>
+      <c r="B66" s="131"/>
+      <c r="C66" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G66" s="145" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="144"/>
+      <c r="B67" s="131"/>
+      <c r="C67" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D67" s="139">
+        <v>43864</v>
+      </c>
+      <c r="E67" s="139">
+        <v>43864</v>
+      </c>
+      <c r="F67" s="139">
+        <v>43087</v>
+      </c>
+      <c r="G67" s="150">
+        <v>42738</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="48" x14ac:dyDescent="0.15">
+      <c r="A68" s="144"/>
+      <c r="B68" s="136" t="s">
+        <v>437</v>
+      </c>
+      <c r="C68" s="129" t="s">
+        <v>337</v>
+      </c>
+      <c r="D68" s="151" t="s">
+        <v>436</v>
+      </c>
+      <c r="E68" s="153"/>
+      <c r="F68" s="153"/>
+      <c r="G68" s="147" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="144"/>
+      <c r="B69" s="131"/>
+      <c r="C69" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="152" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="144"/>
+      <c r="B70" s="131"/>
+      <c r="C70" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="145" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="144"/>
+      <c r="B71" s="131"/>
+      <c r="C71" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="145"/>
+    </row>
+    <row r="72" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="144"/>
+      <c r="B72" s="131"/>
+      <c r="C72" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="145" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="154"/>
+      <c r="B73" s="132"/>
+      <c r="C73" s="133" t="s">
+        <v>355</v>
+      </c>
+      <c r="D73" s="135">
+        <v>43899</v>
+      </c>
+      <c r="E73" s="133"/>
+      <c r="F73" s="133"/>
+      <c r="G73" s="149">
+        <v>42755</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A38:A73"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="A2:A37"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B32:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3554,10 +5485,10 @@
       <c r="B2" s="9">
         <v>43711</v>
       </c>
-      <c r="C2" s="112">
+      <c r="C2" s="93">
         <v>1</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="96" t="s">
         <v>263</v>
       </c>
       <c r="E2" s="26">
@@ -3611,8 +5542,8 @@
         <f>B2+7</f>
         <v>43718</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="116"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="97"/>
       <c r="E3" s="26">
         <v>2</v>
       </c>
@@ -3663,8 +5594,8 @@
         <f>B3+7</f>
         <v>43725</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="116"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="26">
         <v>2</v>
       </c>
@@ -3716,8 +5647,8 @@
         <f t="shared" ref="B5:B8" si="0">B4+7</f>
         <v>43732</v>
       </c>
-      <c r="C5" s="113"/>
-      <c r="D5" s="116"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="97"/>
       <c r="E5" s="26">
         <v>3</v>
       </c>
@@ -3769,8 +5700,8 @@
         <f>B5+7</f>
         <v>43739</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="116"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="97"/>
       <c r="E6" s="26">
         <v>4</v>
       </c>
@@ -3809,7 +5740,9 @@
       <c r="R6" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="33"/>
+      <c r="S6" s="33" t="s">
+        <v>321</v>
+      </c>
       <c r="V6" s="70"/>
       <c r="W6" s="75"/>
       <c r="X6" s="75"/>
@@ -3822,8 +5755,8 @@
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="116"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="26">
         <v>4</v>
       </c>
@@ -3856,7 +5789,9 @@
       <c r="R7" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="32"/>
+      <c r="S7" s="32" t="s">
+        <v>321</v>
+      </c>
       <c r="V7" s="70"/>
       <c r="W7" s="75"/>
       <c r="X7" s="75"/>
@@ -3869,8 +5804,8 @@
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
-      <c r="C8" s="114"/>
-      <c r="D8" s="117"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="98"/>
       <c r="E8" s="26">
         <v>5</v>
       </c>
@@ -3914,24 +5849,24 @@
       <c r="X8" s="75"/>
     </row>
     <row r="9" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="88"/>
-      <c r="P9" s="88"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="92"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="41"/>
       <c r="S9" s="32"/>
@@ -3947,10 +5882,10 @@
         <f>B8+21</f>
         <v>43774</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="93">
         <v>1</v>
       </c>
-      <c r="D10" s="115" t="s">
+      <c r="D10" s="96" t="s">
         <v>263</v>
       </c>
       <c r="E10" s="26">
@@ -4000,8 +5935,8 @@
         <f t="shared" ref="B11:B16" si="1">B10+7</f>
         <v>43781</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="116"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="26">
         <v>6</v>
       </c>
@@ -4047,8 +5982,8 @@
         <f t="shared" si="1"/>
         <v>43788</v>
       </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="116"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="26">
         <v>6</v>
       </c>
@@ -4093,8 +6028,8 @@
         <f t="shared" si="1"/>
         <v>43795</v>
       </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="116"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="97"/>
       <c r="E13" s="26">
         <v>7</v>
       </c>
@@ -4142,8 +6077,8 @@
         <f t="shared" si="1"/>
         <v>43802</v>
       </c>
-      <c r="C14" s="113"/>
-      <c r="D14" s="116"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="97"/>
       <c r="E14" s="26">
         <v>7</v>
       </c>
@@ -4190,8 +6125,8 @@
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
-      <c r="C15" s="113"/>
-      <c r="D15" s="116"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="97"/>
       <c r="E15" s="26">
         <v>8</v>
       </c>
@@ -4241,8 +6176,8 @@
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
-      <c r="C16" s="114"/>
-      <c r="D16" s="117"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="98"/>
       <c r="E16" s="26">
         <v>8</v>
       </c>
@@ -4283,24 +6218,24 @@
       <c r="X16" s="75"/>
     </row>
     <row r="17" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="88"/>
-      <c r="P17" s="88"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="41"/>
       <c r="S17" s="32"/>
@@ -4316,10 +6251,10 @@
         <f>B16+21</f>
         <v>43837</v>
       </c>
-      <c r="C18" s="106">
+      <c r="C18" s="85">
         <v>2</v>
       </c>
-      <c r="D18" s="109" t="s">
+      <c r="D18" s="88" t="s">
         <v>186</v>
       </c>
       <c r="E18" s="28">
@@ -4369,8 +6304,8 @@
         <f>B18+7</f>
         <v>43844</v>
       </c>
-      <c r="C19" s="107"/>
-      <c r="D19" s="110"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="89"/>
       <c r="E19" s="28">
         <v>1</v>
       </c>
@@ -4418,8 +6353,8 @@
         <f t="shared" ref="B20:B40" si="2">B19+7</f>
         <v>43851</v>
       </c>
-      <c r="C20" s="107"/>
-      <c r="D20" s="110"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="28">
         <v>2</v>
       </c>
@@ -4467,8 +6402,8 @@
         <f>B20+7</f>
         <v>43858</v>
       </c>
-      <c r="C21" s="108"/>
-      <c r="D21" s="111"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="90"/>
       <c r="E21" s="28">
         <v>2</v>
       </c>
@@ -4516,10 +6451,10 @@
         <f>B21+7</f>
         <v>43865</v>
       </c>
-      <c r="C22" s="92">
+      <c r="C22" s="104">
         <v>3</v>
       </c>
-      <c r="D22" s="89" t="s">
+      <c r="D22" s="101" t="s">
         <v>61</v>
       </c>
       <c r="E22" s="35">
@@ -4569,8 +6504,8 @@
         <f>B22+7</f>
         <v>43872</v>
       </c>
-      <c r="C23" s="93"/>
-      <c r="D23" s="90"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="102"/>
       <c r="E23" s="35">
         <v>2</v>
       </c>
@@ -4617,8 +6552,8 @@
         <f>B23+7</f>
         <v>43879</v>
       </c>
-      <c r="C24" s="94"/>
-      <c r="D24" s="91"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="103"/>
       <c r="E24" s="34">
         <v>2</v>
       </c>
@@ -4654,24 +6589,24 @@
       <c r="S24" s="33"/>
     </row>
     <row r="25" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="87" t="s">
+      <c r="A25" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="88"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="88"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="92"/>
+      <c r="N25" s="92"/>
+      <c r="O25" s="92"/>
+      <c r="P25" s="92"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="50"/>
       <c r="S25" s="32"/>
@@ -4687,10 +6622,10 @@
         <f>B24+21</f>
         <v>43900</v>
       </c>
-      <c r="C26" s="92">
+      <c r="C26" s="104">
         <v>3</v>
       </c>
-      <c r="D26" s="89" t="s">
+      <c r="D26" s="101" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="29">
@@ -4740,8 +6675,8 @@
         <f t="shared" si="2"/>
         <v>43907</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="90"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="102"/>
       <c r="E27" s="35">
         <v>3</v>
       </c>
@@ -4786,8 +6721,8 @@
         <f t="shared" si="2"/>
         <v>43914</v>
       </c>
-      <c r="C28" s="93"/>
-      <c r="D28" s="90"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="102"/>
       <c r="E28" s="29">
         <v>4</v>
       </c>
@@ -4835,8 +6770,8 @@
         <f t="shared" si="2"/>
         <v>43921</v>
       </c>
-      <c r="C29" s="94"/>
-      <c r="D29" s="91"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="103"/>
       <c r="E29" s="35">
         <v>4</v>
       </c>
@@ -4882,10 +6817,10 @@
         <f t="shared" si="2"/>
         <v>43928</v>
       </c>
-      <c r="C30" s="95">
+      <c r="C30" s="107">
         <v>4</v>
       </c>
-      <c r="D30" s="97" t="s">
+      <c r="D30" s="109" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="30">
@@ -4937,8 +6872,8 @@
         <f t="shared" si="2"/>
         <v>43935</v>
       </c>
-      <c r="C31" s="96"/>
-      <c r="D31" s="98"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="110"/>
       <c r="E31" s="30">
         <v>2</v>
       </c>
@@ -4979,24 +6914,24 @@
       <c r="X31" s="75"/>
     </row>
     <row r="32" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="85" t="s">
+      <c r="A32" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="86"/>
-      <c r="M32" s="86"/>
-      <c r="N32" s="86"/>
-      <c r="O32" s="86"/>
-      <c r="P32" s="86"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="100"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="100"/>
       <c r="Q32" s="47"/>
       <c r="R32" s="51"/>
       <c r="S32" s="32"/>
@@ -5012,10 +6947,10 @@
         <f>B31+21</f>
         <v>43956</v>
       </c>
-      <c r="C33" s="95">
+      <c r="C33" s="107">
         <v>4</v>
       </c>
-      <c r="D33" s="97" t="s">
+      <c r="D33" s="109" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="30">
@@ -5060,8 +6995,8 @@
         <f t="shared" si="2"/>
         <v>43963</v>
       </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="99"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="111"/>
       <c r="E34" s="30">
         <v>3</v>
       </c>
@@ -5106,8 +7041,8 @@
         <f t="shared" si="2"/>
         <v>43970</v>
       </c>
-      <c r="C35" s="96"/>
-      <c r="D35" s="98"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="110"/>
       <c r="E35" s="30">
         <v>4</v>
       </c>
@@ -5151,10 +7086,10 @@
         <f t="shared" si="2"/>
         <v>43977</v>
       </c>
-      <c r="C36" s="103">
+      <c r="C36" s="115">
         <v>5</v>
       </c>
-      <c r="D36" s="101" t="s">
+      <c r="D36" s="113" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="31">
@@ -5194,8 +7129,8 @@
         <f t="shared" si="2"/>
         <v>43984</v>
       </c>
-      <c r="C37" s="104"/>
-      <c r="D37" s="102"/>
+      <c r="C37" s="116"/>
+      <c r="D37" s="114"/>
       <c r="E37" s="31">
         <v>1</v>
       </c>
@@ -5235,8 +7170,8 @@
         <f t="shared" si="2"/>
         <v>43991</v>
       </c>
-      <c r="C38" s="104"/>
-      <c r="D38" s="102"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="114"/>
       <c r="E38" s="31">
         <v>1</v>
       </c>
@@ -5274,8 +7209,8 @@
         <f t="shared" si="2"/>
         <v>43998</v>
       </c>
-      <c r="C39" s="104"/>
-      <c r="D39" s="102"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="114"/>
       <c r="E39" s="31">
         <v>1</v>
       </c>
@@ -5313,8 +7248,8 @@
         <f t="shared" si="2"/>
         <v>44005</v>
       </c>
-      <c r="C40" s="105"/>
-      <c r="D40" s="102"/>
+      <c r="C40" s="117"/>
+      <c r="D40" s="114"/>
       <c r="E40" s="31">
         <v>1</v>
       </c>
@@ -5343,24 +7278,24 @@
       <c r="X40" s="75"/>
     </row>
     <row r="41" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
-      <c r="M41" s="86"/>
-      <c r="N41" s="86"/>
-      <c r="O41" s="86"/>
-      <c r="P41" s="86"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
+      <c r="H41" s="100"/>
+      <c r="I41" s="100"/>
+      <c r="J41" s="100"/>
+      <c r="K41" s="100"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="100"/>
+      <c r="N41" s="100"/>
+      <c r="O41" s="100"/>
+      <c r="P41" s="100"/>
       <c r="Q41" s="47"/>
       <c r="R41" s="51"/>
       <c r="V41" s="70"/>
@@ -5429,14 +7364,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="A9:P9"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D10:D16"/>
-    <mergeCell ref="C10:C16"/>
     <mergeCell ref="A41:P41"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A25:P25"/>
@@ -5450,6 +7377,14 @@
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="D36:D40"/>
     <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A9:P9"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D10:D16"/>
+    <mergeCell ref="C10:C16"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5457,7 +7392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -5528,7 +7463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
@@ -6228,7 +8163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>

</xml_diff>

<commit_message>
modifi TP06 statistiques chaines de caracteres
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="355">
   <si>
     <t>Cours</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Tracé de fonctions</t>
-  </si>
-  <si>
-    <t>Tableaux et chaines de caractères</t>
   </si>
   <si>
     <t>Complexité</t>
@@ -1116,6 +1113,12 @@
   </si>
   <si>
     <t>consignes/consignes_TP6;fichiers/FIC-009;fichiers/FIC-011;fichiers/FIC-012</t>
+  </si>
+  <si>
+    <t>AA.C9; AA.S12; AA.C2: AA.C3; AA.S4; AA.S5</t>
+  </si>
+  <si>
+    <t>Tableaux, chaines de caractères et fichiers</t>
   </si>
 </sst>
 </file>
@@ -3601,16 +3604,16 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.15">
@@ -3618,10 +3621,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="85" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D2" s="86"/>
       <c r="E2" s="86"/>
@@ -3630,10 +3633,10 @@
     <row r="3" spans="1:8" ht="78" x14ac:dyDescent="0.15">
       <c r="A3" s="96"/>
       <c r="B3" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -3642,10 +3645,10 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="96"/>
       <c r="B4" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>342</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>343</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="42"/>
@@ -3654,7 +3657,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="96"/>
       <c r="B5" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C5" s="42">
         <v>1</v>
@@ -3666,7 +3669,7 @@
     <row r="6" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="97"/>
       <c r="B6" s="87" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C6" s="88">
         <v>43754</v>
@@ -3680,10 +3683,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C7" s="86" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D7" s="86"/>
       <c r="E7" s="86"/>
@@ -3692,10 +3695,10 @@
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="96"/>
       <c r="B8" s="90" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D8" s="90"/>
       <c r="E8" s="90"/>
@@ -3704,22 +3707,22 @@
     <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="96"/>
       <c r="B9" s="90" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D9" s="90"/>
       <c r="E9" s="42"/>
       <c r="F9" s="90"/>
       <c r="H9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="96"/>
       <c r="B10" s="90" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C10" s="42">
         <v>1</v>
@@ -3731,7 +3734,7 @@
     <row r="11" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="97"/>
       <c r="B11" s="91" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11" s="88">
         <v>43798</v>
@@ -3745,10 +3748,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C12" s="86" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D12" s="86"/>
       <c r="E12" s="86"/>
@@ -3757,10 +3760,10 @@
     <row r="13" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="96"/>
       <c r="B13" s="93" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D13" s="93"/>
       <c r="E13" s="93"/>
@@ -3769,22 +3772,22 @@
     <row r="14" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="96"/>
       <c r="B14" s="93" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D14" s="93"/>
       <c r="E14" s="42"/>
       <c r="F14" s="93"/>
       <c r="H14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="96"/>
       <c r="B15" s="93" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C15" s="42">
         <v>1</v>
@@ -3796,7 +3799,7 @@
     <row r="16" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="97"/>
       <c r="B16" s="94" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C16" s="88">
         <v>43798</v>
@@ -3807,7 +3810,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3827,8 +3830,8 @@
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3885,16 +3888,16 @@
         <v>1</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="M1" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>13</v>
@@ -3903,10 +3906,10 @@
         <v>22</v>
       </c>
       <c r="Q1" s="41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S1" s="32" t="s">
         <v>24</v>
@@ -3923,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="128" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E2" s="26">
         <v>1</v>
@@ -3945,24 +3948,24 @@
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M2" s="83" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N2" s="83" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="42"/>
       <c r="Q2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R2" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V2" s="70"/>
       <c r="W2" s="75"/>
@@ -3982,13 +3985,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="26">
         <v>2</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I3" s="11">
         <v>1</v>
@@ -3997,24 +4000,24 @@
         <v>27</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M3" s="83" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N3" s="83" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="42"/>
       <c r="Q3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R3" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S3" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V3" s="70"/>
       <c r="W3" s="75"/>
@@ -4034,13 +4037,13 @@
         <v>2</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G4" s="26">
         <v>2</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I4" s="11">
         <v>2</v>
@@ -4050,24 +4053,24 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M4" s="73" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N4" s="83" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="42"/>
       <c r="Q4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R4" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S4" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V4" s="70"/>
       <c r="W4" s="75"/>
@@ -4102,25 +4105,25 @@
         <v>34</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N5" s="83" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="42"/>
       <c r="Q5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R5" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S5" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V5" s="70"/>
       <c r="W5" s="75"/>
@@ -4152,30 +4155,30 @@
         <v>3</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K6" s="82" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L6" s="82" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N6" s="83" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="42"/>
       <c r="Q6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R6" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S6" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V6" s="70"/>
       <c r="W6" s="75"/>
@@ -4213,18 +4216,18 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="83" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R7" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S7" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V7" s="70"/>
       <c r="W7" s="75"/>
@@ -4259,26 +4262,26 @@
         <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L8" s="82" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M8" s="78" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N8" s="73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R8" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S8" s="33"/>
       <c r="V8" s="70"/>
@@ -4323,7 +4326,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="128" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E10" s="26">
         <v>5</v>
@@ -4346,18 +4349,18 @@
       <c r="K10" s="5"/>
       <c r="L10" s="82"/>
       <c r="M10" s="78" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N10" s="73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="42"/>
       <c r="Q10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R10" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S10" s="32"/>
       <c r="V10" s="70"/>
@@ -4393,22 +4396,22 @@
         <v>36</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L11" s="82" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M11" s="78" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="3"/>
       <c r="P11" s="42"/>
       <c r="Q11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R11" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S11" s="33"/>
       <c r="V11" s="70"/>
@@ -4446,16 +4449,16 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="78" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="3"/>
       <c r="P12" s="42"/>
       <c r="Q12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R12" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V12" s="70"/>
       <c r="W12" s="75"/>
@@ -4487,27 +4490,27 @@
         <v>6</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>37</v>
+        <v>354</v>
       </c>
       <c r="K13" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="M13" s="78" t="s">
+      <c r="N13" s="78" t="s">
         <v>275</v>
-      </c>
-      <c r="N13" s="78" t="s">
-        <v>276</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="42"/>
       <c r="Q13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R13" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S13" s="33"/>
       <c r="V13" s="70"/>
@@ -4540,23 +4543,23 @@
         <v>6</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>37</v>
+        <v>354</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="78" t="s">
+      <c r="M14" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="N14" s="78" t="s">
         <v>275</v>
-      </c>
-      <c r="N14" s="78" t="s">
-        <v>276</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="42"/>
       <c r="Q14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R14" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V14" s="70"/>
       <c r="W14" s="75"/>
@@ -4592,21 +4595,21 @@
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="73" t="s">
-        <v>270</v>
+      <c r="M15" s="83" t="s">
+        <v>269</v>
       </c>
       <c r="N15" s="78" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P15" s="42"/>
       <c r="Q15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R15" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S15" s="33"/>
       <c r="V15" s="70"/>
@@ -4644,18 +4647,18 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="73" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N16" s="78" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="36"/>
       <c r="Q16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R16" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S16" s="32"/>
       <c r="V16" s="70"/>
@@ -4700,41 +4703,41 @@
         <v>2</v>
       </c>
       <c r="D18" s="122" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E18" s="28">
         <v>1</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="28">
         <v>1</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I18" s="13">
         <v>8</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="84" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N18" s="84" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O18" s="27"/>
       <c r="P18" s="43"/>
       <c r="Q18" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R18" s="49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S18" s="33"/>
       <c r="V18" s="70"/>
@@ -4755,35 +4758,35 @@
         <v>1</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="28">
         <v>1</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I19" s="13">
         <v>8</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="84" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N19" s="84" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O19" s="27"/>
       <c r="P19" s="43"/>
       <c r="Q19" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R19" s="49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S19" s="33"/>
       <c r="V19" s="70"/>
@@ -4804,35 +4807,35 @@
         <v>2</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="28">
         <v>2</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I20" s="13">
         <v>9</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N20" s="73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="42"/>
       <c r="Q20" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R20" s="49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S20" s="33"/>
       <c r="V20" s="70"/>
@@ -4853,35 +4856,35 @@
         <v>2</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="28">
         <v>2</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I21" s="13">
         <v>9</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N21" s="73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="42"/>
       <c r="Q21" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R21" s="49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S21" s="33"/>
       <c r="V21" s="70"/>
@@ -4900,41 +4903,41 @@
         <v>3</v>
       </c>
       <c r="D22" s="102" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="35">
         <v>1</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G22" s="35">
         <v>1</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" s="15">
         <v>10</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N22" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="42"/>
       <c r="Q22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R22" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S22" s="32"/>
       <c r="V22" s="70"/>
@@ -4955,37 +4958,37 @@
         <v>2</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" s="35">
         <v>2</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I23" s="15">
         <v>10</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N23" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="P23" s="42"/>
       <c r="Q23" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R23" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S23" s="33"/>
     </row>
@@ -5003,33 +5006,33 @@
         <v>2</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="35">
         <v>2</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="15">
         <v>11</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N24" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O24" s="27"/>
       <c r="P24" s="42"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S24" s="33"/>
     </row>
@@ -5071,41 +5074,41 @@
         <v>3</v>
       </c>
       <c r="D26" s="102" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" s="29">
         <v>3</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G26" s="35">
         <v>3</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I26" s="15">
         <v>11</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N26" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O26" s="27"/>
       <c r="P26" s="42"/>
       <c r="Q26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R26" s="52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S26" s="32"/>
       <c r="V26" s="70"/>
@@ -5126,32 +5129,32 @@
         <v>3</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G27" s="35">
         <v>3</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I27" s="15">
         <v>12</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N27" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P27" s="36"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S27" s="33"/>
       <c r="V27" s="70"/>
@@ -5172,35 +5175,35 @@
         <v>4</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" s="29">
         <v>4</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28" s="15">
         <v>12</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N28" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R28" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S28" s="32"/>
       <c r="V28" s="70"/>
@@ -5221,33 +5224,33 @@
         <v>4</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G29" s="35">
         <v>4</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I29" s="15">
         <v>13</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N29" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="42"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S29" s="33"/>
       <c r="V29" s="70"/>
@@ -5266,43 +5269,43 @@
         <v>4</v>
       </c>
       <c r="D30" s="110" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="30">
         <v>1</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G30" s="30">
         <v>1</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I30" s="15">
         <v>13</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="73" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N30" s="73" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P30" s="36"/>
       <c r="Q30" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R30" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S30" s="32"/>
       <c r="V30" s="70"/>
@@ -5323,35 +5326,35 @@
         <v>2</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G31" s="30">
         <v>2</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I31" s="18">
         <v>14</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K31" s="39"/>
       <c r="L31" s="39"/>
       <c r="M31" s="73" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N31" s="73" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O31" s="27"/>
       <c r="P31" s="43"/>
       <c r="Q31" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R31" s="53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S31" s="32"/>
       <c r="V31" s="70"/>
@@ -5396,39 +5399,39 @@
         <v>4</v>
       </c>
       <c r="D33" s="110" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E33" s="30">
         <v>2</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G33" s="30">
         <v>2</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I33" s="18">
         <v>14</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K33" s="38"/>
       <c r="L33" s="38"/>
       <c r="M33" s="73" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N33" s="73" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O33" s="6"/>
       <c r="P33" s="44"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S33" s="33"/>
     </row>
@@ -5446,35 +5449,35 @@
         <v>3</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G34" s="30">
         <v>3</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I34" s="18">
         <v>15</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K34" s="39"/>
       <c r="L34" s="39"/>
       <c r="M34" s="76" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N34" s="76" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="44"/>
       <c r="Q34" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R34" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S34" s="32"/>
     </row>
@@ -5492,13 +5495,13 @@
         <v>4</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G35" s="30">
         <v>4</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I35" s="21">
         <v>15</v>
@@ -5509,17 +5512,17 @@
       <c r="K35" s="39"/>
       <c r="L35" s="39"/>
       <c r="M35" s="77" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N35" s="77" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P35" s="36"/>
       <c r="Q35" s="78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R35" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S35" s="46"/>
     </row>
@@ -5535,13 +5538,13 @@
         <v>5</v>
       </c>
       <c r="D36" s="114" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="31">
         <v>1</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="20"/>
@@ -5549,7 +5552,7 @@
         <v>15</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K36" s="39"/>
       <c r="L36" s="39"/>
@@ -5559,7 +5562,7 @@
       <c r="P36" s="45"/>
       <c r="Q36" s="7"/>
       <c r="R36" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S36" s="33"/>
       <c r="V36" s="70"/>
@@ -5580,7 +5583,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="20"/>
@@ -5588,7 +5591,7 @@
         <v>15</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K37" s="39"/>
       <c r="L37" s="39"/>
@@ -5600,7 +5603,7 @@
       <c r="P37" s="36"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S37" s="46"/>
       <c r="V37" s="70"/>
@@ -5621,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="20"/>
@@ -5629,7 +5632,7 @@
         <v>15</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -5639,7 +5642,7 @@
       <c r="P38" s="36"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S38" s="33"/>
       <c r="V38" s="70"/>
@@ -5660,7 +5663,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="20"/>
@@ -5668,7 +5671,7 @@
         <v>15</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -5678,7 +5681,7 @@
       <c r="P39" s="43"/>
       <c r="Q39" s="27"/>
       <c r="R39" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S39" s="46"/>
       <c r="V39" s="70"/>
@@ -5699,7 +5702,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="20"/>
@@ -5707,7 +5710,7 @@
         <v>15</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K40" s="40"/>
       <c r="L40" s="40"/>
@@ -5715,7 +5718,7 @@
       <c r="N40" s="40"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S40" s="33"/>
       <c r="V40" s="70"/>
@@ -5866,23 +5869,23 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
@@ -5890,7 +5893,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
@@ -5898,7 +5901,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -5926,393 +5929,393 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="C1" s="71" t="s">
         <v>244</v>
-      </c>
-      <c r="C1" s="71" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C4" s="71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="71" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" s="71" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="70" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10" s="71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="71" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="70" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14" s="71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B17" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="71" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20" s="71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21" s="71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B22" s="71" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B23" s="71" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C23" s="71" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="71" t="s">
+        <v>295</v>
+      </c>
+      <c r="C24" s="71" t="s">
         <v>296</v>
-      </c>
-      <c r="C24" s="71" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B27" s="80" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C27" s="80" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="79" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B28" s="80" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" s="80" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="79" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B30" s="80" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C30" s="80" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="79" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B31" s="80" t="s">
+        <v>300</v>
+      </c>
+      <c r="C31" s="80" t="s">
         <v>301</v>
-      </c>
-      <c r="C31" s="80" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="79" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B32" s="80" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C32" s="80" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B33" s="71" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C33" s="71" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B34" s="71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B35" s="71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B37" s="71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A38" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B38" s="71" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39" s="71" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C39" s="71" t="s">
         <v>32</v>
@@ -6320,285 +6323,285 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A42" s="70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B42" s="71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C42" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A43" s="70" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A44" s="70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B44" s="71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B45" s="71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45" s="71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="70" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B46" s="71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B47" s="71" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A48" s="70" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B48" s="71" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B49" s="71" t="s">
+        <v>310</v>
+      </c>
+      <c r="C49" s="71" t="s">
         <v>311</v>
-      </c>
-      <c r="C49" s="71" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A50" s="70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B50" s="71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C50" s="71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B53" s="71" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C53" s="71" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B54" s="71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C54" s="71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B55" s="71" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C55" s="71" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B56" s="71" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C56" s="71" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C57" s="71" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C58" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B59" s="71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C59" s="71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A60" s="70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B60" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C60" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="70" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B61" s="71" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C61" s="71" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C63" s="71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="70" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B64" s="71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C64" s="71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B65" s="71" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C65" s="71" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="36" x14ac:dyDescent="0.15">
       <c r="A66" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B66" s="71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C66" s="71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="70" t="s">
+        <v>321</v>
+      </c>
+      <c r="B67" s="71" t="s">
         <v>322</v>
       </c>
-      <c r="B67" s="71" t="s">
-        <v>323</v>
-      </c>
       <c r="C67" s="71" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="70" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -6624,7 +6627,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="131" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="132"/>
       <c r="C1" s="132"/>
@@ -6632,10 +6635,10 @@
     </row>
     <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>81</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="56"/>
@@ -6644,7 +6647,7 @@
       <c r="A3" s="54"/>
       <c r="B3" s="55"/>
       <c r="C3" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="56"/>
     </row>
@@ -6652,7 +6655,7 @@
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="56"/>
     </row>
@@ -6660,7 +6663,7 @@
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="56"/>
     </row>
@@ -6672,44 +6675,44 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>85</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>86</v>
       </c>
       <c r="C7" s="55"/>
       <c r="D7" s="56"/>
     </row>
     <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A8" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>87</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>88</v>
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="54"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="56" t="s">
         <v>90</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="56" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="59" t="s">
         <v>92</v>
-      </c>
-      <c r="D10" s="59" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -6720,7 +6723,7 @@
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="131" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="132"/>
       <c r="C12" s="132"/>
@@ -6728,80 +6731,80 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="55" t="s">
         <v>95</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>96</v>
       </c>
       <c r="C13" s="55"/>
       <c r="D13" s="56"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="55" t="s">
         <v>97</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>98</v>
       </c>
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="55" t="s">
         <v>99</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>100</v>
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="56"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="55" t="s">
         <v>101</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>102</v>
       </c>
       <c r="C16" s="55"/>
       <c r="D16" s="56"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="55" t="s">
         <v>103</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>104</v>
       </c>
       <c r="C17" s="55"/>
       <c r="D17" s="56"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="55" t="s">
         <v>105</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>106</v>
       </c>
       <c r="C18" s="55"/>
       <c r="D18" s="56"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="55" t="s">
         <v>107</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>108</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="56"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="55" t="s">
         <v>109</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>110</v>
       </c>
       <c r="C20" s="55"/>
       <c r="D20" s="56"/>
@@ -6810,7 +6813,7 @@
       <c r="A21" s="54"/>
       <c r="B21" s="55"/>
       <c r="C21" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="56"/>
     </row>
@@ -6818,7 +6821,7 @@
       <c r="A22" s="54"/>
       <c r="B22" s="55"/>
       <c r="C22" s="55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="56"/>
     </row>
@@ -6826,7 +6829,7 @@
       <c r="A23" s="54"/>
       <c r="B23" s="55"/>
       <c r="C23" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D23" s="56"/>
     </row>
@@ -6834,7 +6837,7 @@
       <c r="A24" s="54"/>
       <c r="B24" s="55"/>
       <c r="C24" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D24" s="56"/>
     </row>
@@ -6842,7 +6845,7 @@
       <c r="A25" s="54"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D25" s="56"/>
     </row>
@@ -6854,60 +6857,60 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="55" t="s">
         <v>116</v>
-      </c>
-      <c r="B27" s="55" t="s">
-        <v>117</v>
       </c>
       <c r="C27" s="55"/>
       <c r="D27" s="56"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="55" t="s">
         <v>118</v>
-      </c>
-      <c r="B28" s="55" t="s">
-        <v>119</v>
       </c>
       <c r="C28" s="55"/>
       <c r="D28" s="56"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="55" t="s">
         <v>120</v>
-      </c>
-      <c r="B29" s="55" t="s">
-        <v>121</v>
       </c>
       <c r="C29" s="55"/>
       <c r="D29" s="56"/>
     </row>
     <row r="30" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A30" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="55" t="s">
         <v>122</v>
-      </c>
-      <c r="B30" s="55" t="s">
-        <v>123</v>
       </c>
       <c r="C30" s="55"/>
       <c r="D30" s="56"/>
     </row>
     <row r="31" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A31" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="55" t="s">
         <v>124</v>
-      </c>
-      <c r="B31" s="55" t="s">
-        <v>125</v>
       </c>
       <c r="C31" s="55"/>
       <c r="D31" s="56"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="55" t="s">
         <v>126</v>
-      </c>
-      <c r="B32" s="55" t="s">
-        <v>127</v>
       </c>
       <c r="C32" s="55"/>
       <c r="D32" s="56"/>
@@ -6916,70 +6919,70 @@
       <c r="A33" s="54"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="56" t="s">
         <v>128</v>
-      </c>
-      <c r="D33" s="56" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A34" s="54"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="56" t="s">
         <v>130</v>
-      </c>
-      <c r="D34" s="56" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A35" s="54"/>
       <c r="B35" s="55"/>
       <c r="C35" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="56" t="s">
         <v>132</v>
-      </c>
-      <c r="D35" s="56" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A36" s="54"/>
       <c r="B36" s="55"/>
       <c r="C36" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="56" t="s">
         <v>134</v>
-      </c>
-      <c r="D36" s="56" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A37" s="54"/>
       <c r="B37" s="55"/>
       <c r="C37" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="56" t="s">
         <v>136</v>
-      </c>
-      <c r="D37" s="56" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="55" x14ac:dyDescent="0.15">
       <c r="A38" s="54"/>
       <c r="B38" s="55"/>
       <c r="C38" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="56" t="s">
         <v>138</v>
-      </c>
-      <c r="D38" s="56" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="34" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="57"/>
       <c r="B39" s="58"/>
       <c r="C39" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="59" t="s">
         <v>140</v>
-      </c>
-      <c r="D39" s="59" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -6990,7 +6993,7 @@
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B41" s="135"/>
       <c r="C41" s="135"/>
@@ -6998,50 +7001,50 @@
     </row>
     <row r="42" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A42" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="62" t="s">
         <v>143</v>
-      </c>
-      <c r="B42" s="62" t="s">
-        <v>144</v>
       </c>
       <c r="C42" s="62"/>
       <c r="D42" s="63"/>
     </row>
     <row r="43" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A43" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="62" t="s">
         <v>145</v>
-      </c>
-      <c r="B43" s="62" t="s">
-        <v>146</v>
       </c>
       <c r="C43" s="62"/>
       <c r="D43" s="63"/>
     </row>
     <row r="44" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A44" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="62" t="s">
         <v>147</v>
-      </c>
-      <c r="B44" s="62" t="s">
-        <v>148</v>
       </c>
       <c r="C44" s="62"/>
       <c r="D44" s="63"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="62" t="s">
         <v>149</v>
-      </c>
-      <c r="B45" s="62" t="s">
-        <v>150</v>
       </c>
       <c r="C45" s="62"/>
       <c r="D45" s="63"/>
     </row>
     <row r="46" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A46" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="62" t="s">
         <v>151</v>
-      </c>
-      <c r="B46" s="62" t="s">
-        <v>152</v>
       </c>
       <c r="C46" s="62"/>
       <c r="D46" s="63"/>
@@ -7050,40 +7053,40 @@
       <c r="A47" s="54"/>
       <c r="B47" s="62"/>
       <c r="C47" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="63" t="s">
         <v>153</v>
-      </c>
-      <c r="D47" s="63" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A48" s="54"/>
       <c r="B48" s="62"/>
       <c r="C48" s="62" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="63" t="s">
         <v>155</v>
-      </c>
-      <c r="D48" s="63" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A49" s="54"/>
       <c r="B49" s="62"/>
       <c r="C49" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="63" t="s">
         <v>157</v>
-      </c>
-      <c r="D49" s="63" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="67" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="57"/>
       <c r="B50" s="64"/>
       <c r="C50" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="65" t="s">
         <v>159</v>
-      </c>
-      <c r="D50" s="65" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7094,7 +7097,7 @@
     </row>
     <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="137" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B52" s="138"/>
       <c r="C52" s="138"/>
@@ -7102,50 +7105,50 @@
     </row>
     <row r="53" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A53" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="68" t="s">
         <v>162</v>
-      </c>
-      <c r="B53" s="68" t="s">
-        <v>163</v>
       </c>
       <c r="C53" s="68"/>
       <c r="D53" s="68"/>
     </row>
     <row r="54" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A54" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="55" t="s">
         <v>164</v>
-      </c>
-      <c r="B54" s="55" t="s">
-        <v>165</v>
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
     </row>
     <row r="55" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A55" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="55" t="s">
         <v>166</v>
-      </c>
-      <c r="B55" s="55" t="s">
-        <v>167</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
     </row>
     <row r="56" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A56" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B56" s="55" t="s">
         <v>168</v>
-      </c>
-      <c r="B56" s="55" t="s">
-        <v>169</v>
       </c>
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
     </row>
     <row r="57" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A57" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="55" t="s">
         <v>170</v>
-      </c>
-      <c r="B57" s="55" t="s">
-        <v>171</v>
       </c>
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
@@ -7154,30 +7157,30 @@
       <c r="A58" s="69"/>
       <c r="B58" s="55"/>
       <c r="C58" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="55" t="s">
         <v>172</v>
-      </c>
-      <c r="D58" s="55" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="55" x14ac:dyDescent="0.15">
       <c r="A59" s="69"/>
       <c r="B59" s="55"/>
       <c r="C59" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" s="55" t="s">
         <v>174</v>
-      </c>
-      <c r="D59" s="55" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="69"/>
       <c r="B60" s="55"/>
       <c r="C60" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="55" t="s">
         <v>176</v>
-      </c>
-      <c r="D60" s="55" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7188,7 +7191,7 @@
     </row>
     <row r="62" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="137" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B62" s="138"/>
       <c r="C62" s="138"/>
@@ -7196,33 +7199,33 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="B63" s="68" t="s">
         <v>179</v>
-      </c>
-      <c r="B63" s="68" t="s">
-        <v>180</v>
       </c>
       <c r="C63" s="68"/>
       <c r="D63" s="68"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="55" t="s">
         <v>181</v>
-      </c>
-      <c r="B64" s="55" t="s">
-        <v>182</v>
       </c>
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
     </row>
     <row r="65" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A65" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="B65" s="55" t="s">
+      <c r="C65" s="55" t="s">
         <v>184</v>
-      </c>
-      <c r="C65" s="55" t="s">
-        <v>185</v>
       </c>
       <c r="D65" s="55"/>
     </row>

</xml_diff>

<commit_message>
modif courd 2-1 et TP8
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="359">
   <si>
     <t>Cours</t>
   </si>
@@ -1125,6 +1125,12 @@
   </si>
   <si>
     <t>algo/ALG-017;algo/ALG-018;python_bases/PYB-517</t>
+  </si>
+  <si>
+    <t>consignes/consignes_TP8;tableaux/TAB-027</t>
+  </si>
+  <si>
+    <t>Tableaux, fichiers et traitement d'images</t>
   </si>
 </sst>
 </file>
@@ -3597,7 +3603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -3839,8 +3845,8 @@
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4732,17 +4738,19 @@
         <v>8</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>50</v>
+        <v>358</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>357</v>
+      </c>
       <c r="M18" s="84" t="s">
         <v>270</v>
       </c>
-      <c r="N18" s="84" t="s">
-        <v>270</v>
+      <c r="N18" s="78" t="s">
+        <v>273</v>
       </c>
       <c r="O18" s="27"/>
       <c r="P18" s="43"/>
@@ -4783,15 +4791,15 @@
         <v>8</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>50</v>
+        <v>358</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="84" t="s">
         <v>270</v>
       </c>
-      <c r="N19" s="84" t="s">
-        <v>270</v>
+      <c r="N19" s="78" t="s">
+        <v>273</v>
       </c>
       <c r="O19" s="27"/>
       <c r="P19" s="43"/>

</xml_diff>

<commit_message>
génération enttete pour TP14
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Informatique_MPSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliendurif/Documents/prepa/MPSI/ipt_mpsi_lamartin/Informatique_MPSI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F976284E-030B-48D0-AB87-E3D531E5DEFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning DS" sheetId="16" r:id="rId1"/>
@@ -28,14 +27,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1183,8 +1182,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2554,18 +2553,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2615,42 +2650,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3329,13 +3328,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="651" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="653" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="Normal 4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="Normal 4 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 4 2" xfId="5"/>
+    <cellStyle name="Normal 4 3" xfId="6"/>
+    <cellStyle name="Normal 5" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3647,22 +3646,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" thickBot="1">
+    <row r="1" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -3678,7 +3677,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="62">
+    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A2" s="96">
         <v>1</v>
       </c>
@@ -3692,7 +3691,7 @@
       <c r="E2" s="86"/>
       <c r="F2" s="86"/>
     </row>
-    <row r="3" spans="1:8" ht="87.5">
+    <row r="3" spans="1:8" ht="78" x14ac:dyDescent="0.15">
       <c r="A3" s="97"/>
       <c r="B3" s="3" t="s">
         <v>332</v>
@@ -3704,7 +3703,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="97"/>
       <c r="B4" s="3" t="s">
         <v>336</v>
@@ -3716,7 +3715,7 @@
       <c r="E4" s="42"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="97"/>
       <c r="B5" s="3" t="s">
         <v>333</v>
@@ -3728,7 +3727,7 @@
       <c r="E5" s="42"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="50" customHeight="1" thickBot="1">
+    <row r="6" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="98"/>
       <c r="B6" s="87" t="s">
         <v>334</v>
@@ -3740,7 +3739,7 @@
       <c r="E6" s="88"/>
       <c r="F6" s="88"/>
     </row>
-    <row r="7" spans="1:8" ht="62">
+    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A7" s="96">
         <v>2</v>
       </c>
@@ -3754,7 +3753,7 @@
       <c r="E7" s="86"/>
       <c r="F7" s="86"/>
     </row>
-    <row r="8" spans="1:8" ht="37.5">
+    <row r="8" spans="1:8" ht="39" x14ac:dyDescent="0.15">
       <c r="A8" s="97"/>
       <c r="B8" s="90" t="s">
         <v>332</v>
@@ -3766,7 +3765,7 @@
       <c r="E8" s="90"/>
       <c r="F8" s="90"/>
     </row>
-    <row r="9" spans="1:8" ht="25">
+    <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="97"/>
       <c r="B9" s="90" t="s">
         <v>336</v>
@@ -3781,7 +3780,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="97"/>
       <c r="B10" s="90" t="s">
         <v>333</v>
@@ -3793,7 +3792,7 @@
       <c r="E10" s="42"/>
       <c r="F10" s="90"/>
     </row>
-    <row r="11" spans="1:8" ht="50" customHeight="1" thickBot="1">
+    <row r="11" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="98"/>
       <c r="B11" s="91" t="s">
         <v>334</v>
@@ -3805,7 +3804,7 @@
       <c r="E11" s="88"/>
       <c r="F11" s="88"/>
     </row>
-    <row r="12" spans="1:8" ht="62">
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A12" s="96">
         <v>3</v>
       </c>
@@ -3819,7 +3818,7 @@
       <c r="E12" s="86"/>
       <c r="F12" s="86"/>
     </row>
-    <row r="13" spans="1:8" ht="25">
+    <row r="13" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="97"/>
       <c r="B13" s="93" t="s">
         <v>332</v>
@@ -3831,7 +3830,7 @@
       <c r="E13" s="93"/>
       <c r="F13" s="93"/>
     </row>
-    <row r="14" spans="1:8" ht="25">
+    <row r="14" spans="1:8" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="97"/>
       <c r="B14" s="93" t="s">
         <v>336</v>
@@ -3846,7 +3845,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="97"/>
       <c r="B15" s="93" t="s">
         <v>333</v>
@@ -3858,7 +3857,7 @@
       <c r="E15" s="42"/>
       <c r="F15" s="93"/>
     </row>
-    <row r="16" spans="1:8" ht="50" customHeight="1" thickBot="1">
+    <row r="16" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="98"/>
       <c r="B16" s="94" t="s">
         <v>334</v>
@@ -3870,7 +3869,7 @@
       <c r="E16" s="88"/>
       <c r="F16" s="88"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>276</v>
       </c>
@@ -3886,39 +3885,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="26" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="10.81640625" style="1"/>
-    <col min="4" max="4" width="20.36328125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.36328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.36328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="42.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="32.6328125" style="1" customWidth="1"/>
-    <col min="15" max="18" width="10.81640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="41.36328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.81640625" style="1"/>
-    <col min="22" max="22" width="10.81640625" style="1" customWidth="1"/>
-    <col min="23" max="24" width="58.453125" style="74" customWidth="1"/>
-    <col min="25" max="16384" width="10.81640625" style="1"/>
+    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="32.6640625" style="1" customWidth="1"/>
+    <col min="15" max="18" width="10.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="10.83203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="58.5" style="74" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="26" customHeight="1">
+    <row r="1" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -3977,17 +3976,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="32" customHeight="1">
+    <row r="2" spans="1:24" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="9">
         <v>43711</v>
       </c>
-      <c r="C2" s="126">
+      <c r="C2" s="107">
         <v>1</v>
       </c>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="110" t="s">
         <v>261</v>
       </c>
       <c r="E2" s="26">
@@ -4033,7 +4032,7 @@
       <c r="W2" s="75"/>
       <c r="X2" s="75"/>
     </row>
-    <row r="3" spans="1:24" ht="32" customHeight="1">
+    <row r="3" spans="1:24" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4041,8 +4040,8 @@
         <f>B2+7</f>
         <v>43718</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="130"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="111"/>
       <c r="E3" s="26">
         <v>2</v>
       </c>
@@ -4085,7 +4084,7 @@
       <c r="W3" s="75"/>
       <c r="X3" s="75"/>
     </row>
-    <row r="4" spans="1:24" ht="56" customHeight="1">
+    <row r="4" spans="1:24" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4093,8 +4092,8 @@
         <f>B3+7</f>
         <v>43725</v>
       </c>
-      <c r="C4" s="127"/>
-      <c r="D4" s="130"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="111"/>
       <c r="E4" s="26">
         <v>2</v>
       </c>
@@ -4138,7 +4137,7 @@
       <c r="W4" s="75"/>
       <c r="X4" s="75"/>
     </row>
-    <row r="5" spans="1:24" ht="32" customHeight="1">
+    <row r="5" spans="1:24" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4146,8 +4145,8 @@
         <f t="shared" ref="B5:B8" si="0">B4+7</f>
         <v>43732</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="130"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="111"/>
       <c r="E5" s="26">
         <v>3</v>
       </c>
@@ -4191,7 +4190,7 @@
       <c r="W5" s="75"/>
       <c r="X5" s="75"/>
     </row>
-    <row r="6" spans="1:24" ht="26" customHeight="1">
+    <row r="6" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4199,8 +4198,8 @@
         <f>B5+7</f>
         <v>43739</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="130"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="111"/>
       <c r="E6" s="26">
         <v>4</v>
       </c>
@@ -4246,7 +4245,7 @@
       <c r="W6" s="75"/>
       <c r="X6" s="75"/>
     </row>
-    <row r="7" spans="1:24" ht="26" customHeight="1">
+    <row r="7" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4254,8 +4253,8 @@
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
-      <c r="C7" s="127"/>
-      <c r="D7" s="130"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="111"/>
       <c r="E7" s="26">
         <v>4</v>
       </c>
@@ -4295,7 +4294,7 @@
       <c r="W7" s="75"/>
       <c r="X7" s="75"/>
     </row>
-    <row r="8" spans="1:24" ht="26" customHeight="1">
+    <row r="8" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4303,8 +4302,8 @@
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
-      <c r="C8" s="128"/>
-      <c r="D8" s="131"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="112"/>
       <c r="E8" s="26">
         <v>5</v>
       </c>
@@ -4350,25 +4349,25 @@
       <c r="W8" s="75"/>
       <c r="X8" s="75"/>
     </row>
-    <row r="9" spans="1:24" ht="26" customHeight="1">
-      <c r="A9" s="101" t="s">
+    <row r="9" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="102"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="106"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="106"/>
+      <c r="I9" s="106"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="106"/>
+      <c r="N9" s="106"/>
+      <c r="O9" s="106"/>
+      <c r="P9" s="106"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="41"/>
       <c r="S9" s="32"/>
@@ -4376,7 +4375,7 @@
       <c r="W9" s="75"/>
       <c r="X9" s="75"/>
     </row>
-    <row r="10" spans="1:24" ht="26" customHeight="1">
+    <row r="10" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4384,10 +4383,10 @@
         <f>B8+21</f>
         <v>43774</v>
       </c>
-      <c r="C10" s="126">
+      <c r="C10" s="107">
         <v>1</v>
       </c>
-      <c r="D10" s="129" t="s">
+      <c r="D10" s="110" t="s">
         <v>261</v>
       </c>
       <c r="E10" s="26">
@@ -4429,7 +4428,7 @@
       <c r="W10" s="75"/>
       <c r="X10" s="75"/>
     </row>
-    <row r="11" spans="1:24" ht="26" customHeight="1">
+    <row r="11" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4437,8 +4436,8 @@
         <f t="shared" ref="B11:B16" si="1">B10+7</f>
         <v>43781</v>
       </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="130"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="111"/>
       <c r="E11" s="26">
         <v>6</v>
       </c>
@@ -4480,7 +4479,7 @@
       <c r="W11" s="75"/>
       <c r="X11" s="75"/>
     </row>
-    <row r="12" spans="1:24" ht="26" customHeight="1">
+    <row r="12" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4488,8 +4487,8 @@
         <f t="shared" si="1"/>
         <v>43788</v>
       </c>
-      <c r="C12" s="127"/>
-      <c r="D12" s="130"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="111"/>
       <c r="E12" s="26">
         <v>6</v>
       </c>
@@ -4526,7 +4525,7 @@
       <c r="W12" s="75"/>
       <c r="X12" s="75"/>
     </row>
-    <row r="13" spans="1:24" ht="26" customHeight="1">
+    <row r="13" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4534,8 +4533,8 @@
         <f t="shared" si="1"/>
         <v>43795</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="130"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="26">
         <v>7</v>
       </c>
@@ -4579,7 +4578,7 @@
       <c r="W13" s="75"/>
       <c r="X13" s="75"/>
     </row>
-    <row r="14" spans="1:24" ht="26" customHeight="1">
+    <row r="14" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4587,8 +4586,8 @@
         <f t="shared" si="1"/>
         <v>43802</v>
       </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="130"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="111"/>
       <c r="E14" s="26">
         <v>7</v>
       </c>
@@ -4627,7 +4626,7 @@
       <c r="W14" s="75"/>
       <c r="X14" s="75"/>
     </row>
-    <row r="15" spans="1:24" ht="26" customHeight="1">
+    <row r="15" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4635,8 +4634,8 @@
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
-      <c r="C15" s="127"/>
-      <c r="D15" s="130"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="26">
         <v>8</v>
       </c>
@@ -4680,7 +4679,7 @@
       <c r="W15" s="75"/>
       <c r="X15" s="75"/>
     </row>
-    <row r="16" spans="1:24" ht="26" customHeight="1">
+    <row r="16" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4688,8 +4687,8 @@
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
-      <c r="C16" s="128"/>
-      <c r="D16" s="131"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="112"/>
       <c r="E16" s="26">
         <v>8</v>
       </c>
@@ -4729,25 +4728,25 @@
       <c r="W16" s="75"/>
       <c r="X16" s="75"/>
     </row>
-    <row r="17" spans="1:24" ht="26" customHeight="1">
-      <c r="A17" s="101" t="s">
+    <row r="17" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="102"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="102"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="102"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="106"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="106"/>
+      <c r="P17" s="106"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="41"/>
       <c r="S17" s="32"/>
@@ -4755,7 +4754,7 @@
       <c r="W17" s="75"/>
       <c r="X17" s="75"/>
     </row>
-    <row r="18" spans="1:24" ht="26" customHeight="1">
+    <row r="18" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -4763,10 +4762,10 @@
         <f>B16+21</f>
         <v>43837</v>
       </c>
-      <c r="C18" s="120">
+      <c r="C18" s="99">
         <v>2</v>
       </c>
-      <c r="D18" s="123" t="s">
+      <c r="D18" s="102" t="s">
         <v>184</v>
       </c>
       <c r="E18" s="28">
@@ -4812,7 +4811,7 @@
       <c r="W18" s="75"/>
       <c r="X18" s="75"/>
     </row>
-    <row r="19" spans="1:24" ht="26" customHeight="1">
+    <row r="19" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -4820,8 +4819,8 @@
         <f>B18+7</f>
         <v>43844</v>
       </c>
-      <c r="C19" s="121"/>
-      <c r="D19" s="124"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="103"/>
       <c r="E19" s="28">
         <v>1</v>
       </c>
@@ -4861,7 +4860,7 @@
       <c r="W19" s="75"/>
       <c r="X19" s="75"/>
     </row>
-    <row r="20" spans="1:24" ht="26" customHeight="1">
+    <row r="20" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -4869,8 +4868,8 @@
         <f t="shared" ref="B20:B40" si="2">B19+7</f>
         <v>43851</v>
       </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="124"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="103"/>
       <c r="E20" s="28">
         <v>2</v>
       </c>
@@ -4914,7 +4913,7 @@
       <c r="W20" s="75"/>
       <c r="X20" s="75"/>
     </row>
-    <row r="21" spans="1:24" ht="26" customHeight="1">
+    <row r="21" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -4922,8 +4921,8 @@
         <f>B20+7</f>
         <v>43858</v>
       </c>
-      <c r="C21" s="122"/>
-      <c r="D21" s="125"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="104"/>
       <c r="E21" s="28">
         <v>2</v>
       </c>
@@ -4963,7 +4962,7 @@
       <c r="W21" s="75"/>
       <c r="X21" s="75"/>
     </row>
-    <row r="22" spans="1:24" ht="26" customHeight="1">
+    <row r="22" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -4971,10 +4970,10 @@
         <f>B21+7</f>
         <v>43865</v>
       </c>
-      <c r="C22" s="106">
+      <c r="C22" s="118">
         <v>3</v>
       </c>
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="115" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="35">
@@ -5020,7 +5019,7 @@
       <c r="W22" s="75"/>
       <c r="X22" s="75"/>
     </row>
-    <row r="23" spans="1:24" ht="26" customHeight="1">
+    <row r="23" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -5028,8 +5027,8 @@
         <f>B22+7</f>
         <v>43872</v>
       </c>
-      <c r="C23" s="107"/>
-      <c r="D23" s="104"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="116"/>
       <c r="E23" s="35">
         <v>2</v>
       </c>
@@ -5070,7 +5069,7 @@
       </c>
       <c r="S23" s="33"/>
     </row>
-    <row r="24" spans="1:24" ht="26" customHeight="1">
+    <row r="24" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -5078,8 +5077,8 @@
         <f>B23+7</f>
         <v>43879</v>
       </c>
-      <c r="C24" s="108"/>
-      <c r="D24" s="105"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="117"/>
       <c r="E24" s="34">
         <v>2</v>
       </c>
@@ -5116,25 +5115,25 @@
       </c>
       <c r="S24" s="33"/>
     </row>
-    <row r="25" spans="1:24" ht="26" customHeight="1">
-      <c r="A25" s="101" t="s">
+    <row r="25" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="102"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="102"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
-      <c r="K25" s="102"/>
-      <c r="L25" s="102"/>
-      <c r="M25" s="102"/>
-      <c r="N25" s="102"/>
-      <c r="O25" s="102"/>
-      <c r="P25" s="102"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="106"/>
+      <c r="K25" s="106"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="106"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="50"/>
       <c r="S25" s="32"/>
@@ -5142,7 +5141,7 @@
       <c r="W25" s="75"/>
       <c r="X25" s="75"/>
     </row>
-    <row r="26" spans="1:24" ht="26" customHeight="1">
+    <row r="26" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -5150,10 +5149,10 @@
         <f>B24+21</f>
         <v>43900</v>
       </c>
-      <c r="C26" s="106">
+      <c r="C26" s="118">
         <v>3</v>
       </c>
-      <c r="D26" s="103" t="s">
+      <c r="D26" s="115" t="s">
         <v>60</v>
       </c>
       <c r="E26" s="29">
@@ -5197,7 +5196,7 @@
       <c r="W26" s="75"/>
       <c r="X26" s="75"/>
     </row>
-    <row r="27" spans="1:24" ht="26" customHeight="1">
+    <row r="27" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -5205,8 +5204,8 @@
         <f t="shared" si="2"/>
         <v>43907</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="104"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="116"/>
       <c r="E27" s="35">
         <v>3</v>
       </c>
@@ -5245,7 +5244,7 @@
       <c r="W27" s="75"/>
       <c r="X27" s="75"/>
     </row>
-    <row r="28" spans="1:24" ht="26" customHeight="1">
+    <row r="28" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>21</v>
       </c>
@@ -5253,8 +5252,8 @@
         <f t="shared" si="2"/>
         <v>43914</v>
       </c>
-      <c r="C28" s="107"/>
-      <c r="D28" s="104"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="116"/>
       <c r="E28" s="29">
         <v>4</v>
       </c>
@@ -5296,7 +5295,7 @@
       <c r="W28" s="75"/>
       <c r="X28" s="75"/>
     </row>
-    <row r="29" spans="1:24" ht="26" customHeight="1">
+    <row r="29" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>22</v>
       </c>
@@ -5304,8 +5303,8 @@
         <f t="shared" si="2"/>
         <v>43921</v>
       </c>
-      <c r="C29" s="108"/>
-      <c r="D29" s="105"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="117"/>
       <c r="E29" s="35">
         <v>4</v>
       </c>
@@ -5345,7 +5344,7 @@
       <c r="W29" s="75"/>
       <c r="X29" s="75"/>
     </row>
-    <row r="30" spans="1:24" ht="26" customHeight="1">
+    <row r="30" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>23</v>
       </c>
@@ -5353,10 +5352,10 @@
         <f t="shared" si="2"/>
         <v>43928</v>
       </c>
-      <c r="C30" s="109">
+      <c r="C30" s="121">
         <v>4</v>
       </c>
-      <c r="D30" s="111" t="s">
+      <c r="D30" s="123" t="s">
         <v>43</v>
       </c>
       <c r="E30" s="30">
@@ -5400,7 +5399,7 @@
       <c r="W30" s="75"/>
       <c r="X30" s="75"/>
     </row>
-    <row r="31" spans="1:24" ht="26" customHeight="1">
+    <row r="31" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>24</v>
       </c>
@@ -5408,8 +5407,8 @@
         <f t="shared" si="2"/>
         <v>43935</v>
       </c>
-      <c r="C31" s="110"/>
-      <c r="D31" s="112"/>
+      <c r="C31" s="122"/>
+      <c r="D31" s="124"/>
       <c r="E31" s="30">
         <v>2</v>
       </c>
@@ -5450,25 +5449,25 @@
       <c r="W31" s="75"/>
       <c r="X31" s="75"/>
     </row>
-    <row r="32" spans="1:24" ht="26" customHeight="1">
-      <c r="A32" s="99" t="s">
+    <row r="32" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="100"/>
-      <c r="I32" s="100"/>
-      <c r="J32" s="100"/>
-      <c r="K32" s="100"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="100"/>
-      <c r="N32" s="100"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="100"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="114"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="114"/>
+      <c r="J32" s="114"/>
+      <c r="K32" s="114"/>
+      <c r="L32" s="114"/>
+      <c r="M32" s="114"/>
+      <c r="N32" s="114"/>
+      <c r="O32" s="114"/>
+      <c r="P32" s="114"/>
       <c r="Q32" s="47"/>
       <c r="R32" s="51"/>
       <c r="S32" s="32"/>
@@ -5476,7 +5475,7 @@
       <c r="W32" s="75"/>
       <c r="X32" s="75"/>
     </row>
-    <row r="33" spans="1:24" ht="26" customHeight="1">
+    <row r="33" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>25</v>
       </c>
@@ -5484,10 +5483,10 @@
         <f>B31+21</f>
         <v>43956</v>
       </c>
-      <c r="C33" s="109">
+      <c r="C33" s="121">
         <v>4</v>
       </c>
-      <c r="D33" s="111" t="s">
+      <c r="D33" s="123" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="30">
@@ -5526,7 +5525,7 @@
       </c>
       <c r="S33" s="33"/>
     </row>
-    <row r="34" spans="1:24" ht="26" customHeight="1">
+    <row r="34" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -5534,8 +5533,8 @@
         <f t="shared" si="2"/>
         <v>43963</v>
       </c>
-      <c r="C34" s="114"/>
-      <c r="D34" s="113"/>
+      <c r="C34" s="126"/>
+      <c r="D34" s="125"/>
       <c r="E34" s="30">
         <v>3</v>
       </c>
@@ -5572,7 +5571,7 @@
       </c>
       <c r="S34" s="32"/>
     </row>
-    <row r="35" spans="1:24" ht="26" customHeight="1">
+    <row r="35" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -5580,8 +5579,8 @@
         <f t="shared" si="2"/>
         <v>43970</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="112"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="124"/>
       <c r="E35" s="30">
         <v>4</v>
       </c>
@@ -5617,7 +5616,7 @@
       </c>
       <c r="S35" s="46"/>
     </row>
-    <row r="36" spans="1:24" ht="26" customHeight="1">
+    <row r="36" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -5625,10 +5624,10 @@
         <f t="shared" si="2"/>
         <v>43977</v>
       </c>
-      <c r="C36" s="117">
+      <c r="C36" s="129">
         <v>5</v>
       </c>
-      <c r="D36" s="115" t="s">
+      <c r="D36" s="127" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="31">
@@ -5660,7 +5659,7 @@
       <c r="W36" s="75"/>
       <c r="X36" s="75"/>
     </row>
-    <row r="37" spans="1:24" ht="26" customHeight="1">
+    <row r="37" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -5668,8 +5667,8 @@
         <f t="shared" si="2"/>
         <v>43984</v>
       </c>
-      <c r="C37" s="118"/>
-      <c r="D37" s="116"/>
+      <c r="C37" s="130"/>
+      <c r="D37" s="128"/>
       <c r="E37" s="31">
         <v>1</v>
       </c>
@@ -5701,7 +5700,7 @@
       <c r="W37" s="75"/>
       <c r="X37" s="75"/>
     </row>
-    <row r="38" spans="1:24" ht="26" customHeight="1">
+    <row r="38" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>30</v>
       </c>
@@ -5709,8 +5708,8 @@
         <f t="shared" si="2"/>
         <v>43991</v>
       </c>
-      <c r="C38" s="118"/>
-      <c r="D38" s="116"/>
+      <c r="C38" s="130"/>
+      <c r="D38" s="128"/>
       <c r="E38" s="31">
         <v>1</v>
       </c>
@@ -5740,7 +5739,7 @@
       <c r="W38" s="75"/>
       <c r="X38" s="75"/>
     </row>
-    <row r="39" spans="1:24" ht="26" customHeight="1">
+    <row r="39" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>31</v>
       </c>
@@ -5748,8 +5747,8 @@
         <f t="shared" si="2"/>
         <v>43998</v>
       </c>
-      <c r="C39" s="118"/>
-      <c r="D39" s="116"/>
+      <c r="C39" s="130"/>
+      <c r="D39" s="128"/>
       <c r="E39" s="31">
         <v>1</v>
       </c>
@@ -5779,7 +5778,7 @@
       <c r="W39" s="75"/>
       <c r="X39" s="75"/>
     </row>
-    <row r="40" spans="1:24" ht="26" customHeight="1">
+    <row r="40" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>32</v>
       </c>
@@ -5787,8 +5786,8 @@
         <f t="shared" si="2"/>
         <v>44005</v>
       </c>
-      <c r="C40" s="119"/>
-      <c r="D40" s="116"/>
+      <c r="C40" s="131"/>
+      <c r="D40" s="128"/>
       <c r="E40" s="31">
         <v>1</v>
       </c>
@@ -5816,101 +5815,93 @@
       <c r="W40" s="75"/>
       <c r="X40" s="75"/>
     </row>
-    <row r="41" spans="1:24" ht="26" customHeight="1">
-      <c r="A41" s="99" t="s">
+    <row r="41" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="100"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="100"/>
-      <c r="H41" s="100"/>
-      <c r="I41" s="100"/>
-      <c r="J41" s="100"/>
-      <c r="K41" s="100"/>
-      <c r="L41" s="100"/>
-      <c r="M41" s="100"/>
-      <c r="N41" s="100"/>
-      <c r="O41" s="100"/>
-      <c r="P41" s="100"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="114"/>
+      <c r="F41" s="114"/>
+      <c r="G41" s="114"/>
+      <c r="H41" s="114"/>
+      <c r="I41" s="114"/>
+      <c r="J41" s="114"/>
+      <c r="K41" s="114"/>
+      <c r="L41" s="114"/>
+      <c r="M41" s="114"/>
+      <c r="N41" s="114"/>
+      <c r="O41" s="114"/>
+      <c r="P41" s="114"/>
       <c r="Q41" s="47"/>
       <c r="R41" s="51"/>
       <c r="V41" s="70"/>
       <c r="W41" s="75"/>
       <c r="X41" s="75"/>
     </row>
-    <row r="42" spans="1:24" ht="26" customHeight="1">
+    <row r="42" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V42" s="70"/>
       <c r="W42" s="75"/>
       <c r="X42" s="75"/>
     </row>
-    <row r="43" spans="1:24" ht="26" customHeight="1">
+    <row r="43" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V43" s="70"/>
       <c r="W43" s="75"/>
       <c r="X43" s="75"/>
     </row>
-    <row r="44" spans="1:24" ht="26" customHeight="1">
+    <row r="44" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V44" s="70"/>
       <c r="W44" s="75"/>
       <c r="X44" s="75"/>
     </row>
-    <row r="45" spans="1:24" ht="26" customHeight="1">
+    <row r="45" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V45" s="70"/>
       <c r="W45" s="75"/>
       <c r="X45" s="75"/>
     </row>
-    <row r="46" spans="1:24" ht="26" customHeight="1">
+    <row r="46" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V46" s="70"/>
       <c r="W46" s="75"/>
       <c r="X46" s="75"/>
     </row>
-    <row r="47" spans="1:24" ht="26" customHeight="1">
+    <row r="47" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V47" s="70"/>
       <c r="W47" s="75"/>
       <c r="X47" s="75"/>
     </row>
-    <row r="48" spans="1:24" ht="26" customHeight="1">
+    <row r="48" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V48" s="70"/>
       <c r="W48" s="75"/>
       <c r="X48" s="75"/>
     </row>
-    <row r="49" spans="22:24" ht="26" customHeight="1">
+    <row r="49" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V49" s="70"/>
       <c r="W49" s="75"/>
       <c r="X49" s="75"/>
     </row>
-    <row r="50" spans="22:24" ht="26" customHeight="1">
+    <row r="50" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V50" s="70"/>
       <c r="W50" s="75"/>
       <c r="X50" s="75"/>
     </row>
-    <row r="51" spans="22:24" ht="26" customHeight="1">
+    <row r="51" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V51" s="70"/>
       <c r="W51" s="75"/>
       <c r="X51" s="75"/>
     </row>
-    <row r="52" spans="22:24" ht="26" customHeight="1">
+    <row r="52" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V52" s="70"/>
       <c r="W52" s="75"/>
       <c r="X52" s="75"/>
     </row>
-    <row r="53" spans="22:24" ht="26" customHeight="1">
+    <row r="53" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="V53" s="70"/>
       <c r="W53" s="75"/>
       <c r="X53" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="A9:P9"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D10:D16"/>
-    <mergeCell ref="C10:C16"/>
     <mergeCell ref="A41:P41"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A25:P25"/>
@@ -5924,6 +5915,14 @@
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="D36:D40"/>
     <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A9:P9"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D10:D16"/>
+    <mergeCell ref="C10:C16"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5932,22 +5931,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="70.453125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.81640625" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="70.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" customHeight="1"/>
-    <row r="2" spans="1:2" ht="31">
+    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -5955,7 +5954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1">
+    <row r="3" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -5963,7 +5962,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1">
+    <row r="4" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
         <v>54</v>
       </c>
@@ -5971,7 +5970,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1">
+    <row r="5" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
@@ -5979,7 +5978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="38" customHeight="1">
+    <row r="6" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="24" t="s">
         <v>6</v>
       </c>
@@ -5987,7 +5986,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38" customHeight="1">
+    <row r="7" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
@@ -6003,22 +6002,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="70"/>
-    <col min="2" max="2" width="108.453125" style="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.453125" style="71" customWidth="1"/>
-    <col min="4" max="16384" width="10.81640625" style="70"/>
+    <col min="1" max="1" width="10.83203125" style="70"/>
+    <col min="2" max="2" width="108.5" style="71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.5" style="71" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="70" t="s">
         <v>241</v>
       </c>
@@ -6029,7 +6028,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
         <v>323</v>
       </c>
@@ -6040,7 +6039,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="70" t="s">
         <v>320</v>
       </c>
@@ -6051,7 +6050,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="70" t="s">
         <v>205</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
         <v>206</v>
       </c>
@@ -6073,7 +6072,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="70" t="s">
         <v>187</v>
       </c>
@@ -6084,7 +6083,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="70" t="s">
         <v>188</v>
       </c>
@@ -6095,7 +6094,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="70" t="s">
         <v>207</v>
       </c>
@@ -6106,7 +6105,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="70" t="s">
         <v>208</v>
       </c>
@@ -6117,17 +6116,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="70" t="s">
         <v>189</v>
       </c>
@@ -6138,7 +6137,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="70" t="s">
         <v>190</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
         <v>191</v>
       </c>
@@ -6160,7 +6159,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="70" t="s">
         <v>199</v>
       </c>
@@ -6171,7 +6170,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
         <v>201</v>
       </c>
@@ -6182,7 +6181,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
         <v>192</v>
       </c>
@@ -6193,7 +6192,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
         <v>193</v>
       </c>
@@ -6204,7 +6203,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
         <v>194</v>
       </c>
@@ -6215,7 +6214,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
         <v>195</v>
       </c>
@@ -6226,7 +6225,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24">
+    <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
         <v>196</v>
       </c>
@@ -6237,7 +6236,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="70" t="s">
         <v>197</v>
       </c>
@@ -6248,7 +6247,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="70" t="s">
         <v>198</v>
       </c>
@@ -6259,17 +6258,17 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="79" t="s">
         <v>200</v>
       </c>
@@ -6280,7 +6279,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="79" t="s">
         <v>202</v>
       </c>
@@ -6291,7 +6290,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="79" t="s">
         <v>203</v>
       </c>
@@ -6302,7 +6301,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="79" t="s">
         <v>204</v>
       </c>
@@ -6313,7 +6312,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="79" t="s">
         <v>237</v>
       </c>
@@ -6324,7 +6323,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="79" t="s">
         <v>238</v>
       </c>
@@ -6335,7 +6334,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="70" t="s">
         <v>209</v>
       </c>
@@ -6346,7 +6345,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="70" t="s">
         <v>210</v>
       </c>
@@ -6357,7 +6356,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
         <v>211</v>
       </c>
@@ -6368,7 +6367,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="70" t="s">
         <v>212</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="70" t="s">
         <v>213</v>
       </c>
@@ -6390,7 +6389,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24">
+    <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A38" s="70" t="s">
         <v>239</v>
       </c>
@@ -6401,7 +6400,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="70" t="s">
         <v>240</v>
       </c>
@@ -6412,17 +6411,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24">
+    <row r="42" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A42" s="70" t="s">
         <v>214</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="36">
+    <row r="43" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A43" s="70" t="s">
         <v>215</v>
       </c>
@@ -6444,7 +6443,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24">
+    <row r="44" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A44" s="70" t="s">
         <v>216</v>
       </c>
@@ -6455,7 +6454,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="70" t="s">
         <v>217</v>
       </c>
@@ -6466,7 +6465,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="70" t="s">
         <v>218</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="70" t="s">
         <v>219</v>
       </c>
@@ -6488,7 +6487,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24">
+    <row r="48" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A48" s="70" t="s">
         <v>220</v>
       </c>
@@ -6499,7 +6498,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="70" t="s">
         <v>221</v>
       </c>
@@ -6510,7 +6509,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="24">
+    <row r="50" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A50" s="70" t="s">
         <v>222</v>
       </c>
@@ -6521,17 +6520,17 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="70" t="s">
         <v>223</v>
       </c>
@@ -6542,7 +6541,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="70" t="s">
         <v>224</v>
       </c>
@@ -6553,7 +6552,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="70" t="s">
         <v>225</v>
       </c>
@@ -6564,7 +6563,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="70" t="s">
         <v>226</v>
       </c>
@@ -6575,7 +6574,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="70" t="s">
         <v>227</v>
       </c>
@@ -6586,7 +6585,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="70" t="s">
         <v>228</v>
       </c>
@@ -6597,7 +6596,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="70" t="s">
         <v>231</v>
       </c>
@@ -6608,7 +6607,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="24">
+    <row r="60" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A60" s="70" t="s">
         <v>232</v>
       </c>
@@ -6619,7 +6618,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="70" t="s">
         <v>233</v>
       </c>
@@ -6630,12 +6629,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="70" t="s">
         <v>234</v>
       </c>
@@ -6646,7 +6645,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="70" t="s">
         <v>235</v>
       </c>
@@ -6657,7 +6656,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="70" t="s">
         <v>236</v>
       </c>
@@ -6668,7 +6667,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="36">
+    <row r="66" spans="1:3" ht="36" x14ac:dyDescent="0.15">
       <c r="A66" s="70" t="s">
         <v>277</v>
       </c>
@@ -6679,7 +6678,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="70" t="s">
         <v>316</v>
       </c>
@@ -6690,7 +6689,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="70" t="s">
         <v>276</v>
       </c>
@@ -6703,20 +6702,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="47.36328125" customWidth="1"/>
+    <col min="2" max="4" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="132" t="s">
         <v>77</v>
       </c>
@@ -6724,7 +6723,7 @@
       <c r="C1" s="133"/>
       <c r="D1" s="134"/>
     </row>
-    <row r="2" spans="1:4" ht="21">
+    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
         <v>78</v>
       </c>
@@ -6734,7 +6733,7 @@
       <c r="C2" s="55"/>
       <c r="D2" s="56"/>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A3" s="54"/>
       <c r="B3" s="55"/>
       <c r="C3" s="55" t="s">
@@ -6742,7 +6741,7 @@
       </c>
       <c r="D3" s="56"/>
     </row>
-    <row r="4" spans="1:4" ht="31.5">
+    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="55" t="s">
@@ -6750,7 +6749,7 @@
       </c>
       <c r="D4" s="56"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55" t="s">
@@ -6758,13 +6757,13 @@
       </c>
       <c r="D5" s="56"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="54"/>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:4" ht="21">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="54" t="s">
         <v>83</v>
       </c>
@@ -6774,7 +6773,7 @@
       <c r="C7" s="55"/>
       <c r="D7" s="56"/>
     </row>
-    <row r="8" spans="1:4" ht="21">
+    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A8" s="54" t="s">
         <v>85</v>
       </c>
@@ -6786,7 +6785,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42">
+    <row r="9" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A9" s="54"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -6796,7 +6795,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="53" thickBot="1">
+    <row r="10" spans="1:4" ht="56" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="58" t="s">
@@ -6806,13 +6805,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13" thickBot="1">
+    <row r="11" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
       <c r="D11" s="61"/>
     </row>
-    <row r="12" spans="1:4" ht="14.5">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="132" t="s">
         <v>92</v>
       </c>
@@ -6820,7 +6819,7 @@
       <c r="C12" s="133"/>
       <c r="D12" s="134"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="54" t="s">
         <v>93</v>
       </c>
@@ -6830,7 +6829,7 @@
       <c r="C13" s="55"/>
       <c r="D13" s="56"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="54" t="s">
         <v>95</v>
       </c>
@@ -6840,7 +6839,7 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="54" t="s">
         <v>97</v>
       </c>
@@ -6850,7 +6849,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="56"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="54" t="s">
         <v>99</v>
       </c>
@@ -6860,7 +6859,7 @@
       <c r="C16" s="55"/>
       <c r="D16" s="56"/>
     </row>
-    <row r="17" spans="1:4" ht="21">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="54" t="s">
         <v>101</v>
       </c>
@@ -6870,7 +6869,7 @@
       <c r="C17" s="55"/>
       <c r="D17" s="56"/>
     </row>
-    <row r="18" spans="1:4" ht="21">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="54" t="s">
         <v>103</v>
       </c>
@@ -6880,7 +6879,7 @@
       <c r="C18" s="55"/>
       <c r="D18" s="56"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="54" t="s">
         <v>105</v>
       </c>
@@ -6890,7 +6889,7 @@
       <c r="C19" s="55"/>
       <c r="D19" s="56"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="54" t="s">
         <v>107</v>
       </c>
@@ -6900,7 +6899,7 @@
       <c r="C20" s="55"/>
       <c r="D20" s="56"/>
     </row>
-    <row r="21" spans="1:4" ht="21">
+    <row r="21" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A21" s="54"/>
       <c r="B21" s="55"/>
       <c r="C21" s="55" t="s">
@@ -6908,7 +6907,7 @@
       </c>
       <c r="D21" s="56"/>
     </row>
-    <row r="22" spans="1:4" ht="21">
+    <row r="22" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A22" s="54"/>
       <c r="B22" s="55"/>
       <c r="C22" s="55" t="s">
@@ -6916,7 +6915,7 @@
       </c>
       <c r="D22" s="56"/>
     </row>
-    <row r="23" spans="1:4" ht="21">
+    <row r="23" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A23" s="54"/>
       <c r="B23" s="55"/>
       <c r="C23" s="55" t="s">
@@ -6924,7 +6923,7 @@
       </c>
       <c r="D23" s="56"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="54"/>
       <c r="B24" s="55"/>
       <c r="C24" s="55" t="s">
@@ -6932,7 +6931,7 @@
       </c>
       <c r="D24" s="56"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="54"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55" t="s">
@@ -6940,13 +6939,13 @@
       </c>
       <c r="D25" s="56"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="54"/>
       <c r="B26" s="55"/>
       <c r="C26" s="55"/>
       <c r="D26" s="56"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="54" t="s">
         <v>114</v>
       </c>
@@ -6956,7 +6955,7 @@
       <c r="C27" s="55"/>
       <c r="D27" s="56"/>
     </row>
-    <row r="28" spans="1:4" ht="21">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="54" t="s">
         <v>116</v>
       </c>
@@ -6966,7 +6965,7 @@
       <c r="C28" s="55"/>
       <c r="D28" s="56"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="54" t="s">
         <v>118</v>
       </c>
@@ -6976,7 +6975,7 @@
       <c r="C29" s="55"/>
       <c r="D29" s="56"/>
     </row>
-    <row r="30" spans="1:4" ht="21">
+    <row r="30" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A30" s="54" t="s">
         <v>120</v>
       </c>
@@ -6986,7 +6985,7 @@
       <c r="C30" s="55"/>
       <c r="D30" s="56"/>
     </row>
-    <row r="31" spans="1:4" ht="21">
+    <row r="31" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A31" s="54" t="s">
         <v>122</v>
       </c>
@@ -6996,7 +6995,7 @@
       <c r="C31" s="55"/>
       <c r="D31" s="56"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="54" t="s">
         <v>124</v>
       </c>
@@ -7006,7 +7005,7 @@
       <c r="C32" s="55"/>
       <c r="D32" s="56"/>
     </row>
-    <row r="33" spans="1:4" ht="21">
+    <row r="33" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A33" s="54"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55" t="s">
@@ -7016,7 +7015,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21">
+    <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A34" s="54"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55" t="s">
@@ -7026,7 +7025,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31.5">
+    <row r="35" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A35" s="54"/>
       <c r="B35" s="55"/>
       <c r="C35" s="55" t="s">
@@ -7036,7 +7035,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31.5">
+    <row r="36" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A36" s="54"/>
       <c r="B36" s="55"/>
       <c r="C36" s="55" t="s">
@@ -7046,7 +7045,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31.5">
+    <row r="37" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A37" s="54"/>
       <c r="B37" s="55"/>
       <c r="C37" s="55" t="s">
@@ -7056,7 +7055,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="52.5">
+    <row r="38" spans="1:4" ht="55" x14ac:dyDescent="0.15">
       <c r="A38" s="54"/>
       <c r="B38" s="55"/>
       <c r="C38" s="55" t="s">
@@ -7066,7 +7065,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" thickBot="1">
+    <row r="39" spans="1:4" ht="34" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="57"/>
       <c r="B39" s="58"/>
       <c r="C39" s="58" t="s">
@@ -7076,13 +7075,13 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="13" thickBot="1">
+    <row r="40" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="60"/>
       <c r="B40" s="61"/>
       <c r="C40" s="61"/>
       <c r="D40" s="61"/>
     </row>
-    <row r="41" spans="1:4" ht="14.5">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="135" t="s">
         <v>140</v>
       </c>
@@ -7090,7 +7089,7 @@
       <c r="C41" s="136"/>
       <c r="D41" s="137"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5">
+    <row r="42" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A42" s="54" t="s">
         <v>141</v>
       </c>
@@ -7100,7 +7099,7 @@
       <c r="C42" s="62"/>
       <c r="D42" s="63"/>
     </row>
-    <row r="43" spans="1:4" ht="42">
+    <row r="43" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A43" s="54" t="s">
         <v>143</v>
       </c>
@@ -7110,7 +7109,7 @@
       <c r="C43" s="62"/>
       <c r="D43" s="63"/>
     </row>
-    <row r="44" spans="1:4" ht="31.5">
+    <row r="44" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A44" s="54" t="s">
         <v>145</v>
       </c>
@@ -7120,7 +7119,7 @@
       <c r="C44" s="62"/>
       <c r="D44" s="63"/>
     </row>
-    <row r="45" spans="1:4" ht="21">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="54" t="s">
         <v>147</v>
       </c>
@@ -7130,7 +7129,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="63"/>
     </row>
-    <row r="46" spans="1:4" ht="21">
+    <row r="46" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A46" s="54" t="s">
         <v>149</v>
       </c>
@@ -7140,7 +7139,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="63"/>
     </row>
-    <row r="47" spans="1:4" ht="42">
+    <row r="47" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A47" s="54"/>
       <c r="B47" s="62"/>
       <c r="C47" s="62" t="s">
@@ -7150,7 +7149,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="31.5">
+    <row r="48" spans="1:4" ht="33" x14ac:dyDescent="0.15">
       <c r="A48" s="54"/>
       <c r="B48" s="62"/>
       <c r="C48" s="62" t="s">
@@ -7160,7 +7159,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="52.5">
+    <row r="49" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A49" s="54"/>
       <c r="B49" s="62"/>
       <c r="C49" s="62" t="s">
@@ -7170,7 +7169,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="74" thickBot="1">
+    <row r="50" spans="1:4" ht="67" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="57"/>
       <c r="B50" s="64"/>
       <c r="C50" s="64" t="s">
@@ -7180,13 +7179,13 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1">
+    <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="60"/>
       <c r="B51" s="66"/>
       <c r="C51" s="66"/>
       <c r="D51" s="66"/>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1">
+    <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="138" t="s">
         <v>159</v>
       </c>
@@ -7194,7 +7193,7 @@
       <c r="C52" s="139"/>
       <c r="D52" s="140"/>
     </row>
-    <row r="53" spans="1:4" ht="21">
+    <row r="53" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A53" s="67" t="s">
         <v>160</v>
       </c>
@@ -7204,7 +7203,7 @@
       <c r="C53" s="68"/>
       <c r="D53" s="68"/>
     </row>
-    <row r="54" spans="1:4" ht="21">
+    <row r="54" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A54" s="69" t="s">
         <v>162</v>
       </c>
@@ -7214,7 +7213,7 @@
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
     </row>
-    <row r="55" spans="1:4" ht="21">
+    <row r="55" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A55" s="69" t="s">
         <v>164</v>
       </c>
@@ -7224,7 +7223,7 @@
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
     </row>
-    <row r="56" spans="1:4" ht="21">
+    <row r="56" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A56" s="69" t="s">
         <v>166</v>
       </c>
@@ -7234,7 +7233,7 @@
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
     </row>
-    <row r="57" spans="1:4" ht="21">
+    <row r="57" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A57" s="69" t="s">
         <v>168</v>
       </c>
@@ -7244,7 +7243,7 @@
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
     </row>
-    <row r="58" spans="1:4" ht="21">
+    <row r="58" spans="1:4" ht="22" x14ac:dyDescent="0.15">
       <c r="A58" s="69"/>
       <c r="B58" s="55"/>
       <c r="C58" s="55" t="s">
@@ -7254,7 +7253,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="52.5">
+    <row r="59" spans="1:4" ht="55" x14ac:dyDescent="0.15">
       <c r="A59" s="69"/>
       <c r="B59" s="55"/>
       <c r="C59" s="55" t="s">
@@ -7264,7 +7263,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="21.5" thickBot="1">
+    <row r="60" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="69"/>
       <c r="B60" s="55"/>
       <c r="C60" s="55" t="s">
@@ -7274,13 +7273,13 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1">
+    <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="60"/>
       <c r="B61" s="66"/>
       <c r="C61" s="66"/>
       <c r="D61" s="66"/>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1">
+    <row r="62" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="138" t="s">
         <v>176</v>
       </c>
@@ -7288,7 +7287,7 @@
       <c r="C62" s="139"/>
       <c r="D62" s="140"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="67" t="s">
         <v>177</v>
       </c>
@@ -7298,7 +7297,7 @@
       <c r="C63" s="68"/>
       <c r="D63" s="68"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="69" t="s">
         <v>179</v>
       </c>
@@ -7308,7 +7307,7 @@
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
     </row>
-    <row r="65" spans="1:4" ht="42">
+    <row r="65" spans="1:4" ht="44" x14ac:dyDescent="0.15">
       <c r="A65" s="69" t="s">
         <v>181</v>
       </c>

</xml_diff>

<commit_message>
Exo pokemon en cours
</commit_message>
<xml_diff>
--- a/progression_2019_2020_IPT_MPSI.xlsx
+++ b/progression_2019_2020_IPT_MPSI.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliendurif/Documents/prepa/MPSI/ipt_mpsi_lamartin/Informatique_MPSI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Informatique_MPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577AF7DE-E7EF-4C4F-80D8-EF7C3489A93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1"/>
+    <workbookView xWindow="430" yWindow="310" windowWidth="10080" windowHeight="8370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning DS" sheetId="16" r:id="rId1"/>
@@ -27,21 +28,21 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="375">
   <si>
     <t>Cours</t>
   </si>
@@ -1177,13 +1178,16 @@
   </si>
   <si>
     <t>consignes/consignes_tp14;sql/SQL-005</t>
+  </si>
+  <si>
+    <t>BDD.C1; BDD.C2; BDD.C5; BDD.S3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2553,6 +2557,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2571,12 +2638,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2593,63 +2654,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3328,13 +3332,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="651" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="653" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="4"/>
-    <cellStyle name="Normal 4 2" xfId="5"/>
-    <cellStyle name="Normal 4 3" xfId="6"/>
-    <cellStyle name="Normal 5" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normal 4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normal 4 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3646,22 +3650,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <cols>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="13" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -3677,7 +3681,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="62">
       <c r="A2" s="96">
         <v>1</v>
       </c>
@@ -3691,7 +3695,7 @@
       <c r="E2" s="86"/>
       <c r="F2" s="86"/>
     </row>
-    <row r="3" spans="1:8" ht="78" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="87.5">
       <c r="A3" s="97"/>
       <c r="B3" s="3" t="s">
         <v>332</v>
@@ -3703,7 +3707,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="97"/>
       <c r="B4" s="3" t="s">
         <v>336</v>
@@ -3715,7 +3719,7 @@
       <c r="E4" s="42"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="97"/>
       <c r="B5" s="3" t="s">
         <v>333</v>
@@ -3727,7 +3731,7 @@
       <c r="E5" s="42"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="50" customHeight="1" thickBot="1">
       <c r="A6" s="98"/>
       <c r="B6" s="87" t="s">
         <v>334</v>
@@ -3739,7 +3743,7 @@
       <c r="E6" s="88"/>
       <c r="F6" s="88"/>
     </row>
-    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="62">
       <c r="A7" s="96">
         <v>2</v>
       </c>
@@ -3753,7 +3757,7 @@
       <c r="E7" s="86"/>
       <c r="F7" s="86"/>
     </row>
-    <row r="8" spans="1:8" ht="39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="37.5">
       <c r="A8" s="97"/>
       <c r="B8" s="90" t="s">
         <v>332</v>
@@ -3765,7 +3769,7 @@
       <c r="E8" s="90"/>
       <c r="F8" s="90"/>
     </row>
-    <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="25">
       <c r="A9" s="97"/>
       <c r="B9" s="90" t="s">
         <v>336</v>
@@ -3780,7 +3784,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="97"/>
       <c r="B10" s="90" t="s">
         <v>333</v>
@@ -3792,7 +3796,7 @@
       <c r="E10" s="42"/>
       <c r="F10" s="90"/>
     </row>
-    <row r="11" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="50" customHeight="1" thickBot="1">
       <c r="A11" s="98"/>
       <c r="B11" s="91" t="s">
         <v>334</v>
@@ -3804,7 +3808,7 @@
       <c r="E11" s="88"/>
       <c r="F11" s="88"/>
     </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="62">
       <c r="A12" s="96">
         <v>3</v>
       </c>
@@ -3818,7 +3822,7 @@
       <c r="E12" s="86"/>
       <c r="F12" s="86"/>
     </row>
-    <row r="13" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="25">
       <c r="A13" s="97"/>
       <c r="B13" s="93" t="s">
         <v>332</v>
@@ -3830,7 +3834,7 @@
       <c r="E13" s="93"/>
       <c r="F13" s="93"/>
     </row>
-    <row r="14" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="25">
       <c r="A14" s="97"/>
       <c r="B14" s="93" t="s">
         <v>336</v>
@@ -3845,7 +3849,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8">
       <c r="A15" s="97"/>
       <c r="B15" s="93" t="s">
         <v>333</v>
@@ -3857,7 +3861,7 @@
       <c r="E15" s="42"/>
       <c r="F15" s="93"/>
     </row>
-    <row r="16" spans="1:8" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="50" customHeight="1" thickBot="1">
       <c r="A16" s="98"/>
       <c r="B16" s="94" t="s">
         <v>334</v>
@@ -3869,7 +3873,7 @@
       <c r="E16" s="88"/>
       <c r="F16" s="88"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>276</v>
       </c>
@@ -3885,39 +3889,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" topLeftCell="L22" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="26" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="10.81640625" style="1"/>
+    <col min="4" max="4" width="20.36328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="32.6640625" style="1" customWidth="1"/>
-    <col min="15" max="18" width="10.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="41.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="1"/>
-    <col min="22" max="22" width="10.83203125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="58.5" style="74" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="37.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.36328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.36328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="42.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="32.6328125" style="1" customWidth="1"/>
+    <col min="15" max="18" width="10.81640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41.36328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.81640625" style="1"/>
+    <col min="22" max="22" width="10.81640625" style="1" customWidth="1"/>
+    <col min="23" max="24" width="58.453125" style="74" customWidth="1"/>
+    <col min="25" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="26" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -3976,17 +3980,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="32" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="9">
         <v>43711</v>
       </c>
-      <c r="C2" s="107">
+      <c r="C2" s="126">
         <v>1</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="129" t="s">
         <v>261</v>
       </c>
       <c r="E2" s="26">
@@ -4032,7 +4036,7 @@
       <c r="W2" s="75"/>
       <c r="X2" s="75"/>
     </row>
-    <row r="3" spans="1:24" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="32" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4040,8 +4044,8 @@
         <f>B2+7</f>
         <v>43718</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="111"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="130"/>
       <c r="E3" s="26">
         <v>2</v>
       </c>
@@ -4084,7 +4088,7 @@
       <c r="W3" s="75"/>
       <c r="X3" s="75"/>
     </row>
-    <row r="4" spans="1:24" ht="56" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="56" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4092,8 +4096,8 @@
         <f>B3+7</f>
         <v>43725</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="111"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="130"/>
       <c r="E4" s="26">
         <v>2</v>
       </c>
@@ -4137,7 +4141,7 @@
       <c r="W4" s="75"/>
       <c r="X4" s="75"/>
     </row>
-    <row r="5" spans="1:24" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="32" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4145,8 +4149,8 @@
         <f t="shared" ref="B5:B8" si="0">B4+7</f>
         <v>43732</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="111"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="130"/>
       <c r="E5" s="26">
         <v>3</v>
       </c>
@@ -4190,7 +4194,7 @@
       <c r="W5" s="75"/>
       <c r="X5" s="75"/>
     </row>
-    <row r="6" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="26" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4198,8 +4202,8 @@
         <f>B5+7</f>
         <v>43739</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="111"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="130"/>
       <c r="E6" s="26">
         <v>4</v>
       </c>
@@ -4245,7 +4249,7 @@
       <c r="W6" s="75"/>
       <c r="X6" s="75"/>
     </row>
-    <row r="7" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="26" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4253,8 +4257,8 @@
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="111"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="130"/>
       <c r="E7" s="26">
         <v>4</v>
       </c>
@@ -4294,7 +4298,7 @@
       <c r="W7" s="75"/>
       <c r="X7" s="75"/>
     </row>
-    <row r="8" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="26" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4302,8 +4306,8 @@
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="112"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="26">
         <v>5</v>
       </c>
@@ -4349,25 +4353,25 @@
       <c r="W8" s="75"/>
       <c r="X8" s="75"/>
     </row>
-    <row r="9" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="105" t="s">
+    <row r="9" spans="1:24" ht="26" customHeight="1">
+      <c r="A9" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="106"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="106"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
+      <c r="O9" s="102"/>
+      <c r="P9" s="102"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="41"/>
       <c r="S9" s="32"/>
@@ -4375,7 +4379,7 @@
       <c r="W9" s="75"/>
       <c r="X9" s="75"/>
     </row>
-    <row r="10" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="26" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4383,10 +4387,10 @@
         <f>B8+21</f>
         <v>43774</v>
       </c>
-      <c r="C10" s="107">
+      <c r="C10" s="126">
         <v>1</v>
       </c>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="129" t="s">
         <v>261</v>
       </c>
       <c r="E10" s="26">
@@ -4428,7 +4432,7 @@
       <c r="W10" s="75"/>
       <c r="X10" s="75"/>
     </row>
-    <row r="11" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="26" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4436,8 +4440,8 @@
         <f t="shared" ref="B11:B16" si="1">B10+7</f>
         <v>43781</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="111"/>
+      <c r="C11" s="127"/>
+      <c r="D11" s="130"/>
       <c r="E11" s="26">
         <v>6</v>
       </c>
@@ -4479,7 +4483,7 @@
       <c r="W11" s="75"/>
       <c r="X11" s="75"/>
     </row>
-    <row r="12" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="26" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4487,8 +4491,8 @@
         <f t="shared" si="1"/>
         <v>43788</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="111"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="130"/>
       <c r="E12" s="26">
         <v>6</v>
       </c>
@@ -4525,7 +4529,7 @@
       <c r="W12" s="75"/>
       <c r="X12" s="75"/>
     </row>
-    <row r="13" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="26" customHeight="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4533,8 +4537,8 @@
         <f t="shared" si="1"/>
         <v>43795</v>
       </c>
-      <c r="C13" s="108"/>
-      <c r="D13" s="111"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="130"/>
       <c r="E13" s="26">
         <v>7</v>
       </c>
@@ -4578,7 +4582,7 @@
       <c r="W13" s="75"/>
       <c r="X13" s="75"/>
     </row>
-    <row r="14" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="26" customHeight="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4586,8 +4590,8 @@
         <f t="shared" si="1"/>
         <v>43802</v>
       </c>
-      <c r="C14" s="108"/>
-      <c r="D14" s="111"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="130"/>
       <c r="E14" s="26">
         <v>7</v>
       </c>
@@ -4626,7 +4630,7 @@
       <c r="W14" s="75"/>
       <c r="X14" s="75"/>
     </row>
-    <row r="15" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="26" customHeight="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4634,8 +4638,8 @@
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="111"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="130"/>
       <c r="E15" s="26">
         <v>8</v>
       </c>
@@ -4679,7 +4683,7 @@
       <c r="W15" s="75"/>
       <c r="X15" s="75"/>
     </row>
-    <row r="16" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="26" customHeight="1">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4687,8 +4691,8 @@
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="112"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="131"/>
       <c r="E16" s="26">
         <v>8</v>
       </c>
@@ -4728,25 +4732,25 @@
       <c r="W16" s="75"/>
       <c r="X16" s="75"/>
     </row>
-    <row r="17" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="105" t="s">
+    <row r="17" spans="1:24" ht="26" customHeight="1">
+      <c r="A17" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="106"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="106"/>
-      <c r="N17" s="106"/>
-      <c r="O17" s="106"/>
-      <c r="P17" s="106"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="41"/>
       <c r="S17" s="32"/>
@@ -4754,7 +4758,7 @@
       <c r="W17" s="75"/>
       <c r="X17" s="75"/>
     </row>
-    <row r="18" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="26" customHeight="1">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -4762,10 +4766,10 @@
         <f>B16+21</f>
         <v>43837</v>
       </c>
-      <c r="C18" s="99">
+      <c r="C18" s="120">
         <v>2</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="123" t="s">
         <v>184</v>
       </c>
       <c r="E18" s="28">
@@ -4811,7 +4815,7 @@
       <c r="W18" s="75"/>
       <c r="X18" s="75"/>
     </row>
-    <row r="19" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="26" customHeight="1">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -4819,8 +4823,8 @@
         <f>B18+7</f>
         <v>43844</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="103"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="124"/>
       <c r="E19" s="28">
         <v>1</v>
       </c>
@@ -4860,7 +4864,7 @@
       <c r="W19" s="75"/>
       <c r="X19" s="75"/>
     </row>
-    <row r="20" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="26" customHeight="1">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -4868,8 +4872,8 @@
         <f t="shared" ref="B20:B40" si="2">B19+7</f>
         <v>43851</v>
       </c>
-      <c r="C20" s="100"/>
-      <c r="D20" s="103"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="124"/>
       <c r="E20" s="28">
         <v>2</v>
       </c>
@@ -4913,7 +4917,7 @@
       <c r="W20" s="75"/>
       <c r="X20" s="75"/>
     </row>
-    <row r="21" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="26" customHeight="1">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -4921,8 +4925,8 @@
         <f>B20+7</f>
         <v>43858</v>
       </c>
-      <c r="C21" s="101"/>
-      <c r="D21" s="104"/>
+      <c r="C21" s="122"/>
+      <c r="D21" s="125"/>
       <c r="E21" s="28">
         <v>2</v>
       </c>
@@ -4962,7 +4966,7 @@
       <c r="W21" s="75"/>
       <c r="X21" s="75"/>
     </row>
-    <row r="22" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="26" customHeight="1">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -4970,10 +4974,10 @@
         <f>B21+7</f>
         <v>43865</v>
       </c>
-      <c r="C22" s="118">
+      <c r="C22" s="106">
         <v>3</v>
       </c>
-      <c r="D22" s="115" t="s">
+      <c r="D22" s="103" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="35">
@@ -5019,7 +5023,7 @@
       <c r="W22" s="75"/>
       <c r="X22" s="75"/>
     </row>
-    <row r="23" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="26" customHeight="1">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -5027,8 +5031,8 @@
         <f>B22+7</f>
         <v>43872</v>
       </c>
-      <c r="C23" s="119"/>
-      <c r="D23" s="116"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="104"/>
       <c r="E23" s="35">
         <v>2</v>
       </c>
@@ -5069,7 +5073,7 @@
       </c>
       <c r="S23" s="33"/>
     </row>
-    <row r="24" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="26" customHeight="1">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -5077,8 +5081,8 @@
         <f>B23+7</f>
         <v>43879</v>
       </c>
-      <c r="C24" s="120"/>
-      <c r="D24" s="117"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="105"/>
       <c r="E24" s="34">
         <v>2</v>
       </c>
@@ -5115,25 +5119,25 @@
       </c>
       <c r="S24" s="33"/>
     </row>
-    <row r="25" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="105" t="s">
+    <row r="25" spans="1:24" ht="26" customHeight="1">
+      <c r="A25" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="106"/>
-      <c r="C25" s="106"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="106"/>
-      <c r="J25" s="106"/>
-      <c r="K25" s="106"/>
-      <c r="L25" s="106"/>
-      <c r="M25" s="106"/>
-      <c r="N25" s="106"/>
-      <c r="O25" s="106"/>
-      <c r="P25" s="106"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="102"/>
+      <c r="P25" s="102"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="50"/>
       <c r="S25" s="32"/>
@@ -5141,7 +5145,7 @@
       <c r="W25" s="75"/>
       <c r="X25" s="75"/>
     </row>
-    <row r="26" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="26" customHeight="1">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -5149,10 +5153,10 @@
         <f>B24+21</f>
         <v>43900</v>
       </c>
-      <c r="C26" s="118">
+      <c r="C26" s="106">
         <v>3</v>
       </c>
-      <c r="D26" s="115" t="s">
+      <c r="D26" s="103" t="s">
         <v>60</v>
       </c>
       <c r="E26" s="29">
@@ -5196,7 +5200,7 @@
       <c r="W26" s="75"/>
       <c r="X26" s="75"/>
     </row>
-    <row r="27" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="26" customHeight="1">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -5204,8 +5208,8 @@
         <f t="shared" si="2"/>
         <v>43907</v>
       </c>
-      <c r="C27" s="119"/>
-      <c r="D27" s="116"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="104"/>
       <c r="E27" s="35">
         <v>3</v>
       </c>
@@ -5244,7 +5248,7 @@
       <c r="W27" s="75"/>
       <c r="X27" s="75"/>
     </row>
-    <row r="28" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="26" customHeight="1">
       <c r="A28" s="1">
         <v>21</v>
       </c>
@@ -5252,8 +5256,8 @@
         <f t="shared" si="2"/>
         <v>43914</v>
       </c>
-      <c r="C28" s="119"/>
-      <c r="D28" s="116"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="104"/>
       <c r="E28" s="29">
         <v>4</v>
       </c>
@@ -5295,7 +5299,7 @@
       <c r="W28" s="75"/>
       <c r="X28" s="75"/>
     </row>
-    <row r="29" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="26" customHeight="1">
       <c r="A29" s="1">
         <v>22</v>
       </c>
@@ -5303,8 +5307,8 @@
         <f t="shared" si="2"/>
         <v>43921</v>
       </c>
-      <c r="C29" s="120"/>
-      <c r="D29" s="117"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="105"/>
       <c r="E29" s="35">
         <v>4</v>
       </c>
@@ -5344,7 +5348,7 @@
       <c r="W29" s="75"/>
       <c r="X29" s="75"/>
     </row>
-    <row r="30" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="26" customHeight="1">
       <c r="A30" s="1">
         <v>23</v>
       </c>
@@ -5352,10 +5356,10 @@
         <f t="shared" si="2"/>
         <v>43928</v>
       </c>
-      <c r="C30" s="121">
+      <c r="C30" s="109">
         <v>4</v>
       </c>
-      <c r="D30" s="123" t="s">
+      <c r="D30" s="111" t="s">
         <v>43</v>
       </c>
       <c r="E30" s="30">
@@ -5399,7 +5403,7 @@
       <c r="W30" s="75"/>
       <c r="X30" s="75"/>
     </row>
-    <row r="31" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="26" customHeight="1">
       <c r="A31" s="1">
         <v>24</v>
       </c>
@@ -5407,8 +5411,8 @@
         <f t="shared" si="2"/>
         <v>43935</v>
       </c>
-      <c r="C31" s="122"/>
-      <c r="D31" s="124"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="112"/>
       <c r="E31" s="30">
         <v>2</v>
       </c>
@@ -5449,25 +5453,25 @@
       <c r="W31" s="75"/>
       <c r="X31" s="75"/>
     </row>
-    <row r="32" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="113" t="s">
+    <row r="32" spans="1:24" ht="26" customHeight="1">
+      <c r="A32" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="114"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-      <c r="G32" s="114"/>
-      <c r="H32" s="114"/>
-      <c r="I32" s="114"/>
-      <c r="J32" s="114"/>
-      <c r="K32" s="114"/>
-      <c r="L32" s="114"/>
-      <c r="M32" s="114"/>
-      <c r="N32" s="114"/>
-      <c r="O32" s="114"/>
-      <c r="P32" s="114"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="100"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="100"/>
       <c r="Q32" s="47"/>
       <c r="R32" s="51"/>
       <c r="S32" s="32"/>
@@ -5475,7 +5479,7 @@
       <c r="W32" s="75"/>
       <c r="X32" s="75"/>
     </row>
-    <row r="33" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="26" customHeight="1">
       <c r="A33" s="1">
         <v>25</v>
       </c>
@@ -5483,10 +5487,10 @@
         <f>B31+21</f>
         <v>43956</v>
       </c>
-      <c r="C33" s="121">
+      <c r="C33" s="109">
         <v>4</v>
       </c>
-      <c r="D33" s="123" t="s">
+      <c r="D33" s="111" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="30">
@@ -5515,7 +5519,7 @@
         <v>264</v>
       </c>
       <c r="N33" s="73" t="s">
-        <v>264</v>
+        <v>374</v>
       </c>
       <c r="O33" s="6"/>
       <c r="P33" s="44"/>
@@ -5525,7 +5529,7 @@
       </c>
       <c r="S33" s="33"/>
     </row>
-    <row r="34" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" ht="26" customHeight="1">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -5533,8 +5537,8 @@
         <f t="shared" si="2"/>
         <v>43963</v>
       </c>
-      <c r="C34" s="126"/>
-      <c r="D34" s="125"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="113"/>
       <c r="E34" s="30">
         <v>3</v>
       </c>
@@ -5571,7 +5575,7 @@
       </c>
       <c r="S34" s="32"/>
     </row>
-    <row r="35" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" ht="26" customHeight="1">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -5579,8 +5583,8 @@
         <f t="shared" si="2"/>
         <v>43970</v>
       </c>
-      <c r="C35" s="122"/>
-      <c r="D35" s="124"/>
+      <c r="C35" s="110"/>
+      <c r="D35" s="112"/>
       <c r="E35" s="30">
         <v>4</v>
       </c>
@@ -5616,7 +5620,7 @@
       </c>
       <c r="S35" s="46"/>
     </row>
-    <row r="36" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="26" customHeight="1">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -5624,10 +5628,10 @@
         <f t="shared" si="2"/>
         <v>43977</v>
       </c>
-      <c r="C36" s="129">
+      <c r="C36" s="117">
         <v>5</v>
       </c>
-      <c r="D36" s="127" t="s">
+      <c r="D36" s="115" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="31">
@@ -5659,7 +5663,7 @@
       <c r="W36" s="75"/>
       <c r="X36" s="75"/>
     </row>
-    <row r="37" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" ht="26" customHeight="1">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -5667,8 +5671,8 @@
         <f t="shared" si="2"/>
         <v>43984</v>
       </c>
-      <c r="C37" s="130"/>
-      <c r="D37" s="128"/>
+      <c r="C37" s="118"/>
+      <c r="D37" s="116"/>
       <c r="E37" s="31">
         <v>1</v>
       </c>
@@ -5700,7 +5704,7 @@
       <c r="W37" s="75"/>
       <c r="X37" s="75"/>
     </row>
-    <row r="38" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="26" customHeight="1">
       <c r="A38" s="1">
         <v>30</v>
       </c>
@@ -5708,8 +5712,8 @@
         <f t="shared" si="2"/>
         <v>43991</v>
       </c>
-      <c r="C38" s="130"/>
-      <c r="D38" s="128"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="116"/>
       <c r="E38" s="31">
         <v>1</v>
       </c>
@@ -5739,7 +5743,7 @@
       <c r="W38" s="75"/>
       <c r="X38" s="75"/>
     </row>
-    <row r="39" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" ht="26" customHeight="1">
       <c r="A39" s="1">
         <v>31</v>
       </c>
@@ -5747,8 +5751,8 @@
         <f t="shared" si="2"/>
         <v>43998</v>
       </c>
-      <c r="C39" s="130"/>
-      <c r="D39" s="128"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="116"/>
       <c r="E39" s="31">
         <v>1</v>
       </c>
@@ -5778,7 +5782,7 @@
       <c r="W39" s="75"/>
       <c r="X39" s="75"/>
     </row>
-    <row r="40" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="26" customHeight="1">
       <c r="A40" s="1">
         <v>32</v>
       </c>
@@ -5786,8 +5790,8 @@
         <f t="shared" si="2"/>
         <v>44005</v>
       </c>
-      <c r="C40" s="131"/>
-      <c r="D40" s="128"/>
+      <c r="C40" s="119"/>
+      <c r="D40" s="116"/>
       <c r="E40" s="31">
         <v>1</v>
       </c>
@@ -5815,93 +5819,101 @@
       <c r="W40" s="75"/>
       <c r="X40" s="75"/>
     </row>
-    <row r="41" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="113" t="s">
+    <row r="41" spans="1:24" ht="26" customHeight="1">
+      <c r="A41" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="114"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="114"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="114"/>
-      <c r="G41" s="114"/>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="114"/>
-      <c r="M41" s="114"/>
-      <c r="N41" s="114"/>
-      <c r="O41" s="114"/>
-      <c r="P41" s="114"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
+      <c r="H41" s="100"/>
+      <c r="I41" s="100"/>
+      <c r="J41" s="100"/>
+      <c r="K41" s="100"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="100"/>
+      <c r="N41" s="100"/>
+      <c r="O41" s="100"/>
+      <c r="P41" s="100"/>
       <c r="Q41" s="47"/>
       <c r="R41" s="51"/>
       <c r="V41" s="70"/>
       <c r="W41" s="75"/>
       <c r="X41" s="75"/>
     </row>
-    <row r="42" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" ht="26" customHeight="1">
       <c r="V42" s="70"/>
       <c r="W42" s="75"/>
       <c r="X42" s="75"/>
     </row>
-    <row r="43" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="26" customHeight="1">
       <c r="V43" s="70"/>
       <c r="W43" s="75"/>
       <c r="X43" s="75"/>
     </row>
-    <row r="44" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="26" customHeight="1">
       <c r="V44" s="70"/>
       <c r="W44" s="75"/>
       <c r="X44" s="75"/>
     </row>
-    <row r="45" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="26" customHeight="1">
       <c r="V45" s="70"/>
       <c r="W45" s="75"/>
       <c r="X45" s="75"/>
     </row>
-    <row r="46" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="26" customHeight="1">
       <c r="V46" s="70"/>
       <c r="W46" s="75"/>
       <c r="X46" s="75"/>
     </row>
-    <row r="47" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" ht="26" customHeight="1">
       <c r="V47" s="70"/>
       <c r="W47" s="75"/>
       <c r="X47" s="75"/>
     </row>
-    <row r="48" spans="1:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" ht="26" customHeight="1">
       <c r="V48" s="70"/>
       <c r="W48" s="75"/>
       <c r="X48" s="75"/>
     </row>
-    <row r="49" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="22:24" ht="26" customHeight="1">
       <c r="V49" s="70"/>
       <c r="W49" s="75"/>
       <c r="X49" s="75"/>
     </row>
-    <row r="50" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="22:24" ht="26" customHeight="1">
       <c r="V50" s="70"/>
       <c r="W50" s="75"/>
       <c r="X50" s="75"/>
     </row>
-    <row r="51" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="22:24" ht="26" customHeight="1">
       <c r="V51" s="70"/>
       <c r="W51" s="75"/>
       <c r="X51" s="75"/>
     </row>
-    <row r="52" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="22:24" ht="26" customHeight="1">
       <c r="V52" s="70"/>
       <c r="W52" s="75"/>
       <c r="X52" s="75"/>
     </row>
-    <row r="53" spans="22:24" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="22:24" ht="26" customHeight="1">
       <c r="V53" s="70"/>
       <c r="W53" s="75"/>
       <c r="X53" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A9:P9"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D10:D16"/>
+    <mergeCell ref="C10:C16"/>
     <mergeCell ref="A41:P41"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A25:P25"/>
@@ -5915,14 +5927,6 @@
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="D36:D40"/>
     <mergeCell ref="C36:C40"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="A9:P9"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D10:D16"/>
-    <mergeCell ref="C10:C16"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5931,22 +5935,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="70.5" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="70.453125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="21" customHeight="1"/>
+    <row r="2" spans="1:2" ht="31">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -5954,7 +5958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="38" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -5962,7 +5966,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="38" customHeight="1">
       <c r="A4" s="22" t="s">
         <v>54</v>
       </c>
@@ -5970,7 +5974,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="38" customHeight="1">
       <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
@@ -5978,7 +5982,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="38" customHeight="1">
       <c r="A6" s="24" t="s">
         <v>6</v>
       </c>
@@ -5986,7 +5990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="38" customHeight="1">
       <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
@@ -6002,22 +6006,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="70"/>
-    <col min="2" max="2" width="108.5" style="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.5" style="71" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="70"/>
+    <col min="1" max="1" width="10.81640625" style="70"/>
+    <col min="2" max="2" width="108.453125" style="71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.453125" style="71" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="70" t="s">
         <v>241</v>
       </c>
@@ -6028,7 +6032,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="70" t="s">
         <v>323</v>
       </c>
@@ -6039,7 +6043,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="24">
       <c r="A3" s="70" t="s">
         <v>320</v>
       </c>
@@ -6050,7 +6054,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="24">
       <c r="A4" s="70" t="s">
         <v>205</v>
       </c>
@@ -6061,7 +6065,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" s="70" t="s">
         <v>206</v>
       </c>
@@ -6072,7 +6076,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3">
       <c r="A7" s="70" t="s">
         <v>187</v>
       </c>
@@ -6083,7 +6087,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3">
       <c r="A8" s="70" t="s">
         <v>188</v>
       </c>
@@ -6094,7 +6098,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3">
       <c r="A9" s="70" t="s">
         <v>207</v>
       </c>
@@ -6105,7 +6109,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3">
       <c r="A10" s="70" t="s">
         <v>208</v>
       </c>
@@ -6116,17 +6120,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="A11" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3">
       <c r="A12" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3">
       <c r="A13" s="70" t="s">
         <v>189</v>
       </c>
@@ -6137,7 +6141,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3">
       <c r="A14" s="70" t="s">
         <v>190</v>
       </c>
@@ -6148,7 +6152,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3">
       <c r="A15" s="70" t="s">
         <v>191</v>
       </c>
@@ -6159,7 +6163,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3">
       <c r="A16" s="70" t="s">
         <v>199</v>
       </c>
@@ -6170,7 +6174,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3">
       <c r="A17" s="70" t="s">
         <v>201</v>
       </c>
@@ -6181,7 +6185,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3">
       <c r="A18" s="70" t="s">
         <v>192</v>
       </c>
@@ -6192,7 +6196,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3">
       <c r="A19" s="70" t="s">
         <v>193</v>
       </c>
@@ -6203,7 +6207,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3">
       <c r="A20" s="70" t="s">
         <v>194</v>
       </c>
@@ -6214,7 +6218,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3">
       <c r="A21" s="70" t="s">
         <v>195</v>
       </c>
@@ -6225,7 +6229,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="24">
       <c r="A22" s="70" t="s">
         <v>196</v>
       </c>
@@ -6236,7 +6240,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3">
       <c r="A23" s="70" t="s">
         <v>197</v>
       </c>
@@ -6247,7 +6251,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3">
       <c r="A24" s="70" t="s">
         <v>198</v>
       </c>
@@ -6258,17 +6262,17 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3">
       <c r="A25" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3">
       <c r="A26" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3">
       <c r="A27" s="79" t="s">
         <v>200</v>
       </c>
@@ -6279,7 +6283,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3">
       <c r="A28" s="79" t="s">
         <v>202</v>
       </c>
@@ -6290,7 +6294,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3">
       <c r="A29" s="79" t="s">
         <v>203</v>
       </c>
@@ -6301,7 +6305,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3">
       <c r="A30" s="79" t="s">
         <v>204</v>
       </c>
@@ -6312,7 +6316,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3">
       <c r="A31" s="79" t="s">
         <v>237</v>
       </c>
@@ -6323,7 +6327,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3">
       <c r="A32" s="79" t="s">
         <v>238</v>
       </c>
@@ -6334,7 +6338,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3">
       <c r="A33" s="70" t="s">
         <v>209</v>
       </c>
@@ -6345,7 +6349,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3">
       <c r="A34" s="70" t="s">
         <v>210</v>
       </c>
@@ -6356,7 +6360,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3">
       <c r="A35" s="70" t="s">
         <v>211</v>
       </c>
@@ -6367,7 +6371,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3">
       <c r="A36" s="70" t="s">
         <v>212</v>
       </c>
@@ -6378,7 +6382,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3">
       <c r="A37" s="70" t="s">
         <v>213</v>
       </c>
@@ -6389,7 +6393,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="24">
       <c r="A38" s="70" t="s">
         <v>239</v>
       </c>
@@ -6400,7 +6404,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3">
       <c r="A39" s="70" t="s">
         <v>240</v>
       </c>
@@ -6411,17 +6415,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3">
       <c r="A40" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3">
       <c r="A41" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="24">
       <c r="A42" s="70" t="s">
         <v>214</v>
       </c>
@@ -6432,7 +6436,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="36">
       <c r="A43" s="70" t="s">
         <v>215</v>
       </c>
@@ -6443,7 +6447,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="24">
       <c r="A44" s="70" t="s">
         <v>216</v>
       </c>
@@ -6454,7 +6458,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3">
       <c r="A45" s="70" t="s">
         <v>217</v>
       </c>
@@ -6465,7 +6469,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3">
       <c r="A46" s="70" t="s">
         <v>218</v>
       </c>
@@ -6476,7 +6480,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3">
       <c r="A47" s="70" t="s">
         <v>219</v>
       </c>
@@ -6487,7 +6491,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="24">
       <c r="A48" s="70" t="s">
         <v>220</v>
       </c>
@@ -6498,7 +6502,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3">
       <c r="A49" s="70" t="s">
         <v>221</v>
       </c>
@@ -6509,7 +6513,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="24">
       <c r="A50" s="70" t="s">
         <v>222</v>
       </c>
@@ -6520,17 +6524,17 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3">
       <c r="A51" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3">
       <c r="A52" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3">
       <c r="A53" s="70" t="s">
         <v>223</v>
       </c>
@@ -6541,7 +6545,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3">
       <c r="A54" s="70" t="s">
         <v>224</v>
       </c>
@@ -6552,7 +6556,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3">
       <c r="A55" s="70" t="s">
         <v>225</v>
       </c>
@@ -6563,7 +6567,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3">
       <c r="A56" s="70" t="s">
         <v>226</v>
       </c>
@@ -6574,7 +6578,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3">
       <c r="A57" s="70" t="s">
         <v>227</v>
       </c>
@@ -6585,7 +6589,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3">
       <c r="A58" s="70" t="s">
         <v>228</v>
       </c>
@@ -6596,7 +6600,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3">
       <c r="A59" s="70" t="s">
         <v>231</v>
       </c>
@@ -6607,7 +6611,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="24" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="24">
       <c r="A60" s="70" t="s">
         <v>232</v>
       </c>
@@ -6618,7 +6622,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3">
       <c r="A61" s="70" t="s">
         <v>233</v>
       </c>
@@ -6629,12 +6633,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3">
       <c r="A62" s="70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3">
       <c r="A63" s="70" t="s">
         <v>234</v>
       </c>
@@ -6645,7 +6649,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3">
       <c r="A64" s="70" t="s">
         <v>235</v>
       </c>
@@ -6656,7 +6660,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3">
       <c r="A65" s="70" t="s">
         <v>236</v>
       </c>
@@ -6667,7 +6671,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="36" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="36">
       <c r="A66" s="70" t="s">
         <v>277</v>
       </c>
@@ -6678,7 +6682,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3">
       <c r="A67" s="70" t="s">
         <v>316</v>
       </c>
@@ -6689,7 +6693,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3">
       <c r="A68" s="70" t="s">
         <v>276</v>
       </c>
@@ -6702,20 +6706,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="47.33203125" customWidth="1"/>
+    <col min="2" max="4" width="47.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="14.5">
       <c r="A1" s="132" t="s">
         <v>77</v>
       </c>
@@ -6723,7 +6727,7 @@
       <c r="C1" s="133"/>
       <c r="D1" s="134"/>
     </row>
-    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="21">
       <c r="A2" s="54" t="s">
         <v>78</v>
       </c>
@@ -6733,7 +6737,7 @@
       <c r="C2" s="55"/>
       <c r="D2" s="56"/>
     </row>
-    <row r="3" spans="1:4" ht="44" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="54"/>
       <c r="B3" s="55"/>
       <c r="C3" s="55" t="s">
@@ -6741,7 +6745,7 @@
       </c>
       <c r="D3" s="56"/>
     </row>
-    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="31.5">
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="55" t="s">
@@ -6749,7 +6753,7 @@
       </c>
       <c r="D4" s="56"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55" t="s">
@@ -6757,13 +6761,13 @@
       </c>
       <c r="D5" s="56"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6" s="54"/>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="21">
       <c r="A7" s="54" t="s">
         <v>83</v>
       </c>
@@ -6773,7 +6777,7 @@
       <c r="C7" s="55"/>
       <c r="D7" s="56"/>
     </row>
-    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="21">
       <c r="A8" s="54" t="s">
         <v>85</v>
       </c>
@@ -6785,7 +6789,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="42">
       <c r="A9" s="54"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -6795,7 +6799,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="53" thickBot="1">
       <c r="A10" s="57"/>
       <c r="B10" s="58"/>
       <c r="C10" s="58" t="s">
@@ -6805,13 +6809,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="13" thickBot="1">
       <c r="A11" s="60"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
       <c r="D11" s="61"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="14.5">
       <c r="A12" s="132" t="s">
         <v>92</v>
       </c>
@@ -6819,7 +6823,7 @@
       <c r="C12" s="133"/>
       <c r="D12" s="134"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13" s="54" t="s">
         <v>93</v>
       </c>
@@ -6829,7 +6833,7 @@
       <c r="C13" s="55"/>
       <c r="D13" s="56"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14" s="54" t="s">
         <v>95</v>
       </c>
@@ -6839,7 +6843,7 @@
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15" s="54" t="s">
         <v>97</v>
       </c>
@@ -6849,7 +6853,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="56"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16" s="54" t="s">
         <v>99</v>
       </c>
@@ -6859,7 +6863,7 @@
       <c r="C16" s="55"/>
       <c r="D16" s="56"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="21">
       <c r="A17" s="54" t="s">
         <v>101</v>
       </c>
@@ -6869,7 +6873,7 @@
       <c r="C17" s="55"/>
       <c r="D17" s="56"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="21">
       <c r="A18" s="54" t="s">
         <v>103</v>
       </c>
@@ -6879,7 +6883,7 @@
       <c r="C18" s="55"/>
       <c r="D18" s="56"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="54" t="s">
         <v>105</v>
       </c>
@@ -6889,7 +6893,7 @@
       <c r="C19" s="55"/>
       <c r="D19" s="56"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="54" t="s">
         <v>107</v>
       </c>
@@ -6899,7 +6903,7 @@
       <c r="C20" s="55"/>
       <c r="D20" s="56"/>
     </row>
-    <row r="21" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="21">
       <c r="A21" s="54"/>
       <c r="B21" s="55"/>
       <c r="C21" s="55" t="s">
@@ -6907,7 +6911,7 @@
       </c>
       <c r="D21" s="56"/>
     </row>
-    <row r="22" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="21">
       <c r="A22" s="54"/>
       <c r="B22" s="55"/>
       <c r="C22" s="55" t="s">
@@ -6915,7 +6919,7 @@
       </c>
       <c r="D22" s="56"/>
     </row>
-    <row r="23" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="21">
       <c r="A23" s="54"/>
       <c r="B23" s="55"/>
       <c r="C23" s="55" t="s">
@@ -6923,7 +6927,7 @@
       </c>
       <c r="D23" s="56"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="54"/>
       <c r="B24" s="55"/>
       <c r="C24" s="55" t="s">
@@ -6931,7 +6935,7 @@
       </c>
       <c r="D24" s="56"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25" s="54"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55" t="s">
@@ -6939,13 +6943,13 @@
       </c>
       <c r="D25" s="56"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26" s="54"/>
       <c r="B26" s="55"/>
       <c r="C26" s="55"/>
       <c r="D26" s="56"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27" s="54" t="s">
         <v>114</v>
       </c>
@@ -6955,7 +6959,7 @@
       <c r="C27" s="55"/>
       <c r="D27" s="56"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="21">
       <c r="A28" s="54" t="s">
         <v>116</v>
       </c>
@@ -6965,7 +6969,7 @@
       <c r="C28" s="55"/>
       <c r="D28" s="56"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29" s="54" t="s">
         <v>118</v>
       </c>
@@ -6975,7 +6979,7 @@
       <c r="C29" s="55"/>
       <c r="D29" s="56"/>
     </row>
-    <row r="30" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="21">
       <c r="A30" s="54" t="s">
         <v>120</v>
       </c>
@@ -6985,7 +6989,7 @@
       <c r="C30" s="55"/>
       <c r="D30" s="56"/>
     </row>
-    <row r="31" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="21">
       <c r="A31" s="54" t="s">
         <v>122</v>
       </c>
@@ -6995,7 +6999,7 @@
       <c r="C31" s="55"/>
       <c r="D31" s="56"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32" s="54" t="s">
         <v>124</v>
       </c>
@@ -7005,7 +7009,7 @@
       <c r="C32" s="55"/>
       <c r="D32" s="56"/>
     </row>
-    <row r="33" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="21">
       <c r="A33" s="54"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55" t="s">
@@ -7015,7 +7019,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="21">
       <c r="A34" s="54"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55" t="s">
@@ -7025,7 +7029,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="31.5">
       <c r="A35" s="54"/>
       <c r="B35" s="55"/>
       <c r="C35" s="55" t="s">
@@ -7035,7 +7039,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="31.5">
       <c r="A36" s="54"/>
       <c r="B36" s="55"/>
       <c r="C36" s="55" t="s">
@@ -7045,7 +7049,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="31.5">
       <c r="A37" s="54"/>
       <c r="B37" s="55"/>
       <c r="C37" s="55" t="s">
@@ -7055,7 +7059,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="55" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="52.5">
       <c r="A38" s="54"/>
       <c r="B38" s="55"/>
       <c r="C38" s="55" t="s">
@@ -7065,7 +7069,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="32" thickBot="1">
       <c r="A39" s="57"/>
       <c r="B39" s="58"/>
       <c r="C39" s="58" t="s">
@@ -7075,13 +7079,13 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="13" thickBot="1">
       <c r="A40" s="60"/>
       <c r="B40" s="61"/>
       <c r="C40" s="61"/>
       <c r="D40" s="61"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="14.5">
       <c r="A41" s="135" t="s">
         <v>140</v>
       </c>
@@ -7089,7 +7093,7 @@
       <c r="C41" s="136"/>
       <c r="D41" s="137"/>
     </row>
-    <row r="42" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="31.5">
       <c r="A42" s="54" t="s">
         <v>141</v>
       </c>
@@ -7099,7 +7103,7 @@
       <c r="C42" s="62"/>
       <c r="D42" s="63"/>
     </row>
-    <row r="43" spans="1:4" ht="44" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="42">
       <c r="A43" s="54" t="s">
         <v>143</v>
       </c>
@@ -7109,7 +7113,7 @@
       <c r="C43" s="62"/>
       <c r="D43" s="63"/>
     </row>
-    <row r="44" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" ht="31.5">
       <c r="A44" s="54" t="s">
         <v>145</v>
       </c>
@@ -7119,7 +7123,7 @@
       <c r="C44" s="62"/>
       <c r="D44" s="63"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" ht="21">
       <c r="A45" s="54" t="s">
         <v>147</v>
       </c>
@@ -7129,7 +7133,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="63"/>
     </row>
-    <row r="46" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" ht="21">
       <c r="A46" s="54" t="s">
         <v>149</v>
       </c>
@@ -7139,7 +7143,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="63"/>
     </row>
-    <row r="47" spans="1:4" ht="44" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" ht="42">
       <c r="A47" s="54"/>
       <c r="B47" s="62"/>
       <c r="C47" s="62" t="s">
@@ -7149,7 +7153,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" ht="31.5">
       <c r="A48" s="54"/>
       <c r="B48" s="62"/>
       <c r="C48" s="62" t="s">
@@ -7159,7 +7163,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="44" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" ht="52.5">
       <c r="A49" s="54"/>
       <c r="B49" s="62"/>
       <c r="C49" s="62" t="s">
@@ -7169,7 +7173,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="67" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="74" thickBot="1">
       <c r="A50" s="57"/>
       <c r="B50" s="64"/>
       <c r="C50" s="64" t="s">
@@ -7179,13 +7183,13 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" thickBot="1">
       <c r="A51" s="60"/>
       <c r="B51" s="66"/>
       <c r="C51" s="66"/>
       <c r="D51" s="66"/>
     </row>
-    <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" thickBot="1">
       <c r="A52" s="138" t="s">
         <v>159</v>
       </c>
@@ -7193,7 +7197,7 @@
       <c r="C52" s="139"/>
       <c r="D52" s="140"/>
     </row>
-    <row r="53" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" ht="21">
       <c r="A53" s="67" t="s">
         <v>160</v>
       </c>
@@ -7203,7 +7207,7 @@
       <c r="C53" s="68"/>
       <c r="D53" s="68"/>
     </row>
-    <row r="54" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" ht="21">
       <c r="A54" s="69" t="s">
         <v>162</v>
       </c>
@@ -7213,7 +7217,7 @@
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
     </row>
-    <row r="55" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" ht="21">
       <c r="A55" s="69" t="s">
         <v>164</v>
       </c>
@@ -7223,7 +7227,7 @@
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
     </row>
-    <row r="56" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" ht="21">
       <c r="A56" s="69" t="s">
         <v>166</v>
       </c>
@@ -7233,7 +7237,7 @@
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
     </row>
-    <row r="57" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" ht="21">
       <c r="A57" s="69" t="s">
         <v>168</v>
       </c>
@@ -7243,7 +7247,7 @@
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
     </row>
-    <row r="58" spans="1:4" ht="22" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" ht="21">
       <c r="A58" s="69"/>
       <c r="B58" s="55"/>
       <c r="C58" s="55" t="s">
@@ -7253,7 +7257,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="55" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" ht="52.5">
       <c r="A59" s="69"/>
       <c r="B59" s="55"/>
       <c r="C59" s="55" t="s">
@@ -7263,7 +7267,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="21.5" thickBot="1">
       <c r="A60" s="69"/>
       <c r="B60" s="55"/>
       <c r="C60" s="55" t="s">
@@ -7273,13 +7277,13 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" thickBot="1">
       <c r="A61" s="60"/>
       <c r="B61" s="66"/>
       <c r="C61" s="66"/>
       <c r="D61" s="66"/>
     </row>
-    <row r="62" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" thickBot="1">
       <c r="A62" s="138" t="s">
         <v>176</v>
       </c>
@@ -7287,7 +7291,7 @@
       <c r="C62" s="139"/>
       <c r="D62" s="140"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4">
       <c r="A63" s="67" t="s">
         <v>177</v>
       </c>
@@ -7297,7 +7301,7 @@
       <c r="C63" s="68"/>
       <c r="D63" s="68"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4">
       <c r="A64" s="69" t="s">
         <v>179</v>
       </c>
@@ -7307,7 +7311,7 @@
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
     </row>
-    <row r="65" spans="1:4" ht="44" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" ht="42">
       <c r="A65" s="69" t="s">
         <v>181</v>
       </c>

</xml_diff>